<commit_message>
Finalizacion de validacion nif nie  Coleccion de errores
</commit_message>
<xml_diff>
--- a/SIS2-2020/resources/SistemasInformacionII.xlsx
+++ b/SIS2-2020/resources/SistemasInformacionII.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\NetBeansProjects\Nominas2020\resources\original 2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\NetBeansProjects\SIS2-2020\SIS2-2020\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BF134B-116F-43A2-8F85-247C84C55EE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F2D9BD-951A-4122-AB1D-4B2D0341F5BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1902,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E67" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5552,7 +5552,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="F2:L106">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:L106">
     <sortCondition ref="F1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Realizado bien la correcion de nif nie
</commit_message>
<xml_diff>
--- a/SIS2-2020/resources/SistemasInformacionII.xlsx
+++ b/SIS2-2020/resources/SistemasInformacionII.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\NetBeansProjects\SIS2-2020\SIS2-2020\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F2D9BD-951A-4122-AB1D-4B2D0341F5BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251BCDA6-254F-44FC-A6D8-DC7593A75535}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2325" yWindow="285" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="487">
   <si>
     <t>Nombre</t>
   </si>
@@ -1487,6 +1487,9 @@
   </si>
   <si>
     <t>99558741836555551120</t>
+  </si>
+  <si>
+    <t>X9924125M</t>
   </si>
 </sst>
 </file>
@@ -1902,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E67" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,7 +1984,7 @@
         <v>55</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>70</v>
+        <v>486</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>80</v>
@@ -5556,7 +5559,7 @@
     <sortCondition ref="F1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fin de la practica 2 -> Comprobacion de NIF`s
</commit_message>
<xml_diff>
--- a/SIS2-2020/resources/SistemasInformacionII.xlsx
+++ b/SIS2-2020/resources/SistemasInformacionII.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\NetBeansProjects\SIS2-2020\SIS2-2020\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251BCDA6-254F-44FC-A6D8-DC7593A75535}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B948988-DE28-4AE7-978F-4174A1D54DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="285" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="1320" windowWidth="15375" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="487">
   <si>
     <t>Nombre</t>
   </si>
@@ -1496,6 +1496,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1906,21 +1907,21 @@
   <dimension ref="A1:M106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.5703125" style="2" collapsed="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="28.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="7.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="8" max="8" style="2" width="11.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="28.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="4" width="7.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="8.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1984,7 +1985,7 @@
         <v>55</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>486</v>
+        <v>70</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>80</v>
@@ -5570,7 +5571,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
@@ -5578,11 +5579,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="44.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5765,7 +5766,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.5703125" customWidth="1"/>
+    <col min="1" max="2" customWidth="true" width="20.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -6183,8 +6184,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -6266,8 +6267,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fin de exportacion XML -> Generar codigo IBAN e insertarlo
</commit_message>
<xml_diff>
--- a/SIS2-2020/resources/SistemasInformacionII.xlsx
+++ b/SIS2-2020/resources/SistemasInformacionII.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\NetBeansProjects\SIS2-2020\SIS2-2020\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B948988-DE28-4AE7-978F-4174A1D54DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4081F765-3B9C-4F46-B96C-7E2636E64403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="1320" windowWidth="15375" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="488">
   <si>
     <t>Nombre</t>
   </si>
@@ -265,9 +265,6 @@
     <t>20960031442124800000</t>
   </si>
   <si>
-    <t>20960056163231500000</t>
-  </si>
-  <si>
     <t>01826530120201560000</t>
   </si>
   <si>
@@ -1117,24 +1114,6 @@
     <t>Latifa Epfouad Erre</t>
   </si>
   <si>
-    <t>51556584121251000254</t>
-  </si>
-  <si>
-    <t>26551681877651415636</t>
-  </si>
-  <si>
-    <t>62541122001110105611</t>
-  </si>
-  <si>
-    <t>65645150005168448896</t>
-  </si>
-  <si>
-    <t>20012541100023365233</t>
-  </si>
-  <si>
-    <t>23658965214585223202</t>
-  </si>
-  <si>
     <t>MC</t>
   </si>
   <si>
@@ -1198,298 +1177,322 @@
     <t>P2418823C</t>
   </si>
   <si>
-    <t>32145464138452163421</t>
+    <t>65614874165615445616</t>
+  </si>
+  <si>
+    <t>32569523016220165156</t>
+  </si>
+  <si>
+    <t>24561937521546497521</t>
+  </si>
+  <si>
+    <t>36520125638451012515</t>
+  </si>
+  <si>
+    <t>20125003305201112544</t>
+  </si>
+  <si>
+    <t>21651484690980008984</t>
+  </si>
+  <si>
+    <t>Y1337652D</t>
+  </si>
+  <si>
+    <t>21564975243245467995</t>
+  </si>
+  <si>
+    <t>32566221522587754554</t>
+  </si>
+  <si>
+    <t>23215465315456411515</t>
+  </si>
+  <si>
+    <t>00750184310702510000</t>
+  </si>
+  <si>
+    <t>21584976902154655487</t>
+  </si>
+  <si>
+    <t>25894363475485700145</t>
+  </si>
+  <si>
+    <t>96431245118150005156</t>
+  </si>
+  <si>
+    <t>25030000114574745458</t>
+  </si>
+  <si>
+    <t>15953684811254695203</t>
+  </si>
+  <si>
+    <t>20960043023096200000</t>
+  </si>
+  <si>
+    <t>Y0806930N</t>
+  </si>
+  <si>
+    <t>23455254943263234457</t>
+  </si>
+  <si>
+    <t>09741995T</t>
+  </si>
+  <si>
+    <t>20960043032159000000</t>
+  </si>
+  <si>
+    <t>12669681115112121210</t>
+  </si>
+  <si>
+    <t>56187775315550000651</t>
+  </si>
+  <si>
+    <t>25516848021156151054</t>
+  </si>
+  <si>
+    <t>64578946740051516490</t>
+  </si>
+  <si>
+    <t>34698752714600549403</t>
+  </si>
+  <si>
+    <t>66649444162310000255</t>
+  </si>
+  <si>
+    <t>23185484465641685100</t>
+  </si>
+  <si>
+    <t>52198484752100515144</t>
+  </si>
+  <si>
+    <t>36250012804785523365</t>
+  </si>
+  <si>
+    <t>22515651915640081000</t>
+  </si>
+  <si>
+    <t>21508149175421346497</t>
+  </si>
+  <si>
+    <t>24304263W</t>
+  </si>
+  <si>
+    <t>21346154503164978451</t>
+  </si>
+  <si>
+    <t>25187786311225455548</t>
+  </si>
+  <si>
+    <t>23164897642213030615</t>
+  </si>
+  <si>
+    <t>96536214865214585214</t>
+  </si>
+  <si>
+    <t>85461325251978750005</t>
+  </si>
+  <si>
+    <t>24587946032003165464</t>
+  </si>
+  <si>
+    <t>24571671N</t>
+  </si>
+  <si>
+    <t>20960043073071400000</t>
+  </si>
+  <si>
+    <t>20960043042158800000</t>
+  </si>
+  <si>
+    <t>21654587985156484454</t>
+  </si>
+  <si>
+    <t>51651681961210656510</t>
+  </si>
+  <si>
+    <t>66552211148855332200</t>
+  </si>
+  <si>
+    <t>09548827D</t>
+  </si>
+  <si>
+    <t>X8996448K</t>
+  </si>
+  <si>
+    <t>01821135910205540000</t>
+  </si>
+  <si>
+    <t>22631245526916432102</t>
+  </si>
+  <si>
+    <t>09548295Y</t>
+  </si>
+  <si>
+    <t>20960043043075700000</t>
+  </si>
+  <si>
+    <t>25635478321002541225</t>
+  </si>
+  <si>
+    <t>32154697195423121000</t>
+  </si>
+  <si>
+    <t>36521452736500658485</t>
+  </si>
+  <si>
+    <t>20008521528775113366</t>
+  </si>
+  <si>
+    <t>51651487910005118185</t>
+  </si>
+  <si>
+    <t>09611087P</t>
+  </si>
+  <si>
+    <t>21651651812511133551</t>
+  </si>
+  <si>
+    <t>20960043033000100000</t>
+  </si>
+  <si>
+    <t>36585214290025478551</t>
+  </si>
+  <si>
+    <t>12548523465214585214</t>
+  </si>
+  <si>
+    <t>31624561042546920007</t>
+  </si>
+  <si>
+    <t>36154231712500312566</t>
+  </si>
+  <si>
+    <t>44875664127231645789</t>
+  </si>
+  <si>
+    <t>09548486J</t>
+  </si>
+  <si>
+    <t>33620012937852100256</t>
+  </si>
+  <si>
+    <t>33218885441445121022</t>
+  </si>
+  <si>
+    <t>62581542713690044508</t>
+  </si>
+  <si>
+    <t>25165151118666365100</t>
+  </si>
+  <si>
+    <t>36952365020014425254</t>
+  </si>
+  <si>
+    <t>65168874641561561500</t>
+  </si>
+  <si>
+    <t>20960583831234500000</t>
+  </si>
+  <si>
+    <t>21416325811510005514</t>
+  </si>
+  <si>
+    <t>32628484504115151115</t>
+  </si>
+  <si>
+    <t>63516541828944000984</t>
+  </si>
+  <si>
+    <t>32658012367712548745</t>
+  </si>
+  <si>
+    <t>23652365142254222000</t>
+  </si>
+  <si>
+    <t>32584216971684051000</t>
+  </si>
+  <si>
+    <t>55065688761051056105</t>
+  </si>
+  <si>
+    <t>95485212315484010000</t>
+  </si>
+  <si>
+    <t>21856333126985542360</t>
+  </si>
+  <si>
+    <t>36245978133245679001</t>
+  </si>
+  <si>
+    <t>31245164156597845124</t>
+  </si>
+  <si>
+    <t>23221158252545471411</t>
+  </si>
+  <si>
+    <t>32574512085411002255</t>
+  </si>
+  <si>
+    <t>20960043013468900000</t>
+  </si>
+  <si>
+    <t>09548443Q</t>
+  </si>
+  <si>
+    <t>31215643855060225021</t>
+  </si>
+  <si>
+    <t>09749147E</t>
+  </si>
+  <si>
+    <t>85550564726165145610</t>
+  </si>
+  <si>
+    <t>65165654918886005001</t>
+  </si>
+  <si>
+    <t>26221011628048788896</t>
+  </si>
+  <si>
+    <t>12548521518742146695</t>
+  </si>
+  <si>
+    <t>32541112811220000588</t>
+  </si>
+  <si>
+    <t>99558741836555551120</t>
+  </si>
+  <si>
+    <t>51556584221251000254</t>
+  </si>
+  <si>
+    <t>20012541150023365233</t>
+  </si>
+  <si>
+    <t>26551681807651415636</t>
+  </si>
+  <si>
+    <t>23658965274585223202</t>
+  </si>
+  <si>
+    <t>20960056133231500000</t>
+  </si>
+  <si>
+    <t>62541122421110105611</t>
+  </si>
+  <si>
+    <t>65645150865168448896</t>
+  </si>
+  <si>
+    <t>20960043053554600000</t>
+  </si>
+  <si>
+    <t>32145464178452163421</t>
+  </si>
+  <si>
+    <t>31645124483461205164</t>
   </si>
   <si>
     <t>31645124473461205164</t>
-  </si>
-  <si>
-    <t>65614874165615445616</t>
-  </si>
-  <si>
-    <t>32569523016220165156</t>
-  </si>
-  <si>
-    <t>24561937521546497521</t>
-  </si>
-  <si>
-    <t>36520125638451012515</t>
-  </si>
-  <si>
-    <t>20125003305201112544</t>
-  </si>
-  <si>
-    <t>21651484690980008984</t>
-  </si>
-  <si>
-    <t>Y1337652D</t>
-  </si>
-  <si>
-    <t>21564975243245467995</t>
-  </si>
-  <si>
-    <t>32566221522587754554</t>
-  </si>
-  <si>
-    <t>23215465315456411515</t>
-  </si>
-  <si>
-    <t>00750184310702510000</t>
-  </si>
-  <si>
-    <t>21584976902154655487</t>
-  </si>
-  <si>
-    <t>25894363475485700145</t>
-  </si>
-  <si>
-    <t>96431245118150005156</t>
-  </si>
-  <si>
-    <t>25030000114574745458</t>
-  </si>
-  <si>
-    <t>15953684811254695203</t>
-  </si>
-  <si>
-    <t>20960043023096200000</t>
-  </si>
-  <si>
-    <t>Y0806930N</t>
-  </si>
-  <si>
-    <t>23455254943263234457</t>
-  </si>
-  <si>
-    <t>09741995T</t>
-  </si>
-  <si>
-    <t>20960043032159000000</t>
-  </si>
-  <si>
-    <t>12669681115112121210</t>
-  </si>
-  <si>
-    <t>56187775315550000651</t>
-  </si>
-  <si>
-    <t>25516848021156151054</t>
-  </si>
-  <si>
-    <t>64578946740051516490</t>
-  </si>
-  <si>
-    <t>34698752714600549403</t>
-  </si>
-  <si>
-    <t>66649444162310000255</t>
-  </si>
-  <si>
-    <t>23185484465641685100</t>
-  </si>
-  <si>
-    <t>52198484752100515144</t>
-  </si>
-  <si>
-    <t>36250012804785523365</t>
-  </si>
-  <si>
-    <t>22515651915640081000</t>
-  </si>
-  <si>
-    <t>21508149175421346497</t>
-  </si>
-  <si>
-    <t>24304263W</t>
-  </si>
-  <si>
-    <t>21346154503164978451</t>
-  </si>
-  <si>
-    <t>25187786311225455548</t>
-  </si>
-  <si>
-    <t>23164897642213030615</t>
-  </si>
-  <si>
-    <t>96536214865214585214</t>
-  </si>
-  <si>
-    <t>85461325251978750005</t>
-  </si>
-  <si>
-    <t>24587946032003165464</t>
-  </si>
-  <si>
-    <t>24571671N</t>
-  </si>
-  <si>
-    <t>20960043073071400000</t>
-  </si>
-  <si>
-    <t>20960043042158800000</t>
-  </si>
-  <si>
-    <t>21654587985156484454</t>
-  </si>
-  <si>
-    <t>51651681961210656510</t>
-  </si>
-  <si>
-    <t>66552211148855332200</t>
-  </si>
-  <si>
-    <t>09548827D</t>
-  </si>
-  <si>
-    <t>X8996448K</t>
-  </si>
-  <si>
-    <t>01821135910205540000</t>
-  </si>
-  <si>
-    <t>22631245526916432102</t>
-  </si>
-  <si>
-    <t>09548295Y</t>
-  </si>
-  <si>
-    <t>20960043043075700000</t>
-  </si>
-  <si>
-    <t>25635478321002541225</t>
-  </si>
-  <si>
-    <t>32154697195423121000</t>
-  </si>
-  <si>
-    <t>36521452736500658485</t>
-  </si>
-  <si>
-    <t>20008521528775113366</t>
-  </si>
-  <si>
-    <t>51651487910005118185</t>
-  </si>
-  <si>
-    <t>09611087P</t>
-  </si>
-  <si>
-    <t>21651651812511133551</t>
-  </si>
-  <si>
-    <t>20960043033000100000</t>
-  </si>
-  <si>
-    <t>36585214290025478551</t>
-  </si>
-  <si>
-    <t>12548523465214585214</t>
-  </si>
-  <si>
-    <t>31624561042546920007</t>
-  </si>
-  <si>
-    <t>36154231712500312566</t>
-  </si>
-  <si>
-    <t>44875664127231645789</t>
-  </si>
-  <si>
-    <t>09548486J</t>
-  </si>
-  <si>
-    <t>33620012937852100256</t>
-  </si>
-  <si>
-    <t>33218885441445121022</t>
-  </si>
-  <si>
-    <t>62581542713690044508</t>
-  </si>
-  <si>
-    <t>25165151118666365100</t>
-  </si>
-  <si>
-    <t>36952365020014425254</t>
-  </si>
-  <si>
-    <t>65168874641561561500</t>
-  </si>
-  <si>
-    <t>20960583831234500000</t>
-  </si>
-  <si>
-    <t>21416325811510005514</t>
-  </si>
-  <si>
-    <t>32628484504115151115</t>
-  </si>
-  <si>
-    <t>63516541828944000984</t>
-  </si>
-  <si>
-    <t>32658012367712548745</t>
-  </si>
-  <si>
-    <t>23652365142254222000</t>
-  </si>
-  <si>
-    <t>32584216971684051000</t>
-  </si>
-  <si>
-    <t>55065688761051056105</t>
-  </si>
-  <si>
-    <t>95485212315484010000</t>
-  </si>
-  <si>
-    <t>21856333126985542360</t>
-  </si>
-  <si>
-    <t>36245978133245679001</t>
-  </si>
-  <si>
-    <t>31245164156597845124</t>
-  </si>
-  <si>
-    <t>23221158252545471411</t>
-  </si>
-  <si>
-    <t>32574512085411002255</t>
-  </si>
-  <si>
-    <t>20960043013468900000</t>
-  </si>
-  <si>
-    <t>09548443Q</t>
-  </si>
-  <si>
-    <t>31215643855060225021</t>
-  </si>
-  <si>
-    <t>09749147E</t>
-  </si>
-  <si>
-    <t>85550564726165145610</t>
-  </si>
-  <si>
-    <t>65165654918886005001</t>
-  </si>
-  <si>
-    <t>26221011628048788896</t>
-  </si>
-  <si>
-    <t>12548521518742146695</t>
-  </si>
-  <si>
-    <t>32541112811220000588</t>
-  </si>
-  <si>
-    <t>99558741836555551120</t>
-  </si>
-  <si>
-    <t>X9924125M</t>
   </si>
 </sst>
 </file>
@@ -1526,7 +1529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1538,6 +1541,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1907,7 +1913,7 @@
   <dimension ref="A1:M106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1956,7 +1962,7 @@
         <v>75</v>
       </c>
       <c r="K1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>13</v>
@@ -1967,10 +1973,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -1988,10 +1994,10 @@
         <v>70</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L2"/>
       <c r="M2" t="s">
@@ -2000,10 +2006,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -2024,10 +2030,10 @@
         <v>70</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>389</v>
+        <v>485</v>
       </c>
       <c r="K3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L3"/>
       <c r="M3" t="s">
@@ -2036,10 +2042,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
@@ -2048,22 +2054,22 @@
         <v>39448</v>
       </c>
       <c r="E4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" t="s">
         <v>131</v>
-      </c>
-      <c r="F4" t="s">
-        <v>132</v>
       </c>
       <c r="G4" t="s">
         <v>31</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>390</v>
+        <v>487</v>
       </c>
       <c r="K4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L4"/>
       <c r="M4" t="s">
@@ -2072,10 +2078,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B5" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C5" t="s">
         <v>50</v>
@@ -2084,22 +2090,22 @@
         <v>40513</v>
       </c>
       <c r="E5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" t="s">
         <v>187</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>188</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>391</v>
+      <c r="J5" s="7" t="s">
+        <v>382</v>
       </c>
       <c r="K5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L5"/>
       <c r="M5" t="s">
@@ -2111,7 +2117,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -2120,22 +2126,22 @@
         <v>40664</v>
       </c>
       <c r="E6" t="s">
+        <v>236</v>
+      </c>
+      <c r="F6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G6" t="s">
         <v>237</v>
       </c>
-      <c r="F6" t="s">
-        <v>188</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="J6" s="5" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="K6" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="L6"/>
       <c r="M6" t="s">
@@ -2144,10 +2150,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -2159,19 +2165,19 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G7" t="s">
         <v>33</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="K7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L7"/>
       <c r="M7" t="s">
@@ -2183,7 +2189,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -2192,22 +2198,22 @@
         <v>38200</v>
       </c>
       <c r="E8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F8" t="s">
         <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="K8" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="L8"/>
       <c r="M8" t="s">
@@ -2220,10 +2226,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B10" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C10" t="s">
         <v>45</v>
@@ -2232,22 +2238,22 @@
         <v>40391</v>
       </c>
       <c r="E10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" t="s">
         <v>165</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>166</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="J10" s="5" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="K10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L10"/>
       <c r="M10" t="s">
@@ -2256,10 +2262,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B11" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -2268,22 +2274,22 @@
         <v>37226</v>
       </c>
       <c r="E11" t="s">
+        <v>278</v>
+      </c>
+      <c r="F11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G11" t="s">
+        <v>241</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G11" t="s">
-        <v>242</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="J11" s="5" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="K11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L11"/>
       <c r="M11" t="s">
@@ -2292,10 +2298,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -2313,13 +2319,13 @@
         <v>58</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L12"/>
       <c r="M12" t="s">
@@ -2328,10 +2334,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -2349,13 +2355,13 @@
         <v>58</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="K13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L13"/>
       <c r="M13" t="s">
@@ -2364,10 +2370,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B14" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C14" t="s">
         <v>49</v>
@@ -2376,22 +2382,22 @@
         <v>38139</v>
       </c>
       <c r="E14" t="s">
+        <v>284</v>
+      </c>
+      <c r="F14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" t="s">
         <v>285</v>
       </c>
-      <c r="F14" t="s">
-        <v>119</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="H14" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="J14" s="5" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="K14" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="L14"/>
       <c r="M14" t="s">
@@ -2400,10 +2406,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B15" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -2412,22 +2418,22 @@
         <v>40087</v>
       </c>
       <c r="E15" t="s">
+        <v>265</v>
+      </c>
+      <c r="F15" t="s">
         <v>266</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
+        <v>138</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="G15" t="s">
-        <v>139</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="J15" s="5" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="K15" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="L15"/>
       <c r="M15" t="s">
@@ -2436,10 +2442,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
@@ -2454,13 +2460,13 @@
         <v>60</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="K16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L16"/>
       <c r="M16" t="s">
@@ -2469,10 +2475,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
@@ -2490,13 +2496,13 @@
         <v>60</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="K17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L17"/>
       <c r="M17" t="s">
@@ -2505,10 +2511,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B18" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -2517,22 +2523,22 @@
         <v>39022</v>
       </c>
       <c r="E18" t="s">
+        <v>328</v>
+      </c>
+      <c r="F18" t="s">
         <v>329</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="G18" t="s">
-        <v>129</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>331</v>
-      </c>
       <c r="J18" s="5" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="K18" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="L18"/>
       <c r="M18" t="s">
@@ -2541,10 +2547,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B19" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C19" t="s">
         <v>47</v>
@@ -2553,22 +2559,22 @@
         <v>40118</v>
       </c>
       <c r="E19" t="s">
+        <v>314</v>
+      </c>
+      <c r="F19" t="s">
         <v>315</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>316</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="J19" s="5" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="K19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L19"/>
       <c r="M19" t="s">
@@ -2577,10 +2583,10 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B20" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C20" t="s">
         <v>48</v>
@@ -2589,22 +2595,22 @@
         <v>36831</v>
       </c>
       <c r="E20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G20" t="s">
         <v>39</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="K20" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="L20"/>
       <c r="M20" t="s">
@@ -2613,10 +2619,10 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B21" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
@@ -2625,22 +2631,22 @@
         <v>41548</v>
       </c>
       <c r="E21" t="s">
+        <v>311</v>
+      </c>
+      <c r="F21" t="s">
         <v>312</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
+        <v>312</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="G21" t="s">
-        <v>313</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>314</v>
-      </c>
       <c r="J21" s="5" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="K21" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="L21"/>
       <c r="M21" t="s">
@@ -2649,10 +2655,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -2661,10 +2667,10 @@
         <v>40909</v>
       </c>
       <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
         <v>92</v>
-      </c>
-      <c r="F22" t="s">
-        <v>93</v>
       </c>
       <c r="G22" t="s">
         <v>33</v>
@@ -2673,10 +2679,10 @@
         <v>43</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="K22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L22"/>
       <c r="M22" t="s">
@@ -2685,10 +2691,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B23" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -2697,19 +2703,19 @@
         <v>41913</v>
       </c>
       <c r="E23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F23" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="K23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L23"/>
       <c r="M23" t="s">
@@ -2721,7 +2727,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -2730,7 +2736,7 @@
         <v>41944</v>
       </c>
       <c r="E24" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F24" t="s">
         <v>61</v>
@@ -2739,13 +2745,13 @@
         <v>61</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="K24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L24"/>
       <c r="M24" t="s">
@@ -2754,10 +2760,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -2775,10 +2781,10 @@
         <v>64</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L25"/>
       <c r="M25" t="s">
@@ -2790,7 +2796,7 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -2808,13 +2814,13 @@
         <v>33</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="K26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L26"/>
       <c r="M26" t="s">
@@ -2823,10 +2829,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B27" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C27" t="s">
         <v>48</v>
@@ -2835,22 +2841,22 @@
         <v>40452</v>
       </c>
       <c r="E27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F27" t="s">
         <v>41</v>
       </c>
       <c r="G27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="K27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L27"/>
       <c r="M27" t="s">
@@ -2863,10 +2869,10 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -2875,22 +2881,22 @@
         <v>35735</v>
       </c>
       <c r="E29" t="s">
+        <v>298</v>
+      </c>
+      <c r="F29" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29" t="s">
         <v>299</v>
       </c>
-      <c r="F29" t="s">
-        <v>196</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="H29" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>301</v>
-      </c>
       <c r="J29" s="5" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="K29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L29"/>
       <c r="M29" t="s">
@@ -2899,10 +2905,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B30" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -2911,22 +2917,22 @@
         <v>40603</v>
       </c>
       <c r="E30" t="s">
+        <v>182</v>
+      </c>
+      <c r="F30" t="s">
         <v>183</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>184</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="J30" s="5" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="K30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L30"/>
       <c r="M30" t="s">
@@ -2935,10 +2941,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B31" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
@@ -2947,22 +2953,22 @@
         <v>36465</v>
       </c>
       <c r="E31" t="s">
+        <v>318</v>
+      </c>
+      <c r="F31" t="s">
         <v>319</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>320</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>322</v>
-      </c>
       <c r="J31" s="5" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="K31" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="L31"/>
       <c r="M31" t="s">
@@ -2971,10 +2977,10 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -2983,22 +2989,22 @@
         <v>36039</v>
       </c>
       <c r="E32" t="s">
+        <v>322</v>
+      </c>
+      <c r="F32" t="s">
         <v>323</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>324</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="J32" s="5" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="K32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L32"/>
       <c r="M32" t="s">
@@ -3007,10 +3013,10 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B33" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -3019,22 +3025,22 @@
         <v>38777</v>
       </c>
       <c r="E33" t="s">
+        <v>331</v>
+      </c>
+      <c r="F33" t="s">
         <v>332</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>333</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>335</v>
-      </c>
       <c r="J33" s="5" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="K33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L33"/>
       <c r="M33" t="s">
@@ -3046,7 +3052,7 @@
         <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
         <v>48</v>
@@ -3055,22 +3061,22 @@
         <v>38169</v>
       </c>
       <c r="E34" t="s">
+        <v>268</v>
+      </c>
+      <c r="F34" t="s">
         <v>269</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
+        <v>241</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="G34" t="s">
-        <v>242</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="J34" s="5" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="K34" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="L34"/>
       <c r="M34" t="s">
@@ -3082,7 +3088,7 @@
         <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
         <v>50</v>
@@ -3091,22 +3097,22 @@
         <v>40118</v>
       </c>
       <c r="E35" t="s">
+        <v>214</v>
+      </c>
+      <c r="F35" t="s">
         <v>215</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>216</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="J35" s="5" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="K35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L35"/>
       <c r="M35" t="s">
@@ -3115,10 +3121,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B36" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
@@ -3127,22 +3133,22 @@
         <v>40664</v>
       </c>
       <c r="E36" t="s">
+        <v>233</v>
+      </c>
+      <c r="F36" t="s">
         <v>234</v>
-      </c>
-      <c r="F36" t="s">
-        <v>235</v>
       </c>
       <c r="G36" t="s">
         <v>33</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="K36" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="L36"/>
       <c r="M36" t="s">
@@ -3151,10 +3157,10 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B37" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
@@ -3163,22 +3169,22 @@
         <v>37865</v>
       </c>
       <c r="E37" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F37" t="s">
         <v>39</v>
       </c>
       <c r="G37" t="s">
+        <v>209</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="J37" s="5" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="K37" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="L37"/>
       <c r="M37" t="s">
@@ -3187,10 +3193,10 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B38" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C38" t="s">
         <v>49</v>
@@ -3199,22 +3205,22 @@
         <v>36192</v>
       </c>
       <c r="E38" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F38" t="s">
         <v>39</v>
       </c>
       <c r="G38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="K38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L38"/>
       <c r="M38" t="s">
@@ -3226,7 +3232,7 @@
         <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
         <v>45</v>
@@ -3235,22 +3241,22 @@
         <v>40817</v>
       </c>
       <c r="E39" t="s">
+        <v>351</v>
+      </c>
+      <c r="F39" t="s">
         <v>352</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>353</v>
       </c>
-      <c r="G39" t="s">
-        <v>354</v>
-      </c>
       <c r="H39" s="2" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="K39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L39"/>
       <c r="M39" t="s">
@@ -3259,10 +3265,10 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B40" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C40" t="s">
         <v>71</v>
@@ -3271,22 +3277,22 @@
         <v>42979</v>
       </c>
       <c r="E40" t="s">
+        <v>335</v>
+      </c>
+      <c r="F40" t="s">
         <v>336</v>
-      </c>
-      <c r="F40" t="s">
-        <v>337</v>
       </c>
       <c r="G40" t="s">
         <v>39</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="K40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L40"/>
       <c r="M40" t="s">
@@ -3295,10 +3301,10 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
@@ -3307,22 +3313,22 @@
         <v>40057</v>
       </c>
       <c r="E41" t="s">
+        <v>338</v>
+      </c>
+      <c r="F41" t="s">
         <v>339</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>340</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>342</v>
-      </c>
       <c r="J41" s="5" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="K41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L41"/>
       <c r="M41" t="s">
@@ -3331,10 +3337,10 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
@@ -3343,22 +3349,22 @@
         <v>37865</v>
       </c>
       <c r="E42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" t="s">
         <v>123</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>124</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="J42" s="5" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="K42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L42"/>
       <c r="M42" t="s">
@@ -3367,10 +3373,10 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B43" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
@@ -3379,22 +3385,22 @@
         <v>39600</v>
       </c>
       <c r="E43" t="s">
+        <v>342</v>
+      </c>
+      <c r="F43" t="s">
         <v>343</v>
-      </c>
-      <c r="F43" t="s">
-        <v>344</v>
       </c>
       <c r="G43" t="s">
         <v>31</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="K43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L43"/>
       <c r="M43" t="s">
@@ -3403,10 +3409,10 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C44" t="s">
         <v>48</v>
@@ -3415,22 +3421,22 @@
         <v>42370</v>
       </c>
       <c r="E44" t="s">
+        <v>345</v>
+      </c>
+      <c r="F44" t="s">
         <v>346</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>347</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="H44" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="J44" s="5" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="K44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L44"/>
       <c r="M44" t="s">
@@ -3439,10 +3445,10 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" t="s">
         <v>51</v>
@@ -3460,13 +3466,13 @@
         <v>39</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L45"/>
       <c r="M45" t="s">
@@ -3475,10 +3481,10 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" t="s">
         <v>46</v>
@@ -3499,10 +3505,10 @@
         <v>42</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="K46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L46"/>
       <c r="M46" t="s">
@@ -3511,10 +3517,10 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B47" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
@@ -3523,22 +3529,22 @@
         <v>42767</v>
       </c>
       <c r="E47" t="s">
+        <v>178</v>
+      </c>
+      <c r="F47" t="s">
         <v>179</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>180</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="J47" s="5" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="K47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L47"/>
       <c r="M47" t="s">
@@ -3547,10 +3553,10 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B48" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
@@ -3559,22 +3565,22 @@
         <v>39692</v>
       </c>
       <c r="E48" t="s">
+        <v>137</v>
+      </c>
+      <c r="F48" t="s">
         <v>138</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>139</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="J48" s="5" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="K48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L48"/>
       <c r="M48" t="s">
@@ -3586,7 +3592,7 @@
         <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
         <v>51</v>
@@ -3595,22 +3601,22 @@
         <v>41030</v>
       </c>
       <c r="E49" t="s">
+        <v>243</v>
+      </c>
+      <c r="F49" t="s">
         <v>244</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>245</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="J49" s="5" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="K49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L49"/>
       <c r="M49" t="s">
@@ -3619,10 +3625,10 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C50" t="s">
         <v>10</v>
@@ -3637,13 +3643,13 @@
         <v>66</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L50"/>
       <c r="M50" t="s">
@@ -3652,10 +3658,10 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B51" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C51" t="s">
         <v>46</v>
@@ -3670,13 +3676,13 @@
         <v>68</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="K51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L51"/>
       <c r="M51" t="s">
@@ -3685,10 +3691,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C52" t="s">
         <v>45</v>
@@ -3697,22 +3703,22 @@
         <v>42887</v>
       </c>
       <c r="E52" t="s">
+        <v>133</v>
+      </c>
+      <c r="F52" t="s">
         <v>134</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>135</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="J52" s="5" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="K52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L52"/>
       <c r="M52" t="s">
@@ -3721,10 +3727,10 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" t="s">
         <v>10</v>
@@ -3742,13 +3748,13 @@
         <v>22</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="K53" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L53"/>
       <c r="M53" t="s">
@@ -3760,7 +3766,7 @@
         <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s">
         <v>10</v>
@@ -3769,22 +3775,22 @@
         <v>39995</v>
       </c>
       <c r="E54" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F54" t="s">
         <v>29</v>
       </c>
       <c r="G54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="K54" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="L54"/>
       <c r="M54" t="s">
@@ -3793,10 +3799,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B55" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C55" t="s">
         <v>11</v>
@@ -3805,22 +3811,22 @@
         <v>40299</v>
       </c>
       <c r="E55" t="s">
+        <v>190</v>
+      </c>
+      <c r="F55" t="s">
         <v>191</v>
-      </c>
-      <c r="F55" t="s">
-        <v>192</v>
       </c>
       <c r="G55" t="s">
         <v>29</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="K55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L55"/>
       <c r="M55" t="s">
@@ -3829,10 +3835,10 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B56" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C56" t="s">
         <v>51</v>
@@ -3841,22 +3847,22 @@
         <v>43040</v>
       </c>
       <c r="E56" t="s">
+        <v>205</v>
+      </c>
+      <c r="F56" t="s">
+        <v>191</v>
+      </c>
+      <c r="G56" t="s">
         <v>206</v>
       </c>
-      <c r="F56" t="s">
-        <v>192</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="H56" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>208</v>
-      </c>
       <c r="J56" s="5" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="K56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L56"/>
       <c r="M56" t="s">
@@ -3865,10 +3871,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B57" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C57" t="s">
         <v>51</v>
@@ -3877,22 +3883,22 @@
         <v>40969</v>
       </c>
       <c r="E57" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F57" t="s">
         <v>27</v>
       </c>
       <c r="G57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="K57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L57"/>
       <c r="M57" t="s">
@@ -3904,7 +3910,7 @@
         <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C58" t="s">
         <v>51</v>
@@ -3913,22 +3919,22 @@
         <v>38869</v>
       </c>
       <c r="E58" t="s">
+        <v>274</v>
+      </c>
+      <c r="F58" t="s">
         <v>275</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>276</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>278</v>
-      </c>
       <c r="J58" s="5" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="K58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L58"/>
       <c r="M58" t="s">
@@ -3941,10 +3947,10 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C60" t="s">
         <v>48</v>
@@ -3962,13 +3968,13 @@
         <v>32</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L60"/>
       <c r="M60" t="s">
@@ -3977,10 +3983,10 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B61" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C61" t="s">
         <v>46</v>
@@ -3989,7 +3995,7 @@
         <v>40026</v>
       </c>
       <c r="E61" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F61" t="s">
         <v>33</v>
@@ -3998,13 +4004,13 @@
         <v>33</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="K61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L61"/>
       <c r="M61" t="s">
@@ -4013,10 +4019,10 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C62" t="s">
         <v>8</v>
@@ -4025,22 +4031,22 @@
         <v>42309</v>
       </c>
       <c r="E62" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F62" t="s">
         <v>33</v>
       </c>
       <c r="G62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>69</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="K62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L62"/>
       <c r="M62" t="s">
@@ -4049,10 +4055,10 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B63" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C63" t="s">
         <v>8</v>
@@ -4061,22 +4067,22 @@
         <v>38504</v>
       </c>
       <c r="E63" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F63" t="s">
         <v>33</v>
       </c>
       <c r="G63" t="s">
+        <v>203</v>
+      </c>
+      <c r="H63" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="J63" s="5" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="K63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L63"/>
       <c r="M63" t="s">
@@ -4085,10 +4091,10 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B64" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C64" t="s">
         <v>48</v>
@@ -4097,22 +4103,22 @@
         <v>40544</v>
       </c>
       <c r="E64" t="s">
+        <v>118</v>
+      </c>
+      <c r="F64" t="s">
         <v>119</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>120</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="J64" s="5" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="K64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L64"/>
       <c r="M64" t="s">
@@ -4124,7 +4130,7 @@
         <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
@@ -4133,22 +4139,22 @@
         <v>41487</v>
       </c>
       <c r="E65" t="s">
+        <v>218</v>
+      </c>
+      <c r="F65" t="s">
         <v>219</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>220</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="H65" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="J65" s="5" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="K65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L65"/>
       <c r="M65" t="s">
@@ -4157,10 +4163,10 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B66" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C66" t="s">
         <v>46</v>
@@ -4169,22 +4175,22 @@
         <v>43282</v>
       </c>
       <c r="E66" t="s">
+        <v>149</v>
+      </c>
+      <c r="F66" t="s">
         <v>150</v>
-      </c>
-      <c r="F66" t="s">
-        <v>151</v>
       </c>
       <c r="G66" t="s">
         <v>31</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="K66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L66"/>
       <c r="M66" t="s">
@@ -4193,10 +4199,10 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C67" t="s">
         <v>11</v>
@@ -4205,22 +4211,22 @@
         <v>36465</v>
       </c>
       <c r="E67" t="s">
+        <v>356</v>
+      </c>
+      <c r="F67" t="s">
+        <v>150</v>
+      </c>
+      <c r="G67" t="s">
         <v>357</v>
       </c>
-      <c r="F67" t="s">
-        <v>151</v>
-      </c>
-      <c r="G67" t="s">
+      <c r="H67" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>359</v>
-      </c>
       <c r="J67" s="5" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="K67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L67"/>
       <c r="M67" t="s">
@@ -4229,10 +4235,10 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B68" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C68" t="s">
         <v>45</v>
@@ -4241,22 +4247,22 @@
         <v>40057</v>
       </c>
       <c r="E68" t="s">
+        <v>93</v>
+      </c>
+      <c r="F68" t="s">
         <v>94</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>95</v>
       </c>
-      <c r="G68" t="s">
-        <v>96</v>
-      </c>
       <c r="H68" s="3" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>77</v>
       </c>
       <c r="K68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L68"/>
       <c r="M68" t="s">
@@ -4265,10 +4271,10 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B69" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
@@ -4277,22 +4283,22 @@
         <v>42795</v>
       </c>
       <c r="E69" t="s">
+        <v>305</v>
+      </c>
+      <c r="F69" t="s">
+        <v>196</v>
+      </c>
+      <c r="G69" t="s">
         <v>306</v>
       </c>
-      <c r="F69" t="s">
-        <v>197</v>
-      </c>
-      <c r="G69" t="s">
-        <v>307</v>
-      </c>
       <c r="H69" s="2" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="K69" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L69"/>
       <c r="M69" t="s">
@@ -4301,10 +4307,10 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B70" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C70" t="s">
         <v>48</v>
@@ -4313,22 +4319,22 @@
         <v>41426</v>
       </c>
       <c r="E70" t="s">
+        <v>251</v>
+      </c>
+      <c r="F70" t="s">
+        <v>148</v>
+      </c>
+      <c r="G70" t="s">
+        <v>139</v>
+      </c>
+      <c r="H70" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F70" t="s">
-        <v>149</v>
-      </c>
-      <c r="G70" t="s">
-        <v>140</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="J70" s="5" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="K70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L70"/>
       <c r="M70" t="s">
@@ -4337,10 +4343,10 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B71" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C71" t="s">
         <v>9</v>
@@ -4349,22 +4355,22 @@
         <v>40513</v>
       </c>
       <c r="E71" t="s">
+        <v>160</v>
+      </c>
+      <c r="F71" t="s">
         <v>161</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>162</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="H71" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="J71" s="5" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="K71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L71"/>
       <c r="M71" t="s">
@@ -4373,10 +4379,10 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B72" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C72" t="s">
         <v>10</v>
@@ -4385,22 +4391,22 @@
         <v>40057</v>
       </c>
       <c r="E72" t="s">
+        <v>280</v>
+      </c>
+      <c r="F72" t="s">
         <v>281</v>
       </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>282</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="H72" s="2" t="s">
-        <v>284</v>
-      </c>
       <c r="J72" s="5" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="K72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L72"/>
       <c r="M72" t="s">
@@ -4409,10 +4415,10 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B73" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C73" t="s">
         <v>52</v>
@@ -4430,13 +4436,13 @@
         <v>35</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="K73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L73"/>
       <c r="M73" t="s">
@@ -4445,10 +4451,10 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C74" t="s">
         <v>10</v>
@@ -4457,22 +4463,22 @@
         <v>37591</v>
       </c>
       <c r="E74" t="s">
+        <v>301</v>
+      </c>
+      <c r="F74" t="s">
         <v>302</v>
       </c>
-      <c r="F74" t="s">
+      <c r="G74" t="s">
         <v>303</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="H74" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="J74" s="5" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="K74" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="L74"/>
       <c r="M74" t="s">
@@ -4481,10 +4487,10 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B75" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C75" t="s">
         <v>11</v>
@@ -4493,22 +4499,22 @@
         <v>36770</v>
       </c>
       <c r="E75" t="s">
+        <v>295</v>
+      </c>
+      <c r="F75" t="s">
         <v>296</v>
       </c>
-      <c r="F75" t="s">
+      <c r="G75" t="s">
+        <v>128</v>
+      </c>
+      <c r="H75" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="G75" t="s">
-        <v>129</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="J75" s="5" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="K75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L75"/>
       <c r="M75" t="s">
@@ -4517,10 +4523,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B76" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C76" t="s">
         <v>8</v>
@@ -4541,10 +4547,10 @@
         <v>69</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="K76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L76"/>
       <c r="M76" t="s">
@@ -4553,10 +4559,10 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B77" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
@@ -4565,22 +4571,22 @@
         <v>40299</v>
       </c>
       <c r="E77" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F77" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G77" t="s">
         <v>33</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="K77" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L77"/>
       <c r="M77" t="s">
@@ -4592,7 +4598,7 @@
         <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C78" t="s">
         <v>45</v>
@@ -4601,22 +4607,22 @@
         <v>40664</v>
       </c>
       <c r="E78" t="s">
+        <v>229</v>
+      </c>
+      <c r="F78" t="s">
         <v>230</v>
       </c>
-      <c r="F78" t="s">
+      <c r="G78" t="s">
         <v>231</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="H78" s="2" t="s">
-        <v>233</v>
-      </c>
       <c r="J78" s="5" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="K78" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="L78"/>
       <c r="M78" t="s">
@@ -4629,10 +4635,10 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B80" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C80" t="s">
         <v>12</v>
@@ -4641,7 +4647,7 @@
         <v>42705</v>
       </c>
       <c r="E80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F80" t="s">
         <v>36</v>
@@ -4651,10 +4657,10 @@
       </c>
       <c r="H80" s="3"/>
       <c r="J80" s="5" t="s">
-        <v>78</v>
+        <v>481</v>
       </c>
       <c r="K80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M80" t="s">
         <v>20</v>
@@ -4662,10 +4668,10 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B81" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C81" t="s">
         <v>52</v>
@@ -4674,22 +4680,22 @@
         <v>42186</v>
       </c>
       <c r="E81" t="s">
+        <v>170</v>
+      </c>
+      <c r="F81" t="s">
         <v>171</v>
       </c>
-      <c r="F81" t="s">
+      <c r="G81" t="s">
         <v>172</v>
       </c>
-      <c r="G81" t="s">
+      <c r="H81" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="H81" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="J81" s="5" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="K81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L81"/>
       <c r="M81" t="s">
@@ -4698,10 +4704,10 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82" t="s">
         <v>46</v>
@@ -4710,22 +4716,22 @@
         <v>43647</v>
       </c>
       <c r="E82" t="s">
+        <v>307</v>
+      </c>
+      <c r="F82" t="s">
         <v>308</v>
       </c>
-      <c r="F82" t="s">
+      <c r="G82" t="s">
         <v>309</v>
       </c>
-      <c r="G82" t="s">
+      <c r="H82" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="H82" s="2" t="s">
-        <v>311</v>
-      </c>
       <c r="J82" s="5" t="s">
-        <v>367</v>
+        <v>480</v>
       </c>
       <c r="K82" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M82" t="s">
         <v>53</v>
@@ -4733,10 +4739,10 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B83" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C83" t="s">
         <v>50</v>
@@ -4745,22 +4751,22 @@
         <v>38139</v>
       </c>
       <c r="E83" t="s">
+        <v>126</v>
+      </c>
+      <c r="F83" t="s">
         <v>127</v>
       </c>
-      <c r="F83" t="s">
+      <c r="G83" t="s">
         <v>128</v>
       </c>
-      <c r="G83" t="s">
+      <c r="H83" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H83" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="J83" s="5" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="K83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L83"/>
       <c r="M83" t="s">
@@ -4769,10 +4775,10 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B84" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C84" t="s">
         <v>48</v>
@@ -4781,22 +4787,22 @@
         <v>37165</v>
       </c>
       <c r="E84" t="s">
+        <v>292</v>
+      </c>
+      <c r="F84" t="s">
         <v>293</v>
       </c>
-      <c r="F84" t="s">
+      <c r="G84" t="s">
+        <v>272</v>
+      </c>
+      <c r="H84" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="G84" t="s">
-        <v>273</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="J84" s="5" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K84" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L84"/>
       <c r="M84" t="s">
@@ -4805,10 +4811,10 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B85" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C85" t="s">
         <v>9</v>
@@ -4817,19 +4823,19 @@
         <v>37500</v>
       </c>
       <c r="E85" t="s">
+        <v>289</v>
+      </c>
+      <c r="F85" t="s">
         <v>290</v>
       </c>
-      <c r="F85" t="s">
+      <c r="G85" t="s">
         <v>291</v>
       </c>
-      <c r="G85" t="s">
-        <v>292</v>
-      </c>
       <c r="J85" s="5" t="s">
-        <v>366</v>
+        <v>478</v>
       </c>
       <c r="K85" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="M85" t="s">
         <v>20</v>
@@ -4837,10 +4843,10 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B86" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C86" t="s">
         <v>8</v>
@@ -4849,22 +4855,22 @@
         <v>42370</v>
       </c>
       <c r="E86" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F86" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G86" t="s">
         <v>29</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="K86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L86"/>
       <c r="M86" t="s">
@@ -4873,10 +4879,10 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B87" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C87" t="s">
         <v>9</v>
@@ -4885,22 +4891,22 @@
         <v>38687</v>
       </c>
       <c r="E87" t="s">
+        <v>141</v>
+      </c>
+      <c r="F87" t="s">
         <v>142</v>
       </c>
-      <c r="F87" t="s">
+      <c r="G87" t="s">
         <v>143</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H87" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="H87" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="J87" s="5" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="K87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L87"/>
       <c r="M87" t="s">
@@ -4909,10 +4915,10 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B88" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C88" t="s">
         <v>8</v>
@@ -4921,22 +4927,22 @@
         <v>43282</v>
       </c>
       <c r="E88" t="s">
+        <v>145</v>
+      </c>
+      <c r="F88" t="s">
         <v>146</v>
-      </c>
-      <c r="F88" t="s">
-        <v>147</v>
       </c>
       <c r="G88" t="s">
         <v>33</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="K88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L88"/>
       <c r="M88" t="s">
@@ -4948,7 +4954,7 @@
         <v>19</v>
       </c>
       <c r="B89" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C89" t="s">
         <v>10</v>
@@ -4957,22 +4963,22 @@
         <v>39052</v>
       </c>
       <c r="E89" t="s">
+        <v>257</v>
+      </c>
+      <c r="F89" t="s">
         <v>258</v>
       </c>
-      <c r="F89" t="s">
+      <c r="G89" t="s">
+        <v>258</v>
+      </c>
+      <c r="H89" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G89" t="s">
-        <v>259</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>260</v>
-      </c>
       <c r="J89" s="5" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="K89" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="L89"/>
       <c r="M89" t="s">
@@ -4981,10 +4987,10 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B90" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C90" t="s">
         <v>48</v>
@@ -4993,22 +4999,22 @@
         <v>41426</v>
       </c>
       <c r="E90" t="s">
+        <v>152</v>
+      </c>
+      <c r="F90" t="s">
         <v>153</v>
       </c>
-      <c r="F90" t="s">
+      <c r="G90" t="s">
         <v>154</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H90" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="J90" s="5" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="K90" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L90"/>
       <c r="M90" t="s">
@@ -5017,10 +5023,10 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B91" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
@@ -5029,22 +5035,22 @@
         <v>38838</v>
       </c>
       <c r="E91" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F91" t="s">
         <v>32</v>
       </c>
       <c r="G91" t="s">
+        <v>116</v>
+      </c>
+      <c r="H91" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H91" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="J91" s="5" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="K91" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L91"/>
       <c r="M91" t="s">
@@ -5053,10 +5059,10 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B92" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -5065,7 +5071,7 @@
         <v>36951</v>
       </c>
       <c r="E92" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F92" t="s">
         <v>32</v>
@@ -5074,13 +5080,13 @@
         <v>33</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="K92" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="L92"/>
       <c r="M92" t="s">
@@ -5092,7 +5098,7 @@
         <v>19</v>
       </c>
       <c r="B93" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C93" t="s">
         <v>71</v>
@@ -5101,22 +5107,22 @@
         <v>38534</v>
       </c>
       <c r="E93" t="s">
+        <v>239</v>
+      </c>
+      <c r="F93" t="s">
         <v>240</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>241</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H93" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="H93" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="J93" s="5" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="K93" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="L93"/>
       <c r="M93" t="s">
@@ -5125,10 +5131,10 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B94" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C94" t="s">
         <v>8</v>
@@ -5149,10 +5155,10 @@
         <v>44</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="K94" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L94"/>
       <c r="M94" t="s">
@@ -5164,7 +5170,7 @@
         <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C95" t="s">
         <v>9</v>
@@ -5179,16 +5185,16 @@
         <v>40</v>
       </c>
       <c r="G95" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="J95" s="5" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="K95" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L95"/>
       <c r="M95" t="s">
@@ -5200,7 +5206,7 @@
         <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C96" t="s">
         <v>11</v>
@@ -5209,22 +5215,22 @@
         <v>41852</v>
       </c>
       <c r="E96" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F96" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G96" t="s">
         <v>33</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="K96" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="L96"/>
       <c r="M96" t="s">
@@ -5233,10 +5239,10 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B97" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C97" t="s">
         <v>12</v>
@@ -5245,22 +5251,22 @@
         <v>40299</v>
       </c>
       <c r="E97" t="s">
+        <v>174</v>
+      </c>
+      <c r="F97" t="s">
         <v>175</v>
       </c>
-      <c r="F97" t="s">
+      <c r="G97" t="s">
         <v>176</v>
       </c>
-      <c r="G97" t="s">
+      <c r="H97" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="H97" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="J97" s="5" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="K97" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L97"/>
       <c r="M97" t="s">
@@ -5269,10 +5275,10 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B98" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C98" t="s">
         <v>11</v>
@@ -5281,22 +5287,22 @@
         <v>39295</v>
       </c>
       <c r="E98" t="s">
+        <v>156</v>
+      </c>
+      <c r="F98" t="s">
         <v>157</v>
       </c>
-      <c r="F98" t="s">
+      <c r="G98" t="s">
         <v>158</v>
       </c>
-      <c r="G98" t="s">
+      <c r="H98" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H98" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="J98" s="5" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="K98" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L98"/>
       <c r="M98" t="s">
@@ -5305,10 +5311,10 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B99" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C99" t="s">
         <v>52</v>
@@ -5317,22 +5323,22 @@
         <v>39203</v>
       </c>
       <c r="E99" t="s">
+        <v>111</v>
+      </c>
+      <c r="F99" t="s">
         <v>112</v>
       </c>
-      <c r="F99" t="s">
+      <c r="G99" t="s">
         <v>113</v>
       </c>
-      <c r="G99" t="s">
+      <c r="H99" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H99" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="J99" s="5" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="K99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L99"/>
       <c r="M99" t="s">
@@ -5345,10 +5351,10 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B101" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C101" t="s">
         <v>10</v>
@@ -5357,22 +5363,22 @@
         <v>44317</v>
       </c>
       <c r="E101" t="s">
+        <v>211</v>
+      </c>
+      <c r="F101" t="s">
+        <v>112</v>
+      </c>
+      <c r="G101" t="s">
         <v>212</v>
       </c>
-      <c r="F101" t="s">
-        <v>113</v>
-      </c>
-      <c r="G101" t="s">
+      <c r="H101" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H101" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="J101" s="5" t="s">
-        <v>362</v>
+        <v>477</v>
       </c>
       <c r="K101" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="M101" t="s">
         <v>20</v>
@@ -5380,10 +5386,10 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B102" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C102" t="s">
         <v>45</v>
@@ -5392,22 +5398,22 @@
         <v>41548</v>
       </c>
       <c r="E102" t="s">
+        <v>199</v>
+      </c>
+      <c r="F102" t="s">
         <v>200</v>
       </c>
-      <c r="F102" t="s">
+      <c r="G102" t="s">
+        <v>139</v>
+      </c>
+      <c r="H102" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="G102" t="s">
-        <v>140</v>
-      </c>
-      <c r="H102" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="J102" s="5" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="K102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L102"/>
       <c r="M102" t="s">
@@ -5419,7 +5425,7 @@
         <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C103" t="s">
         <v>48</v>
@@ -5428,22 +5434,22 @@
         <v>44378</v>
       </c>
       <c r="E103" t="s">
+        <v>226</v>
+      </c>
+      <c r="F103" t="s">
         <v>227</v>
-      </c>
-      <c r="F103" t="s">
-        <v>228</v>
       </c>
       <c r="G103" t="s">
         <v>29</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J103" s="5" t="s">
-        <v>364</v>
+        <v>482</v>
       </c>
       <c r="K103" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="M103" t="s">
         <v>20</v>
@@ -5451,10 +5457,10 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B104" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C104" t="s">
         <v>50</v>
@@ -5463,22 +5469,22 @@
         <v>43709</v>
       </c>
       <c r="E104" t="s">
+        <v>261</v>
+      </c>
+      <c r="F104" t="s">
         <v>262</v>
       </c>
-      <c r="F104" t="s">
+      <c r="G104" t="s">
         <v>263</v>
       </c>
-      <c r="G104" t="s">
+      <c r="H104" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="H104" s="2" t="s">
-        <v>265</v>
-      </c>
       <c r="J104" s="5" t="s">
-        <v>365</v>
+        <v>483</v>
       </c>
       <c r="K104" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="M104" t="s">
         <v>20</v>
@@ -5489,7 +5495,7 @@
         <v>19</v>
       </c>
       <c r="B105" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C105" t="s">
         <v>52</v>
@@ -5498,22 +5504,22 @@
         <v>43862</v>
       </c>
       <c r="E105" t="s">
+        <v>223</v>
+      </c>
+      <c r="F105" t="s">
         <v>224</v>
       </c>
-      <c r="F105" t="s">
+      <c r="G105" t="s">
+        <v>112</v>
+      </c>
+      <c r="H105" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="G105" t="s">
-        <v>113</v>
-      </c>
-      <c r="H105" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="J105" s="5" t="s">
-        <v>363</v>
+        <v>479</v>
       </c>
       <c r="K105" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="M105" t="s">
         <v>20</v>
@@ -5524,7 +5530,7 @@
         <v>19</v>
       </c>
       <c r="B106" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C106" t="s">
         <v>45</v>
@@ -5533,22 +5539,22 @@
         <v>41730</v>
       </c>
       <c r="E106" t="s">
+        <v>271</v>
+      </c>
+      <c r="F106" t="s">
         <v>272</v>
       </c>
-      <c r="F106" t="s">
+      <c r="G106" t="s">
+        <v>112</v>
+      </c>
+      <c r="H106" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="G106" t="s">
-        <v>113</v>
-      </c>
-      <c r="H106" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="J106" s="5" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="K106" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="L106"/>
       <c r="M106" t="s">
@@ -6190,7 +6196,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1">
         <v>4.7</v>
@@ -6198,7 +6204,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2">
         <v>1.6</v>
@@ -6206,7 +6212,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3">
         <v>0.1</v>
@@ -6214,7 +6220,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4">
         <v>23.6</v>
@@ -6222,7 +6228,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5">
         <v>0.2</v>
@@ -6230,7 +6236,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6">
         <v>6.7</v>
@@ -6238,7 +6244,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7">
         <v>0.6</v>
@@ -6246,7 +6252,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -6273,10 +6279,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Perfecta generacion de IBAN-> Aunque a los duplicados no se lo hace
</commit_message>
<xml_diff>
--- a/SIS2-2020/resources/SistemasInformacionII.xlsx
+++ b/SIS2-2020/resources/SistemasInformacionII.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="584">
   <si>
     <t>Nombre</t>
   </si>
@@ -1493,6 +1493,294 @@
   </si>
   <si>
     <t>31645124473461205164</t>
+  </si>
+  <si>
+    <t>ES8265614874165615445616</t>
+  </si>
+  <si>
+    <t>ES3520960043043554600000</t>
+  </si>
+  <si>
+    <t>DK7331645124473461205164</t>
+  </si>
+  <si>
+    <t>RO8832569523016220165156</t>
+  </si>
+  <si>
+    <t>DE7424561937521546497521</t>
+  </si>
+  <si>
+    <t>AT6825030000114574745458</t>
+  </si>
+  <si>
+    <t>DK5800750184310702510000</t>
+  </si>
+  <si>
+    <t>SM7325635478321002541225</t>
+  </si>
+  <si>
+    <t>DE9301821135910205540000</t>
+  </si>
+  <si>
+    <t>ES8462581542713690044508</t>
+  </si>
+  <si>
+    <t>ES9021651651812511133551</t>
+  </si>
+  <si>
+    <t>ES6832154697195423121000</t>
+  </si>
+  <si>
+    <t>ES9001826530120201560000</t>
+  </si>
+  <si>
+    <t>ES6931624561042546920007</t>
+  </si>
+  <si>
+    <t>ES4723164897642213030615</t>
+  </si>
+  <si>
+    <t>ES9232584216971684051000</t>
+  </si>
+  <si>
+    <t>IE6851556584221251000254</t>
+  </si>
+  <si>
+    <t>ES8220960043042158800000</t>
+  </si>
+  <si>
+    <t>ES4534698752714600549403</t>
+  </si>
+  <si>
+    <t>AT3122515651915640081000</t>
+  </si>
+  <si>
+    <t>ES5020960043073071400000</t>
+  </si>
+  <si>
+    <t>ES5023455254943263234457</t>
+  </si>
+  <si>
+    <t>ES9012548523465214585214</t>
+  </si>
+  <si>
+    <t>ES7631245164156597845124</t>
+  </si>
+  <si>
+    <t>DE5512669681115112121210</t>
+  </si>
+  <si>
+    <t>IT8915953684811254695203</t>
+  </si>
+  <si>
+    <t>DE5021508149175421346497</t>
+  </si>
+  <si>
+    <t>ES2766649444162310000255</t>
+  </si>
+  <si>
+    <t>CZ9536250012804785523365</t>
+  </si>
+  <si>
+    <t>ES3925165151118666365100</t>
+  </si>
+  <si>
+    <t>FR3820012541150023365233</t>
+  </si>
+  <si>
+    <t>ES2396536214865214585214</t>
+  </si>
+  <si>
+    <t>ES6885461325251978750005</t>
+  </si>
+  <si>
+    <t>ES7221416325811510005514</t>
+  </si>
+  <si>
+    <t>BE9400750184310702510000</t>
+  </si>
+  <si>
+    <t>ES9712548521518742146695</t>
+  </si>
+  <si>
+    <t>ES7521654587985156484454</t>
+  </si>
+  <si>
+    <t>ES7426221011628048788896</t>
+  </si>
+  <si>
+    <t>PT3536952365020014425254</t>
+  </si>
+  <si>
+    <t>ES7223652365142254222000</t>
+  </si>
+  <si>
+    <t>ES1665165654918886005001</t>
+  </si>
+  <si>
+    <t>LU0932628484504115151115</t>
+  </si>
+  <si>
+    <t>GR3836521452736500658485</t>
+  </si>
+  <si>
+    <t>MC6436520125638451012515</t>
+  </si>
+  <si>
+    <t>DE7822631245526916432102</t>
+  </si>
+  <si>
+    <t>ES3220960583831234500000</t>
+  </si>
+  <si>
+    <t>AT3285550564726165145610</t>
+  </si>
+  <si>
+    <t>GB9720910936583000000000</t>
+  </si>
+  <si>
+    <t>ES2956187775315550000651</t>
+  </si>
+  <si>
+    <t>ES8020960043033000100000</t>
+  </si>
+  <si>
+    <t>FI6132658012367712548745</t>
+  </si>
+  <si>
+    <t>PT5764578946740051516490</t>
+  </si>
+  <si>
+    <t>ES4352198484752100515144</t>
+  </si>
+  <si>
+    <t>IT3526551681807651415636</t>
+  </si>
+  <si>
+    <t>ES5631215643855060225021</t>
+  </si>
+  <si>
+    <t>ES2120960043043075700000</t>
+  </si>
+  <si>
+    <t>GB5520008521528775113366</t>
+  </si>
+  <si>
+    <t>ES6855065688761051056105</t>
+  </si>
+  <si>
+    <t>HU2399558741836555551120</t>
+  </si>
+  <si>
+    <t>LT9321856333126985542360</t>
+  </si>
+  <si>
+    <t>ES6223658965274585223202</t>
+  </si>
+  <si>
+    <t>ES0425516848021156151054</t>
+  </si>
+  <si>
+    <t>GR9420125003305201112544</t>
+  </si>
+  <si>
+    <t>ES5736245978133245679001</t>
+  </si>
+  <si>
+    <t>ES7395485212315484010000</t>
+  </si>
+  <si>
+    <t>ES3720960043032159000000</t>
+  </si>
+  <si>
+    <t>ES1633620012937852100256</t>
+  </si>
+  <si>
+    <t>ES9020960043023096200000</t>
+  </si>
+  <si>
+    <t>GR4920910936583000000000</t>
+  </si>
+  <si>
+    <t>DK9032541112811220000588</t>
+  </si>
+  <si>
+    <t>GB0836585214290025478551</t>
+  </si>
+  <si>
+    <t>ES7920960031442124800000</t>
+  </si>
+  <si>
+    <t>ES2821651484690980008984</t>
+  </si>
+  <si>
+    <t>ES1933218885441445121022</t>
+  </si>
+  <si>
+    <t>ES6851651487910005118185</t>
+  </si>
+  <si>
+    <t>FI5620960043043554600000</t>
+  </si>
+  <si>
+    <t>ES5566552211148855332200</t>
+  </si>
+  <si>
+    <t>ES1436154231712500312566</t>
+  </si>
+  <si>
+    <t>ES9596431245118150005156</t>
+  </si>
+  <si>
+    <t>DE6721346154503164978451</t>
+  </si>
+  <si>
+    <t>ES2220960056133231500000</t>
+  </si>
+  <si>
+    <t>LT8032566221522587754554</t>
+  </si>
+  <si>
+    <t>EE2023215465315456411515</t>
+  </si>
+  <si>
+    <t>ES8244875664127231645789</t>
+  </si>
+  <si>
+    <t>ES9565168874641561561500</t>
+  </si>
+  <si>
+    <t>SM4423221158252545471411</t>
+  </si>
+  <si>
+    <t>LT9362541122421110105611</t>
+  </si>
+  <si>
+    <t>SE6832574512085411002255</t>
+  </si>
+  <si>
+    <t>ES8163516541828944000984</t>
+  </si>
+  <si>
+    <t>SM2125894363475485700145</t>
+  </si>
+  <si>
+    <t>FR5623185484465641685100</t>
+  </si>
+  <si>
+    <t>AT8365645150865168448896</t>
+  </si>
+  <si>
+    <t>ES3251651681961210656510</t>
+  </si>
+  <si>
+    <t>ES4420960043013468900000</t>
+  </si>
+  <si>
+    <t>ES7225187786311225455548</t>
+  </si>
+  <si>
+    <t>FI5024587946032003165464</t>
   </si>
 </sst>
 </file>
@@ -1999,7 +2287,9 @@
       <c r="K2" t="s">
         <v>84</v>
       </c>
-      <c r="L2"/>
+      <c r="L2" t="s">
+        <v>489</v>
+      </c>
       <c r="M2" t="s">
         <v>53</v>
       </c>
@@ -2071,7 +2361,9 @@
       <c r="K4" t="s">
         <v>89</v>
       </c>
-      <c r="L4"/>
+      <c r="L4" t="s">
+        <v>490</v>
+      </c>
       <c r="M4" t="s">
         <v>53</v>
       </c>
@@ -2107,7 +2399,9 @@
       <c r="K5" t="s">
         <v>84</v>
       </c>
-      <c r="L5"/>
+      <c r="L5" t="s">
+        <v>488</v>
+      </c>
       <c r="M5" t="s">
         <v>53</v>
       </c>
@@ -2143,7 +2437,9 @@
       <c r="K6" t="s">
         <v>368</v>
       </c>
-      <c r="L6"/>
+      <c r="L6" t="s">
+        <v>491</v>
+      </c>
       <c r="M6" t="s">
         <v>53</v>
       </c>
@@ -2179,7 +2475,9 @@
       <c r="K7" t="s">
         <v>85</v>
       </c>
-      <c r="L7"/>
+      <c r="L7" t="s">
+        <v>492</v>
+      </c>
       <c r="M7" t="s">
         <v>20</v>
       </c>
@@ -2215,7 +2513,9 @@
       <c r="K8" t="s">
         <v>361</v>
       </c>
-      <c r="L8"/>
+      <c r="L8" t="s">
+        <v>531</v>
+      </c>
       <c r="M8" t="s">
         <v>20</v>
       </c>
@@ -2255,7 +2555,9 @@
       <c r="K10" t="s">
         <v>86</v>
       </c>
-      <c r="L10"/>
+      <c r="L10" t="s">
+        <v>550</v>
+      </c>
       <c r="M10" t="s">
         <v>53</v>
       </c>
@@ -2291,7 +2593,9 @@
       <c r="K11" t="s">
         <v>84</v>
       </c>
-      <c r="L11"/>
+      <c r="L11" t="s">
+        <v>560</v>
+      </c>
       <c r="M11" t="s">
         <v>53</v>
       </c>
@@ -2327,7 +2631,9 @@
       <c r="K12" t="s">
         <v>88</v>
       </c>
-      <c r="L12"/>
+      <c r="L12" t="s">
+        <v>563</v>
+      </c>
       <c r="M12" t="s">
         <v>53</v>
       </c>
@@ -2399,7 +2705,9 @@
       <c r="K14" t="s">
         <v>365</v>
       </c>
-      <c r="L14"/>
+      <c r="L14" t="s">
+        <v>569</v>
+      </c>
       <c r="M14" t="s">
         <v>20</v>
       </c>
@@ -2435,7 +2743,9 @@
       <c r="K15" t="s">
         <v>371</v>
       </c>
-      <c r="L15"/>
+      <c r="L15" t="s">
+        <v>570</v>
+      </c>
       <c r="M15" t="s">
         <v>53</v>
       </c>
@@ -2468,7 +2778,9 @@
       <c r="K16" t="s">
         <v>87</v>
       </c>
-      <c r="L16"/>
+      <c r="L16" t="s">
+        <v>522</v>
+      </c>
       <c r="M16" t="s">
         <v>20</v>
       </c>
@@ -2540,7 +2852,9 @@
       <c r="K18" t="s">
         <v>370</v>
       </c>
-      <c r="L18"/>
+      <c r="L18" t="s">
+        <v>577</v>
+      </c>
       <c r="M18" t="s">
         <v>20</v>
       </c>
@@ -2576,7 +2890,9 @@
       <c r="K19" t="s">
         <v>84</v>
       </c>
-      <c r="L19"/>
+      <c r="L19" t="s">
+        <v>566</v>
+      </c>
       <c r="M19" t="s">
         <v>53</v>
       </c>
@@ -2612,7 +2928,9 @@
       <c r="K20" t="s">
         <v>362</v>
       </c>
-      <c r="L20"/>
+      <c r="L20" t="s">
+        <v>493</v>
+      </c>
       <c r="M20" t="s">
         <v>20</v>
       </c>
@@ -2648,7 +2966,9 @@
       <c r="K21" t="s">
         <v>364</v>
       </c>
-      <c r="L21"/>
+      <c r="L21" t="s">
+        <v>513</v>
+      </c>
       <c r="M21" t="s">
         <v>53</v>
       </c>
@@ -2684,7 +3004,9 @@
       <c r="K22" t="s">
         <v>84</v>
       </c>
-      <c r="L22"/>
+      <c r="L22" t="s">
+        <v>555</v>
+      </c>
       <c r="M22" t="s">
         <v>53</v>
       </c>
@@ -2717,7 +3039,9 @@
       <c r="K23" t="s">
         <v>89</v>
       </c>
-      <c r="L23"/>
+      <c r="L23" t="s">
+        <v>494</v>
+      </c>
       <c r="M23" t="s">
         <v>20</v>
       </c>
@@ -2753,7 +3077,9 @@
       <c r="K24" t="s">
         <v>84</v>
       </c>
-      <c r="L24"/>
+      <c r="L24" t="s">
+        <v>509</v>
+      </c>
       <c r="M24" t="s">
         <v>20</v>
       </c>
@@ -2786,7 +3112,9 @@
       <c r="K25" t="s">
         <v>86</v>
       </c>
-      <c r="L25"/>
+      <c r="L25" t="s">
+        <v>556</v>
+      </c>
       <c r="M25" t="s">
         <v>20</v>
       </c>
@@ -2822,7 +3150,9 @@
       <c r="K26" t="s">
         <v>84</v>
       </c>
-      <c r="L26"/>
+      <c r="L26" t="s">
+        <v>553</v>
+      </c>
       <c r="M26" t="s">
         <v>53</v>
       </c>
@@ -2858,7 +3188,9 @@
       <c r="K27" t="s">
         <v>85</v>
       </c>
-      <c r="L27"/>
+      <c r="L27" t="s">
+        <v>512</v>
+      </c>
       <c r="M27" t="s">
         <v>53</v>
       </c>
@@ -2898,7 +3230,9 @@
       <c r="K29" t="s">
         <v>84</v>
       </c>
-      <c r="L29"/>
+      <c r="L29" t="s">
+        <v>536</v>
+      </c>
       <c r="M29" t="s">
         <v>53</v>
       </c>
@@ -2934,7 +3268,9 @@
       <c r="K30" t="s">
         <v>84</v>
       </c>
-      <c r="L30"/>
+      <c r="L30" t="s">
+        <v>549</v>
+      </c>
       <c r="M30" t="s">
         <v>20</v>
       </c>
@@ -2970,7 +3306,9 @@
       <c r="K31" t="s">
         <v>374</v>
       </c>
-      <c r="L31"/>
+      <c r="L31" t="s">
+        <v>539</v>
+      </c>
       <c r="M31" t="s">
         <v>53</v>
       </c>
@@ -3006,7 +3344,9 @@
       <c r="K32" t="s">
         <v>84</v>
       </c>
-      <c r="L32"/>
+      <c r="L32" t="s">
+        <v>506</v>
+      </c>
       <c r="M32" t="s">
         <v>20</v>
       </c>
@@ -3042,7 +3382,9 @@
       <c r="K33" t="s">
         <v>84</v>
       </c>
-      <c r="L33"/>
+      <c r="L33" t="s">
+        <v>515</v>
+      </c>
       <c r="M33" t="s">
         <v>20</v>
       </c>
@@ -3078,7 +3420,9 @@
       <c r="K34" t="s">
         <v>372</v>
       </c>
-      <c r="L34"/>
+      <c r="L34" t="s">
+        <v>578</v>
+      </c>
       <c r="M34" t="s">
         <v>20</v>
       </c>
@@ -3114,7 +3458,9 @@
       <c r="K35" t="s">
         <v>84</v>
       </c>
-      <c r="L35"/>
+      <c r="L35" t="s">
+        <v>540</v>
+      </c>
       <c r="M35" t="s">
         <v>53</v>
       </c>
@@ -3150,7 +3496,9 @@
       <c r="K36" t="s">
         <v>367</v>
       </c>
-      <c r="L36"/>
+      <c r="L36" t="s">
+        <v>516</v>
+      </c>
       <c r="M36" t="s">
         <v>53</v>
       </c>
@@ -3186,7 +3534,9 @@
       <c r="K37" t="s">
         <v>362</v>
       </c>
-      <c r="L37"/>
+      <c r="L37" t="s">
+        <v>507</v>
+      </c>
       <c r="M37" t="s">
         <v>53</v>
       </c>
@@ -3222,7 +3572,9 @@
       <c r="K38" t="s">
         <v>85</v>
       </c>
-      <c r="L38"/>
+      <c r="L38" t="s">
+        <v>514</v>
+      </c>
       <c r="M38" t="s">
         <v>53</v>
       </c>
@@ -3258,7 +3610,9 @@
       <c r="K39" t="s">
         <v>85</v>
       </c>
-      <c r="L39"/>
+      <c r="L39" t="s">
+        <v>567</v>
+      </c>
       <c r="M39" t="s">
         <v>20</v>
       </c>
@@ -3294,7 +3648,9 @@
       <c r="K40" t="s">
         <v>84</v>
       </c>
-      <c r="L40"/>
+      <c r="L40" t="s">
+        <v>582</v>
+      </c>
       <c r="M40" t="s">
         <v>53</v>
       </c>
@@ -3330,7 +3686,9 @@
       <c r="K41" t="s">
         <v>84</v>
       </c>
-      <c r="L41"/>
+      <c r="L41" t="s">
+        <v>502</v>
+      </c>
       <c r="M41" t="s">
         <v>53</v>
       </c>
@@ -3366,7 +3724,9 @@
       <c r="K42" t="s">
         <v>84</v>
       </c>
-      <c r="L42"/>
+      <c r="L42" t="s">
+        <v>519</v>
+      </c>
       <c r="M42" t="s">
         <v>53</v>
       </c>
@@ -3402,7 +3762,9 @@
       <c r="K43" t="s">
         <v>84</v>
       </c>
-      <c r="L43"/>
+      <c r="L43" t="s">
+        <v>520</v>
+      </c>
       <c r="M43" t="s">
         <v>53</v>
       </c>
@@ -3438,7 +3800,9 @@
       <c r="K44" t="s">
         <v>88</v>
       </c>
-      <c r="L44"/>
+      <c r="L44" t="s">
+        <v>583</v>
+      </c>
       <c r="M44" t="s">
         <v>53</v>
       </c>
@@ -3474,7 +3838,9 @@
       <c r="K45" t="s">
         <v>84</v>
       </c>
-      <c r="L45"/>
+      <c r="L45" t="s">
+        <v>508</v>
+      </c>
       <c r="M45" t="s">
         <v>53</v>
       </c>
@@ -3510,7 +3876,9 @@
       <c r="K46" t="s">
         <v>84</v>
       </c>
-      <c r="L46"/>
+      <c r="L46" t="s">
+        <v>505</v>
+      </c>
       <c r="M46" t="s">
         <v>53</v>
       </c>
@@ -3546,7 +3914,9 @@
       <c r="K47" t="s">
         <v>84</v>
       </c>
-      <c r="L47"/>
+      <c r="L47" t="s">
+        <v>524</v>
+      </c>
       <c r="M47" t="s">
         <v>53</v>
       </c>
@@ -3582,7 +3952,9 @@
       <c r="K48" t="s">
         <v>84</v>
       </c>
-      <c r="L48"/>
+      <c r="L48" t="s">
+        <v>580</v>
+      </c>
       <c r="M48" t="s">
         <v>53</v>
       </c>
@@ -3618,7 +3990,9 @@
       <c r="K49" t="s">
         <v>84</v>
       </c>
-      <c r="L49"/>
+      <c r="L49" t="s">
+        <v>564</v>
+      </c>
       <c r="M49" t="s">
         <v>20</v>
       </c>
@@ -3651,7 +4025,9 @@
       <c r="K50" t="s">
         <v>90</v>
       </c>
-      <c r="L50"/>
+      <c r="L50" t="s">
+        <v>535</v>
+      </c>
       <c r="M50" t="s">
         <v>20</v>
       </c>
@@ -3684,7 +4060,9 @@
       <c r="K51" t="s">
         <v>85</v>
       </c>
-      <c r="L51"/>
+      <c r="L51" t="s">
+        <v>496</v>
+      </c>
       <c r="M51" t="s">
         <v>20</v>
       </c>
@@ -3720,7 +4098,9 @@
       <c r="K52" t="s">
         <v>85</v>
       </c>
-      <c r="L52"/>
+      <c r="L52" t="s">
+        <v>532</v>
+      </c>
       <c r="M52" t="s">
         <v>53</v>
       </c>
@@ -3756,7 +4136,9 @@
       <c r="K53" t="s">
         <v>84</v>
       </c>
-      <c r="L53"/>
+      <c r="L53" t="s">
+        <v>543</v>
+      </c>
       <c r="M53" t="s">
         <v>20</v>
       </c>
@@ -3792,7 +4174,9 @@
       <c r="K54" t="s">
         <v>370</v>
       </c>
-      <c r="L54"/>
+      <c r="L54" t="s">
+        <v>495</v>
+      </c>
       <c r="M54" t="s">
         <v>20</v>
       </c>
@@ -3828,7 +4212,9 @@
       <c r="K55" t="s">
         <v>84</v>
       </c>
-      <c r="L55"/>
+      <c r="L55" t="s">
+        <v>499</v>
+      </c>
       <c r="M55" t="s">
         <v>20</v>
       </c>
@@ -3864,7 +4250,9 @@
       <c r="K56" t="s">
         <v>86</v>
       </c>
-      <c r="L56"/>
+      <c r="L56" t="s">
+        <v>530</v>
+      </c>
       <c r="M56" t="s">
         <v>20</v>
       </c>
@@ -3900,7 +4288,9 @@
       <c r="K57" t="s">
         <v>90</v>
       </c>
-      <c r="L57"/>
+      <c r="L57" t="s">
+        <v>544</v>
+      </c>
       <c r="M57" t="s">
         <v>53</v>
       </c>
@@ -3936,7 +4326,9 @@
       <c r="K58" t="s">
         <v>84</v>
       </c>
-      <c r="L58"/>
+      <c r="L58" t="s">
+        <v>562</v>
+      </c>
       <c r="M58" t="s">
         <v>20</v>
       </c>
@@ -3976,7 +4368,9 @@
       <c r="K60" t="s">
         <v>84</v>
       </c>
-      <c r="L60"/>
+      <c r="L60" t="s">
+        <v>500</v>
+      </c>
       <c r="M60" t="s">
         <v>20</v>
       </c>
@@ -4012,7 +4406,9 @@
       <c r="K61" t="s">
         <v>84</v>
       </c>
-      <c r="L61"/>
+      <c r="L61" t="s">
+        <v>498</v>
+      </c>
       <c r="M61" t="s">
         <v>53</v>
       </c>
@@ -4048,7 +4444,9 @@
       <c r="K62" t="s">
         <v>84</v>
       </c>
-      <c r="L62"/>
+      <c r="L62" t="s">
+        <v>537</v>
+      </c>
       <c r="M62" t="s">
         <v>20</v>
       </c>
@@ -4084,7 +4482,9 @@
       <c r="K63" t="s">
         <v>90</v>
       </c>
-      <c r="L63"/>
+      <c r="L63" t="s">
+        <v>558</v>
+      </c>
       <c r="M63" t="s">
         <v>53</v>
       </c>
@@ -4120,7 +4520,9 @@
       <c r="K64" t="s">
         <v>84</v>
       </c>
-      <c r="L64"/>
+      <c r="L64" t="s">
+        <v>510</v>
+      </c>
       <c r="M64" t="s">
         <v>20</v>
       </c>
@@ -4156,7 +4558,9 @@
       <c r="K65" t="s">
         <v>84</v>
       </c>
-      <c r="L65"/>
+      <c r="L65" t="s">
+        <v>501</v>
+      </c>
       <c r="M65" t="s">
         <v>53</v>
       </c>
@@ -4192,7 +4596,9 @@
       <c r="K66" t="s">
         <v>84</v>
       </c>
-      <c r="L66"/>
+      <c r="L66" t="s">
+        <v>565</v>
+      </c>
       <c r="M66" t="s">
         <v>20</v>
       </c>
@@ -4228,7 +4634,9 @@
       <c r="K67" t="s">
         <v>84</v>
       </c>
-      <c r="L67"/>
+      <c r="L67" t="s">
+        <v>571</v>
+      </c>
       <c r="M67" t="s">
         <v>20</v>
       </c>
@@ -4264,7 +4672,9 @@
       <c r="K68" t="s">
         <v>84</v>
       </c>
-      <c r="L68"/>
+      <c r="L68" t="s">
+        <v>559</v>
+      </c>
       <c r="M68" t="s">
         <v>20</v>
       </c>
@@ -4300,7 +4710,9 @@
       <c r="K69" t="s">
         <v>84</v>
       </c>
-      <c r="L69"/>
+      <c r="L69" t="s">
+        <v>554</v>
+      </c>
       <c r="M69" t="s">
         <v>53</v>
       </c>
@@ -4336,7 +4748,9 @@
       <c r="K70" t="s">
         <v>84</v>
       </c>
-      <c r="L70"/>
+      <c r="L70" t="s">
+        <v>561</v>
+      </c>
       <c r="M70" t="s">
         <v>20</v>
       </c>
@@ -4372,7 +4786,9 @@
       <c r="K71" t="s">
         <v>84</v>
       </c>
-      <c r="L71"/>
+      <c r="L71" t="s">
+        <v>497</v>
+      </c>
       <c r="M71" t="s">
         <v>20</v>
       </c>
@@ -4408,7 +4824,9 @@
       <c r="K72" t="s">
         <v>84</v>
       </c>
-      <c r="L72"/>
+      <c r="L72" t="s">
+        <v>517</v>
+      </c>
       <c r="M72" t="s">
         <v>20</v>
       </c>
@@ -4444,7 +4862,9 @@
       <c r="K73" t="s">
         <v>84</v>
       </c>
-      <c r="L73"/>
+      <c r="L73" t="s">
+        <v>537</v>
+      </c>
       <c r="M73" t="s">
         <v>20</v>
       </c>
@@ -4480,7 +4900,9 @@
       <c r="K74" t="s">
         <v>374</v>
       </c>
-      <c r="L74"/>
+      <c r="L74" t="s">
+        <v>526</v>
+      </c>
       <c r="M74" t="s">
         <v>53</v>
       </c>
@@ -4516,7 +4938,9 @@
       <c r="K75" t="s">
         <v>84</v>
       </c>
-      <c r="L75"/>
+      <c r="L75" t="s">
+        <v>572</v>
+      </c>
       <c r="M75" t="s">
         <v>53</v>
       </c>
@@ -4552,7 +4976,9 @@
       <c r="K76" t="s">
         <v>84</v>
       </c>
-      <c r="L76"/>
+      <c r="L76" t="s">
+        <v>533</v>
+      </c>
       <c r="M76" t="s">
         <v>20</v>
       </c>
@@ -4588,7 +5014,9 @@
       <c r="K77" t="s">
         <v>84</v>
       </c>
-      <c r="L77"/>
+      <c r="L77" t="s">
+        <v>521</v>
+      </c>
       <c r="M77" t="s">
         <v>20</v>
       </c>
@@ -4624,7 +5052,9 @@
       <c r="K78" t="s">
         <v>366</v>
       </c>
-      <c r="L78"/>
+      <c r="L78" t="s">
+        <v>529</v>
+      </c>
       <c r="M78" t="s">
         <v>53</v>
       </c>
@@ -4662,6 +5092,9 @@
       <c r="K80" t="s">
         <v>84</v>
       </c>
+      <c r="L80" t="s">
+        <v>568</v>
+      </c>
       <c r="M80" t="s">
         <v>20</v>
       </c>
@@ -4697,7 +5130,9 @@
       <c r="K81" t="s">
         <v>84</v>
       </c>
-      <c r="L81"/>
+      <c r="L81" t="s">
+        <v>576</v>
+      </c>
       <c r="M81" t="s">
         <v>53</v>
       </c>
@@ -4733,6 +5168,9 @@
       <c r="K82" t="s">
         <v>84</v>
       </c>
+      <c r="L82" t="s">
+        <v>548</v>
+      </c>
       <c r="M82" t="s">
         <v>53</v>
       </c>
@@ -4768,7 +5206,9 @@
       <c r="K83" t="s">
         <v>88</v>
       </c>
-      <c r="L83"/>
+      <c r="L83" t="s">
+        <v>538</v>
+      </c>
       <c r="M83" t="s">
         <v>20</v>
       </c>
@@ -4804,7 +5244,9 @@
       <c r="K84" t="s">
         <v>84</v>
       </c>
-      <c r="L84"/>
+      <c r="L84" t="s">
+        <v>527</v>
+      </c>
       <c r="M84" t="s">
         <v>53</v>
       </c>
@@ -4837,6 +5279,9 @@
       <c r="K85" t="s">
         <v>372</v>
       </c>
+      <c r="L85" t="s">
+        <v>518</v>
+      </c>
       <c r="M85" t="s">
         <v>20</v>
       </c>
@@ -4872,7 +5317,9 @@
       <c r="K86" t="s">
         <v>84</v>
       </c>
-      <c r="L86"/>
+      <c r="L86" t="s">
+        <v>503</v>
+      </c>
       <c r="M86" t="s">
         <v>20</v>
       </c>
@@ -4908,7 +5355,9 @@
       <c r="K87" t="s">
         <v>84</v>
       </c>
-      <c r="L87"/>
+      <c r="L87" t="s">
+        <v>545</v>
+      </c>
       <c r="M87" t="s">
         <v>53</v>
       </c>
@@ -4944,7 +5393,9 @@
       <c r="K88" t="s">
         <v>84</v>
       </c>
-      <c r="L88"/>
+      <c r="L88" t="s">
+        <v>552</v>
+      </c>
       <c r="M88" t="s">
         <v>53</v>
       </c>
@@ -4980,7 +5431,9 @@
       <c r="K89" t="s">
         <v>365</v>
       </c>
-      <c r="L89"/>
+      <c r="L89" t="s">
+        <v>547</v>
+      </c>
       <c r="M89" t="s">
         <v>20</v>
       </c>
@@ -5016,7 +5469,9 @@
       <c r="K90" t="s">
         <v>84</v>
       </c>
-      <c r="L90"/>
+      <c r="L90" t="s">
+        <v>551</v>
+      </c>
       <c r="M90" t="s">
         <v>20</v>
       </c>
@@ -5052,7 +5507,9 @@
       <c r="K91" t="s">
         <v>84</v>
       </c>
-      <c r="L91"/>
+      <c r="L91" t="s">
+        <v>511</v>
+      </c>
       <c r="M91" t="s">
         <v>20</v>
       </c>
@@ -5088,7 +5545,9 @@
       <c r="K92" t="s">
         <v>370</v>
       </c>
-      <c r="L92"/>
+      <c r="L92" t="s">
+        <v>573</v>
+      </c>
       <c r="M92" t="s">
         <v>20</v>
       </c>
@@ -5124,7 +5583,9 @@
       <c r="K93" t="s">
         <v>369</v>
       </c>
-      <c r="L93"/>
+      <c r="L93" t="s">
+        <v>575</v>
+      </c>
       <c r="M93" t="s">
         <v>53</v>
       </c>
@@ -5160,7 +5621,9 @@
       <c r="K94" t="s">
         <v>84</v>
       </c>
-      <c r="L94"/>
+      <c r="L94" t="s">
+        <v>581</v>
+      </c>
       <c r="M94" t="s">
         <v>20</v>
       </c>
@@ -5196,7 +5659,9 @@
       <c r="K95" t="s">
         <v>84</v>
       </c>
-      <c r="L95"/>
+      <c r="L95" t="s">
+        <v>542</v>
+      </c>
       <c r="M95" t="s">
         <v>20</v>
       </c>
@@ -5232,7 +5697,9 @@
       <c r="K96" t="s">
         <v>362</v>
       </c>
-      <c r="L96"/>
+      <c r="L96" t="s">
+        <v>534</v>
+      </c>
       <c r="M96" t="s">
         <v>20</v>
       </c>
@@ -5268,7 +5735,9 @@
       <c r="K97" t="s">
         <v>84</v>
       </c>
-      <c r="L97"/>
+      <c r="L97" t="s">
+        <v>528</v>
+      </c>
       <c r="M97" t="s">
         <v>20</v>
       </c>
@@ -5304,7 +5773,9 @@
       <c r="K98" t="s">
         <v>84</v>
       </c>
-      <c r="L98"/>
+      <c r="L98" t="s">
+        <v>525</v>
+      </c>
       <c r="M98" t="s">
         <v>20</v>
       </c>
@@ -5340,7 +5811,9 @@
       <c r="K99" t="s">
         <v>84</v>
       </c>
-      <c r="L99"/>
+      <c r="L99" t="s">
+        <v>523</v>
+      </c>
       <c r="M99" t="s">
         <v>20</v>
       </c>
@@ -5380,6 +5853,9 @@
       <c r="K101" t="s">
         <v>363</v>
       </c>
+      <c r="L101" t="s">
+        <v>504</v>
+      </c>
       <c r="M101" t="s">
         <v>20</v>
       </c>
@@ -5415,7 +5891,9 @@
       <c r="K102" t="s">
         <v>89</v>
       </c>
-      <c r="L102"/>
+      <c r="L102" t="s">
+        <v>557</v>
+      </c>
       <c r="M102" t="s">
         <v>20</v>
       </c>
@@ -5451,6 +5929,9 @@
       <c r="K103" t="s">
         <v>365</v>
       </c>
+      <c r="L103" t="s">
+        <v>574</v>
+      </c>
       <c r="M103" t="s">
         <v>20</v>
       </c>
@@ -5486,6 +5967,9 @@
       <c r="K104" t="s">
         <v>362</v>
       </c>
+      <c r="L104" t="s">
+        <v>579</v>
+      </c>
       <c r="M104" t="s">
         <v>20</v>
       </c>
@@ -5521,6 +6005,9 @@
       <c r="K105" t="s">
         <v>364</v>
       </c>
+      <c r="L105" t="s">
+        <v>541</v>
+      </c>
       <c r="M105" t="s">
         <v>20</v>
       </c>
@@ -5556,7 +6043,9 @@
       <c r="K106" t="s">
         <v>373</v>
       </c>
-      <c r="L106"/>
+      <c r="L106" t="s">
+        <v>546</v>
+      </c>
       <c r="M106" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Modificacion NIF/NIE -> Funcionando ahora bien
</commit_message>
<xml_diff>
--- a/SIS2-2020/resources/SistemasInformacionII.xlsx
+++ b/SIS2-2020/resources/SistemasInformacionII.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\NetBeansProjects\SIS2-2020\SIS2-2020\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4081F765-3B9C-4F46-B96C-7E2636E64403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3551EBC0-E65F-461A-9382-184B17622728}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="1380" windowWidth="15375" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="582">
   <si>
     <t>Nombre</t>
   </si>
@@ -1483,304 +1483,298 @@
     <t>65645150865168448896</t>
   </si>
   <si>
-    <t>20960043053554600000</t>
-  </si>
-  <si>
-    <t>32145464178452163421</t>
-  </si>
-  <si>
-    <t>31645124483461205164</t>
-  </si>
-  <si>
     <t>31645124473461205164</t>
   </si>
   <si>
+    <t>AT6825030000114574745458</t>
+  </si>
+  <si>
+    <t>DK5800750184310702510000</t>
+  </si>
+  <si>
+    <t>SM7325635478321002541225</t>
+  </si>
+  <si>
+    <t>DE9301821135910205540000</t>
+  </si>
+  <si>
+    <t>ES8462581542713690044508</t>
+  </si>
+  <si>
+    <t>ES9021651651812511133551</t>
+  </si>
+  <si>
+    <t>ES6832154697195423121000</t>
+  </si>
+  <si>
+    <t>ES9001826530120201560000</t>
+  </si>
+  <si>
+    <t>ES6931624561042546920007</t>
+  </si>
+  <si>
+    <t>ES4723164897642213030615</t>
+  </si>
+  <si>
+    <t>ES9232584216971684051000</t>
+  </si>
+  <si>
+    <t>IE6851556584221251000254</t>
+  </si>
+  <si>
+    <t>ES8220960043042158800000</t>
+  </si>
+  <si>
+    <t>ES4534698752714600549403</t>
+  </si>
+  <si>
+    <t>AT3122515651915640081000</t>
+  </si>
+  <si>
+    <t>ES5020960043073071400000</t>
+  </si>
+  <si>
+    <t>ES5023455254943263234457</t>
+  </si>
+  <si>
+    <t>ES9012548523465214585214</t>
+  </si>
+  <si>
+    <t>ES7631245164156597845124</t>
+  </si>
+  <si>
+    <t>DE5512669681115112121210</t>
+  </si>
+  <si>
+    <t>IT8915953684811254695203</t>
+  </si>
+  <si>
+    <t>DE5021508149175421346497</t>
+  </si>
+  <si>
+    <t>ES2766649444162310000255</t>
+  </si>
+  <si>
+    <t>CZ9536250012804785523365</t>
+  </si>
+  <si>
+    <t>ES3925165151118666365100</t>
+  </si>
+  <si>
+    <t>FR3820012541150023365233</t>
+  </si>
+  <si>
+    <t>ES2396536214865214585214</t>
+  </si>
+  <si>
+    <t>ES6885461325251978750005</t>
+  </si>
+  <si>
+    <t>ES7221416325811510005514</t>
+  </si>
+  <si>
+    <t>ES9712548521518742146695</t>
+  </si>
+  <si>
+    <t>ES7521654587985156484454</t>
+  </si>
+  <si>
+    <t>ES7426221011628048788896</t>
+  </si>
+  <si>
+    <t>PT3536952365020014425254</t>
+  </si>
+  <si>
+    <t>ES7223652365142254222000</t>
+  </si>
+  <si>
+    <t>ES1665165654918886005001</t>
+  </si>
+  <si>
+    <t>LU0932628484504115151115</t>
+  </si>
+  <si>
+    <t>GR3836521452736500658485</t>
+  </si>
+  <si>
+    <t>DE7822631245526916432102</t>
+  </si>
+  <si>
+    <t>ES3220960583831234500000</t>
+  </si>
+  <si>
+    <t>AT3285550564726165145610</t>
+  </si>
+  <si>
+    <t>GB9720910936583000000000</t>
+  </si>
+  <si>
+    <t>ES2956187775315550000651</t>
+  </si>
+  <si>
+    <t>ES8020960043033000100000</t>
+  </si>
+  <si>
+    <t>FI6132658012367712548745</t>
+  </si>
+  <si>
+    <t>PT5764578946740051516490</t>
+  </si>
+  <si>
+    <t>ES4352198484752100515144</t>
+  </si>
+  <si>
+    <t>IT3526551681807651415636</t>
+  </si>
+  <si>
+    <t>ES5631215643855060225021</t>
+  </si>
+  <si>
+    <t>ES2120960043043075700000</t>
+  </si>
+  <si>
+    <t>GB5520008521528775113366</t>
+  </si>
+  <si>
+    <t>ES6855065688761051056105</t>
+  </si>
+  <si>
+    <t>HU2399558741836555551120</t>
+  </si>
+  <si>
+    <t>LT9321856333126985542360</t>
+  </si>
+  <si>
+    <t>ES6223658965274585223202</t>
+  </si>
+  <si>
+    <t>ES0425516848021156151054</t>
+  </si>
+  <si>
+    <t>ES5736245978133245679001</t>
+  </si>
+  <si>
+    <t>ES7395485212315484010000</t>
+  </si>
+  <si>
+    <t>ES3720960043032159000000</t>
+  </si>
+  <si>
+    <t>ES1633620012937852100256</t>
+  </si>
+  <si>
+    <t>ES9020960043023096200000</t>
+  </si>
+  <si>
+    <t>GR4920910936583000000000</t>
+  </si>
+  <si>
+    <t>DK9032541112811220000588</t>
+  </si>
+  <si>
+    <t>GB0836585214290025478551</t>
+  </si>
+  <si>
+    <t>ES7920960031442124800000</t>
+  </si>
+  <si>
+    <t>ES1933218885441445121022</t>
+  </si>
+  <si>
+    <t>ES6851651487910005118185</t>
+  </si>
+  <si>
+    <t>ES5566552211148855332200</t>
+  </si>
+  <si>
+    <t>ES1436154231712500312566</t>
+  </si>
+  <si>
+    <t>DE6721346154503164978451</t>
+  </si>
+  <si>
+    <t>ES2220960056133231500000</t>
+  </si>
+  <si>
+    <t>ES8244875664127231645789</t>
+  </si>
+  <si>
+    <t>ES9565168874641561561500</t>
+  </si>
+  <si>
+    <t>SM4423221158252545471411</t>
+  </si>
+  <si>
+    <t>LT9362541122421110105611</t>
+  </si>
+  <si>
+    <t>SE6832574512085411002255</t>
+  </si>
+  <si>
+    <t>ES8163516541828944000984</t>
+  </si>
+  <si>
+    <t>FR5623185484465641685100</t>
+  </si>
+  <si>
+    <t>AT8365645150865168448896</t>
+  </si>
+  <si>
+    <t>ES3251651681961210656510</t>
+  </si>
+  <si>
+    <t>ES4420960043013468900000</t>
+  </si>
+  <si>
+    <t>ES7225187786311225455548</t>
+  </si>
+  <si>
+    <t>FI5024587946032003165464</t>
+  </si>
+  <si>
+    <t>MC6436520125638451012515</t>
+  </si>
+  <si>
+    <t>DK7331645124473461205164</t>
+  </si>
+  <si>
+    <t>SM2125894363475485700145</t>
+  </si>
+  <si>
+    <t>ES9596431245118150005156</t>
+  </si>
+  <si>
+    <t>BE9400750184310702510000</t>
+  </si>
+  <si>
     <t>ES8265614874165615445616</t>
   </si>
   <si>
-    <t>ES3520960043043554600000</t>
-  </si>
-  <si>
-    <t>DK7331645124473461205164</t>
-  </si>
-  <si>
     <t>RO8832569523016220165156</t>
   </si>
   <si>
     <t>DE7424561937521546497521</t>
   </si>
   <si>
-    <t>AT6825030000114574745458</t>
-  </si>
-  <si>
-    <t>DK5800750184310702510000</t>
-  </si>
-  <si>
-    <t>SM7325635478321002541225</t>
-  </si>
-  <si>
-    <t>DE9301821135910205540000</t>
-  </si>
-  <si>
-    <t>ES8462581542713690044508</t>
-  </si>
-  <si>
-    <t>ES9021651651812511133551</t>
-  </si>
-  <si>
-    <t>ES6832154697195423121000</t>
-  </si>
-  <si>
-    <t>ES9001826530120201560000</t>
-  </si>
-  <si>
-    <t>ES6931624561042546920007</t>
-  </si>
-  <si>
-    <t>ES4723164897642213030615</t>
-  </si>
-  <si>
-    <t>ES9232584216971684051000</t>
-  </si>
-  <si>
-    <t>IE6851556584221251000254</t>
-  </si>
-  <si>
-    <t>ES8220960043042158800000</t>
-  </si>
-  <si>
-    <t>ES4534698752714600549403</t>
-  </si>
-  <si>
-    <t>AT3122515651915640081000</t>
-  </si>
-  <si>
-    <t>ES5020960043073071400000</t>
-  </si>
-  <si>
-    <t>ES5023455254943263234457</t>
-  </si>
-  <si>
-    <t>ES9012548523465214585214</t>
-  </si>
-  <si>
-    <t>ES7631245164156597845124</t>
-  </si>
-  <si>
-    <t>DE5512669681115112121210</t>
-  </si>
-  <si>
-    <t>IT8915953684811254695203</t>
-  </si>
-  <si>
-    <t>DE5021508149175421346497</t>
-  </si>
-  <si>
-    <t>ES2766649444162310000255</t>
-  </si>
-  <si>
-    <t>CZ9536250012804785523365</t>
-  </si>
-  <si>
-    <t>ES3925165151118666365100</t>
-  </si>
-  <si>
-    <t>FR3820012541150023365233</t>
-  </si>
-  <si>
-    <t>ES2396536214865214585214</t>
-  </si>
-  <si>
-    <t>ES6885461325251978750005</t>
-  </si>
-  <si>
-    <t>ES7221416325811510005514</t>
-  </si>
-  <si>
-    <t>BE9400750184310702510000</t>
-  </si>
-  <si>
-    <t>ES9712548521518742146695</t>
-  </si>
-  <si>
-    <t>ES7521654587985156484454</t>
-  </si>
-  <si>
-    <t>ES7426221011628048788896</t>
-  </si>
-  <si>
-    <t>PT3536952365020014425254</t>
-  </si>
-  <si>
-    <t>ES7223652365142254222000</t>
-  </si>
-  <si>
-    <t>ES1665165654918886005001</t>
-  </si>
-  <si>
-    <t>LU0932628484504115151115</t>
-  </si>
-  <si>
-    <t>GR3836521452736500658485</t>
-  </si>
-  <si>
-    <t>MC6436520125638451012515</t>
-  </si>
-  <si>
-    <t>DE7822631245526916432102</t>
-  </si>
-  <si>
-    <t>ES3220960583831234500000</t>
-  </si>
-  <si>
-    <t>AT3285550564726165145610</t>
-  </si>
-  <si>
-    <t>GB9720910936583000000000</t>
-  </si>
-  <si>
-    <t>ES2956187775315550000651</t>
-  </si>
-  <si>
-    <t>ES8020960043033000100000</t>
-  </si>
-  <si>
-    <t>FI6132658012367712548745</t>
-  </si>
-  <si>
-    <t>PT5764578946740051516490</t>
-  </si>
-  <si>
-    <t>ES4352198484752100515144</t>
-  </si>
-  <si>
-    <t>IT3526551681807651415636</t>
-  </si>
-  <si>
-    <t>ES5631215643855060225021</t>
-  </si>
-  <si>
-    <t>ES2120960043043075700000</t>
-  </si>
-  <si>
-    <t>GB5520008521528775113366</t>
-  </si>
-  <si>
-    <t>ES6855065688761051056105</t>
-  </si>
-  <si>
-    <t>HU2399558741836555551120</t>
-  </si>
-  <si>
-    <t>LT9321856333126985542360</t>
-  </si>
-  <si>
-    <t>ES6223658965274585223202</t>
-  </si>
-  <si>
-    <t>ES0425516848021156151054</t>
-  </si>
-  <si>
     <t>GR9420125003305201112544</t>
   </si>
   <si>
-    <t>ES5736245978133245679001</t>
-  </si>
-  <si>
-    <t>ES7395485212315484010000</t>
-  </si>
-  <si>
-    <t>ES3720960043032159000000</t>
-  </si>
-  <si>
-    <t>ES1633620012937852100256</t>
-  </si>
-  <si>
-    <t>ES9020960043023096200000</t>
-  </si>
-  <si>
-    <t>GR4920910936583000000000</t>
-  </si>
-  <si>
-    <t>DK9032541112811220000588</t>
-  </si>
-  <si>
-    <t>GB0836585214290025478551</t>
-  </si>
-  <si>
-    <t>ES7920960031442124800000</t>
-  </si>
-  <si>
     <t>ES2821651484690980008984</t>
   </si>
   <si>
-    <t>ES1933218885441445121022</t>
-  </si>
-  <si>
-    <t>ES6851651487910005118185</t>
-  </si>
-  <si>
     <t>FI5620960043043554600000</t>
   </si>
   <si>
-    <t>ES5566552211148855332200</t>
-  </si>
-  <si>
-    <t>ES1436154231712500312566</t>
-  </si>
-  <si>
-    <t>ES9596431245118150005156</t>
-  </si>
-  <si>
-    <t>DE6721346154503164978451</t>
-  </si>
-  <si>
-    <t>ES2220960056133231500000</t>
-  </si>
-  <si>
     <t>LT8032566221522587754554</t>
   </si>
   <si>
     <t>EE2023215465315456411515</t>
   </si>
   <si>
-    <t>ES8244875664127231645789</t>
-  </si>
-  <si>
-    <t>ES9565168874641561561500</t>
-  </si>
-  <si>
-    <t>SM4423221158252545471411</t>
-  </si>
-  <si>
-    <t>LT9362541122421110105611</t>
-  </si>
-  <si>
-    <t>SE6832574512085411002255</t>
-  </si>
-  <si>
-    <t>ES8163516541828944000984</t>
-  </si>
-  <si>
-    <t>SM2125894363475485700145</t>
-  </si>
-  <si>
-    <t>FR5623185484465641685100</t>
-  </si>
-  <si>
-    <t>AT8365645150865168448896</t>
-  </si>
-  <si>
-    <t>ES3251651681961210656510</t>
-  </si>
-  <si>
-    <t>ES4420960043013468900000</t>
-  </si>
-  <si>
-    <t>ES7225187786311225455548</t>
-  </si>
-  <si>
-    <t>FI5024587946032003165464</t>
+    <t>32145464138452163421</t>
+  </si>
+  <si>
+    <t>X9924125M</t>
   </si>
 </sst>
 </file>
@@ -2201,7 +2195,7 @@
   <dimension ref="A1:M106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,9 +2281,7 @@
       <c r="K2" t="s">
         <v>84</v>
       </c>
-      <c r="L2" t="s">
-        <v>489</v>
-      </c>
+      <c r="L2"/>
       <c r="M2" t="s">
         <v>53</v>
       </c>
@@ -2320,7 +2312,7 @@
         <v>70</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>485</v>
+        <v>580</v>
       </c>
       <c r="K3" t="s">
         <v>84</v>
@@ -2356,13 +2348,13 @@
         <v>132</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="K4" t="s">
         <v>89</v>
       </c>
       <c r="L4" t="s">
-        <v>490</v>
+        <v>568</v>
       </c>
       <c r="M4" t="s">
         <v>53</v>
@@ -2400,7 +2392,7 @@
         <v>84</v>
       </c>
       <c r="L5" t="s">
-        <v>488</v>
+        <v>572</v>
       </c>
       <c r="M5" t="s">
         <v>53</v>
@@ -2438,7 +2430,7 @@
         <v>368</v>
       </c>
       <c r="L6" t="s">
-        <v>491</v>
+        <v>573</v>
       </c>
       <c r="M6" t="s">
         <v>53</v>
@@ -2476,7 +2468,7 @@
         <v>85</v>
       </c>
       <c r="L7" t="s">
-        <v>492</v>
+        <v>574</v>
       </c>
       <c r="M7" t="s">
         <v>20</v>
@@ -2514,7 +2506,7 @@
         <v>361</v>
       </c>
       <c r="L8" t="s">
-        <v>531</v>
+        <v>567</v>
       </c>
       <c r="M8" t="s">
         <v>20</v>
@@ -2556,7 +2548,7 @@
         <v>86</v>
       </c>
       <c r="L10" t="s">
-        <v>550</v>
+        <v>575</v>
       </c>
       <c r="M10" t="s">
         <v>53</v>
@@ -2594,7 +2586,7 @@
         <v>84</v>
       </c>
       <c r="L11" t="s">
-        <v>560</v>
+        <v>576</v>
       </c>
       <c r="M11" t="s">
         <v>53</v>
@@ -2632,7 +2624,7 @@
         <v>88</v>
       </c>
       <c r="L12" t="s">
-        <v>563</v>
+        <v>577</v>
       </c>
       <c r="M12" t="s">
         <v>53</v>
@@ -2706,7 +2698,7 @@
         <v>365</v>
       </c>
       <c r="L14" t="s">
-        <v>569</v>
+        <v>578</v>
       </c>
       <c r="M14" t="s">
         <v>20</v>
@@ -2744,7 +2736,7 @@
         <v>371</v>
       </c>
       <c r="L15" t="s">
-        <v>570</v>
+        <v>579</v>
       </c>
       <c r="M15" t="s">
         <v>53</v>
@@ -2779,7 +2771,7 @@
         <v>87</v>
       </c>
       <c r="L16" t="s">
-        <v>522</v>
+        <v>571</v>
       </c>
       <c r="M16" t="s">
         <v>20</v>
@@ -2853,7 +2845,7 @@
         <v>370</v>
       </c>
       <c r="L18" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="M18" t="s">
         <v>20</v>
@@ -2891,7 +2883,7 @@
         <v>84</v>
       </c>
       <c r="L19" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="M19" t="s">
         <v>53</v>
@@ -2929,7 +2921,7 @@
         <v>362</v>
       </c>
       <c r="L20" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="M20" t="s">
         <v>20</v>
@@ -2967,7 +2959,7 @@
         <v>364</v>
       </c>
       <c r="L21" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="M21" t="s">
         <v>53</v>
@@ -3005,7 +2997,7 @@
         <v>84</v>
       </c>
       <c r="L22" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="M22" t="s">
         <v>53</v>
@@ -3040,7 +3032,7 @@
         <v>89</v>
       </c>
       <c r="L23" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="M23" t="s">
         <v>20</v>
@@ -3078,7 +3070,7 @@
         <v>84</v>
       </c>
       <c r="L24" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="M24" t="s">
         <v>20</v>
@@ -3113,7 +3105,7 @@
         <v>86</v>
       </c>
       <c r="L25" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="M25" t="s">
         <v>20</v>
@@ -3151,7 +3143,7 @@
         <v>84</v>
       </c>
       <c r="L26" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="M26" t="s">
         <v>53</v>
@@ -3189,7 +3181,7 @@
         <v>85</v>
       </c>
       <c r="L27" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="M27" t="s">
         <v>53</v>
@@ -3231,7 +3223,7 @@
         <v>84</v>
       </c>
       <c r="L29" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="M29" t="s">
         <v>53</v>
@@ -3269,7 +3261,7 @@
         <v>84</v>
       </c>
       <c r="L30" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="M30" t="s">
         <v>20</v>
@@ -3307,7 +3299,7 @@
         <v>374</v>
       </c>
       <c r="L31" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="M31" t="s">
         <v>53</v>
@@ -3345,7 +3337,7 @@
         <v>84</v>
       </c>
       <c r="L32" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="M32" t="s">
         <v>20</v>
@@ -3383,7 +3375,7 @@
         <v>84</v>
       </c>
       <c r="L33" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="M33" t="s">
         <v>20</v>
@@ -3421,7 +3413,7 @@
         <v>372</v>
       </c>
       <c r="L34" t="s">
-        <v>578</v>
+        <v>561</v>
       </c>
       <c r="M34" t="s">
         <v>20</v>
@@ -3459,7 +3451,7 @@
         <v>84</v>
       </c>
       <c r="L35" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="M35" t="s">
         <v>53</v>
@@ -3497,7 +3489,7 @@
         <v>367</v>
       </c>
       <c r="L36" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="M36" t="s">
         <v>53</v>
@@ -3535,7 +3527,7 @@
         <v>362</v>
       </c>
       <c r="L37" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="M37" t="s">
         <v>53</v>
@@ -3573,7 +3565,7 @@
         <v>85</v>
       </c>
       <c r="L38" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="M38" t="s">
         <v>53</v>
@@ -3611,7 +3603,7 @@
         <v>85</v>
       </c>
       <c r="L39" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="M39" t="s">
         <v>20</v>
@@ -3649,7 +3641,7 @@
         <v>84</v>
       </c>
       <c r="L40" t="s">
-        <v>582</v>
+        <v>565</v>
       </c>
       <c r="M40" t="s">
         <v>53</v>
@@ -3687,7 +3679,7 @@
         <v>84</v>
       </c>
       <c r="L41" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="M41" t="s">
         <v>53</v>
@@ -3725,7 +3717,7 @@
         <v>84</v>
       </c>
       <c r="L42" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="M42" t="s">
         <v>53</v>
@@ -3763,7 +3755,7 @@
         <v>84</v>
       </c>
       <c r="L43" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="M43" t="s">
         <v>53</v>
@@ -3801,7 +3793,7 @@
         <v>88</v>
       </c>
       <c r="L44" t="s">
-        <v>583</v>
+        <v>566</v>
       </c>
       <c r="M44" t="s">
         <v>53</v>
@@ -3839,7 +3831,7 @@
         <v>84</v>
       </c>
       <c r="L45" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="M45" t="s">
         <v>53</v>
@@ -3877,7 +3869,7 @@
         <v>84</v>
       </c>
       <c r="L46" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="M46" t="s">
         <v>53</v>
@@ -3915,7 +3907,7 @@
         <v>84</v>
       </c>
       <c r="L47" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="M47" t="s">
         <v>53</v>
@@ -3953,7 +3945,7 @@
         <v>84</v>
       </c>
       <c r="L48" t="s">
-        <v>580</v>
+        <v>563</v>
       </c>
       <c r="M48" t="s">
         <v>53</v>
@@ -3991,7 +3983,7 @@
         <v>84</v>
       </c>
       <c r="L49" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
       <c r="M49" t="s">
         <v>20</v>
@@ -4026,7 +4018,7 @@
         <v>90</v>
       </c>
       <c r="L50" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="M50" t="s">
         <v>20</v>
@@ -4061,7 +4053,7 @@
         <v>85</v>
       </c>
       <c r="L51" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="M51" t="s">
         <v>20</v>
@@ -4099,7 +4091,7 @@
         <v>85</v>
       </c>
       <c r="L52" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="M52" t="s">
         <v>53</v>
@@ -4137,7 +4129,7 @@
         <v>84</v>
       </c>
       <c r="L53" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="M53" t="s">
         <v>20</v>
@@ -4175,7 +4167,7 @@
         <v>370</v>
       </c>
       <c r="L54" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="M54" t="s">
         <v>20</v>
@@ -4213,7 +4205,7 @@
         <v>84</v>
       </c>
       <c r="L55" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="M55" t="s">
         <v>20</v>
@@ -4251,7 +4243,7 @@
         <v>86</v>
       </c>
       <c r="L56" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="M56" t="s">
         <v>20</v>
@@ -4289,7 +4281,7 @@
         <v>90</v>
       </c>
       <c r="L57" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="M57" t="s">
         <v>53</v>
@@ -4327,7 +4319,7 @@
         <v>84</v>
       </c>
       <c r="L58" t="s">
-        <v>562</v>
+        <v>550</v>
       </c>
       <c r="M58" t="s">
         <v>20</v>
@@ -4369,7 +4361,7 @@
         <v>84</v>
       </c>
       <c r="L60" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="M60" t="s">
         <v>20</v>
@@ -4407,7 +4399,7 @@
         <v>84</v>
       </c>
       <c r="L61" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="M61" t="s">
         <v>53</v>
@@ -4445,7 +4437,7 @@
         <v>84</v>
       </c>
       <c r="L62" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="M62" t="s">
         <v>20</v>
@@ -4483,7 +4475,7 @@
         <v>90</v>
       </c>
       <c r="L63" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="M63" t="s">
         <v>53</v>
@@ -4521,7 +4513,7 @@
         <v>84</v>
       </c>
       <c r="L64" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="M64" t="s">
         <v>20</v>
@@ -4559,7 +4551,7 @@
         <v>84</v>
       </c>
       <c r="L65" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="M65" t="s">
         <v>53</v>
@@ -4597,7 +4589,7 @@
         <v>84</v>
       </c>
       <c r="L66" t="s">
-        <v>565</v>
+        <v>552</v>
       </c>
       <c r="M66" t="s">
         <v>20</v>
@@ -4635,7 +4627,7 @@
         <v>84</v>
       </c>
       <c r="L67" t="s">
-        <v>571</v>
+        <v>555</v>
       </c>
       <c r="M67" t="s">
         <v>20</v>
@@ -4673,7 +4665,7 @@
         <v>84</v>
       </c>
       <c r="L68" t="s">
-        <v>559</v>
+        <v>548</v>
       </c>
       <c r="M68" t="s">
         <v>20</v>
@@ -4711,7 +4703,7 @@
         <v>84</v>
       </c>
       <c r="L69" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="M69" t="s">
         <v>53</v>
@@ -4749,7 +4741,7 @@
         <v>84</v>
       </c>
       <c r="L70" t="s">
-        <v>561</v>
+        <v>549</v>
       </c>
       <c r="M70" t="s">
         <v>20</v>
@@ -4787,7 +4779,7 @@
         <v>84</v>
       </c>
       <c r="L71" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="M71" t="s">
         <v>20</v>
@@ -4825,7 +4817,7 @@
         <v>84</v>
       </c>
       <c r="L72" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="M72" t="s">
         <v>20</v>
@@ -4863,7 +4855,7 @@
         <v>84</v>
       </c>
       <c r="L73" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="M73" t="s">
         <v>20</v>
@@ -4901,7 +4893,7 @@
         <v>374</v>
       </c>
       <c r="L74" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
       <c r="M74" t="s">
         <v>53</v>
@@ -4939,7 +4931,7 @@
         <v>84</v>
       </c>
       <c r="L75" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="M75" t="s">
         <v>53</v>
@@ -4977,7 +4969,7 @@
         <v>84</v>
       </c>
       <c r="L76" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="M76" t="s">
         <v>20</v>
@@ -5015,7 +5007,7 @@
         <v>84</v>
       </c>
       <c r="L77" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="M77" t="s">
         <v>20</v>
@@ -5053,7 +5045,7 @@
         <v>366</v>
       </c>
       <c r="L78" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="M78" t="s">
         <v>53</v>
@@ -5093,7 +5085,7 @@
         <v>84</v>
       </c>
       <c r="L80" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="M80" t="s">
         <v>20</v>
@@ -5131,7 +5123,7 @@
         <v>84</v>
       </c>
       <c r="L81" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="M81" t="s">
         <v>53</v>
@@ -5169,7 +5161,7 @@
         <v>84</v>
       </c>
       <c r="L82" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="M82" t="s">
         <v>53</v>
@@ -5207,7 +5199,7 @@
         <v>88</v>
       </c>
       <c r="L83" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="M83" t="s">
         <v>20</v>
@@ -5245,7 +5237,7 @@
         <v>84</v>
       </c>
       <c r="L84" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="M84" t="s">
         <v>53</v>
@@ -5280,7 +5272,7 @@
         <v>372</v>
       </c>
       <c r="L85" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="M85" t="s">
         <v>20</v>
@@ -5318,7 +5310,7 @@
         <v>84</v>
       </c>
       <c r="L86" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="M86" t="s">
         <v>20</v>
@@ -5356,7 +5348,7 @@
         <v>84</v>
       </c>
       <c r="L87" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="M87" t="s">
         <v>53</v>
@@ -5394,7 +5386,7 @@
         <v>84</v>
       </c>
       <c r="L88" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="M88" t="s">
         <v>53</v>
@@ -5432,7 +5424,7 @@
         <v>365</v>
       </c>
       <c r="L89" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="M89" t="s">
         <v>20</v>
@@ -5470,7 +5462,7 @@
         <v>84</v>
       </c>
       <c r="L90" t="s">
-        <v>551</v>
+        <v>540</v>
       </c>
       <c r="M90" t="s">
         <v>20</v>
@@ -5508,7 +5500,7 @@
         <v>84</v>
       </c>
       <c r="L91" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="M91" t="s">
         <v>20</v>
@@ -5546,7 +5538,7 @@
         <v>370</v>
       </c>
       <c r="L92" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="M92" t="s">
         <v>20</v>
@@ -5584,7 +5576,7 @@
         <v>369</v>
       </c>
       <c r="L93" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="M93" t="s">
         <v>53</v>
@@ -5622,7 +5614,7 @@
         <v>84</v>
       </c>
       <c r="L94" t="s">
-        <v>581</v>
+        <v>564</v>
       </c>
       <c r="M94" t="s">
         <v>20</v>
@@ -5660,7 +5652,7 @@
         <v>84</v>
       </c>
       <c r="L95" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="M95" t="s">
         <v>20</v>
@@ -5698,7 +5690,7 @@
         <v>362</v>
       </c>
       <c r="L96" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="M96" t="s">
         <v>20</v>
@@ -5736,7 +5728,7 @@
         <v>84</v>
       </c>
       <c r="L97" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="M97" t="s">
         <v>20</v>
@@ -5774,7 +5766,7 @@
         <v>84</v>
       </c>
       <c r="L98" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="M98" t="s">
         <v>20</v>
@@ -5812,7 +5804,7 @@
         <v>84</v>
       </c>
       <c r="L99" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="M99" t="s">
         <v>20</v>
@@ -5854,7 +5846,7 @@
         <v>363</v>
       </c>
       <c r="L101" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="M101" t="s">
         <v>20</v>
@@ -5892,7 +5884,7 @@
         <v>89</v>
       </c>
       <c r="L102" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="M102" t="s">
         <v>20</v>
@@ -5930,7 +5922,7 @@
         <v>365</v>
       </c>
       <c r="L103" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="M103" t="s">
         <v>20</v>
@@ -5968,7 +5960,7 @@
         <v>362</v>
       </c>
       <c r="L104" t="s">
-        <v>579</v>
+        <v>562</v>
       </c>
       <c r="M104" t="s">
         <v>20</v>
@@ -6006,7 +5998,7 @@
         <v>364</v>
       </c>
       <c r="L105" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="M105" t="s">
         <v>20</v>
@@ -6044,7 +6036,7 @@
         <v>373</v>
       </c>
       <c r="L106" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="M106" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Finalizacion de la practica 3 -> Faltan cargar los valores de las otras hojas
</commit_message>
<xml_diff>
--- a/SIS2-2020/resources/SistemasInformacionII.xlsx
+++ b/SIS2-2020/resources/SistemasInformacionII.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="684">
   <si>
     <t>Nombre</t>
   </si>
@@ -1775,6 +1775,312 @@
   </si>
   <si>
     <t>X9924125M</t>
+  </si>
+  <si>
+    <t>am00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>aam00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>aab00@asoftware.es</t>
+  </si>
+  <si>
+    <t>acd00@asoftware.es</t>
+  </si>
+  <si>
+    <t>abg00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>agm00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>ari00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>amg00@asoftware.es</t>
+  </si>
+  <si>
+    <t>afr00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>ala00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>ala01@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>agr00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>ads00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>bv00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>bbv00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>bba00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>bam00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>bca00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>bbl00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>bga00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>bl00@asoftware.es</t>
+  </si>
+  <si>
+    <t>bbl00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>bs00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>bga00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>bgd00@asoftware.es</t>
+  </si>
+  <si>
+    <t>cim00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>cqc00@asoftware.es</t>
+  </si>
+  <si>
+    <t>cvm00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>cpf00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>cci00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>cfs00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>cje00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>cgg00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>cpe00@asoftware.es</t>
+  </si>
+  <si>
+    <t>csm00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>clm00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>ccj00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>cpj00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>ccb00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>can00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>ccm00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>dam00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>dfc00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>dlc00@asoftware.es</t>
+  </si>
+  <si>
+    <t>eah00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>ek00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>es00@asoftware.es</t>
+  </si>
+  <si>
+    <t>fpb00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>faa00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>ffi00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>ffd00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>fme00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>flc00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>gar00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>gpl00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>gge00@asoftware.es</t>
+  </si>
+  <si>
+    <t>gpl00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>gfd00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>gsa00@asoftware.es</t>
+  </si>
+  <si>
+    <t>gif00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>gac00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>gra00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>gmn00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>glj00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>hdd00@asoftware.es</t>
+  </si>
+  <si>
+    <t>ldr00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>lrf00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>mcn00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>mbo00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>mfj00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>mgj00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>moh00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>mvp00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>mmc00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>mbm00@tecnoproyectsl.es</t>
+  </si>
+  <si>
+    <t>nbb00@asoftware.es</t>
+  </si>
+  <si>
+    <t>osp00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>odp00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>ofj00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>pdc00@asoftware.es</t>
+  </si>
+  <si>
+    <t>pgc00@asoftware.es</t>
+  </si>
+  <si>
+    <t>ppv00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>pac00@asoftware.es</t>
+  </si>
+  <si>
+    <t>pma00@asoftware.es</t>
+  </si>
+  <si>
+    <t>pgr00@pblanksa.es</t>
+  </si>
+  <si>
+    <t>rfi00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>raf00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>rdf00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>rgt00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>rlc00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>sbc00@asoftware.es</t>
+  </si>
+  <si>
+    <t>sas00@asoftware.es</t>
+  </si>
+  <si>
+    <t>she00@asoftware.es</t>
+  </si>
+  <si>
+    <t>sld00@asoftware.es</t>
+  </si>
+  <si>
+    <t>sfh00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>sgs00@aphonsa.es</t>
+  </si>
+  <si>
+    <t>ssg00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>sss00@tecnoleonsl.es</t>
+  </si>
+  <si>
+    <t>ES3520960043043554600000</t>
+  </si>
+  <si>
+    <t>ES7832145464138452163421</t>
+  </si>
+  <si>
+    <t>ES7921564975243245467995</t>
+  </si>
+  <si>
+    <t>ES0721584976902154655487</t>
   </si>
 </sst>
 </file>
@@ -2275,13 +2581,18 @@
       <c r="H2" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="I2" t="s">
+        <v>582</v>
+      </c>
       <c r="J2" s="5" t="s">
         <v>79</v>
       </c>
       <c r="K2" t="s">
         <v>84</v>
       </c>
-      <c r="L2"/>
+      <c r="L2" t="s">
+        <v>680</v>
+      </c>
       <c r="M2" t="s">
         <v>53</v>
       </c>
@@ -2311,13 +2622,18 @@
       <c r="H3" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="I3" t="s">
+        <v>583</v>
+      </c>
       <c r="J3" s="5" t="s">
         <v>580</v>
       </c>
       <c r="K3" t="s">
         <v>84</v>
       </c>
-      <c r="L3"/>
+      <c r="L3" t="s">
+        <v>681</v>
+      </c>
       <c r="M3" t="s">
         <v>53</v>
       </c>
@@ -2347,6 +2663,9 @@
       <c r="H4" s="2" t="s">
         <v>132</v>
       </c>
+      <c r="I4" t="s">
+        <v>584</v>
+      </c>
       <c r="J4" s="5" t="s">
         <v>484</v>
       </c>
@@ -2385,6 +2704,9 @@
       <c r="H5" s="2" t="s">
         <v>189</v>
       </c>
+      <c r="I5" t="s">
+        <v>585</v>
+      </c>
       <c r="J5" s="7" t="s">
         <v>382</v>
       </c>
@@ -2423,6 +2745,9 @@
       <c r="H6" s="2" t="s">
         <v>238</v>
       </c>
+      <c r="I6" t="s">
+        <v>586</v>
+      </c>
       <c r="J6" s="5" t="s">
         <v>383</v>
       </c>
@@ -2461,6 +2786,9 @@
       <c r="H7" s="2" t="s">
         <v>355</v>
       </c>
+      <c r="I7" t="s">
+        <v>587</v>
+      </c>
       <c r="J7" s="5" t="s">
         <v>384</v>
       </c>
@@ -2499,6 +2827,9 @@
       <c r="H8" s="2" t="s">
         <v>250</v>
       </c>
+      <c r="I8" t="s">
+        <v>588</v>
+      </c>
       <c r="J8" s="5" t="s">
         <v>385</v>
       </c>
@@ -2541,6 +2872,9 @@
       <c r="H10" s="2" t="s">
         <v>167</v>
       </c>
+      <c r="I10" t="s">
+        <v>589</v>
+      </c>
       <c r="J10" s="5" t="s">
         <v>386</v>
       </c>
@@ -2579,6 +2913,9 @@
       <c r="H11" s="2" t="s">
         <v>279</v>
       </c>
+      <c r="I11" t="s">
+        <v>590</v>
+      </c>
       <c r="J11" s="5" t="s">
         <v>387</v>
       </c>
@@ -2617,6 +2954,9 @@
       <c r="H12" s="3" t="s">
         <v>388</v>
       </c>
+      <c r="I12" t="s">
+        <v>591</v>
+      </c>
       <c r="J12" s="5" t="s">
         <v>79</v>
       </c>
@@ -2655,13 +2995,18 @@
       <c r="H13" s="2" t="s">
         <v>388</v>
       </c>
+      <c r="I13" t="s">
+        <v>592</v>
+      </c>
       <c r="J13" s="5" t="s">
         <v>389</v>
       </c>
       <c r="K13" t="s">
         <v>84</v>
       </c>
-      <c r="L13"/>
+      <c r="L13" t="s">
+        <v>682</v>
+      </c>
       <c r="M13" t="s">
         <v>53</v>
       </c>
@@ -2691,6 +3036,9 @@
       <c r="H14" s="2" t="s">
         <v>286</v>
       </c>
+      <c r="I14" t="s">
+        <v>593</v>
+      </c>
       <c r="J14" s="5" t="s">
         <v>390</v>
       </c>
@@ -2729,6 +3077,9 @@
       <c r="H15" s="2" t="s">
         <v>267</v>
       </c>
+      <c r="I15" t="s">
+        <v>594</v>
+      </c>
       <c r="J15" s="5" t="s">
         <v>391</v>
       </c>
@@ -2764,6 +3115,9 @@
       <c r="H16" s="3" t="s">
         <v>359</v>
       </c>
+      <c r="I16" t="s">
+        <v>595</v>
+      </c>
       <c r="J16" s="5" t="s">
         <v>392</v>
       </c>
@@ -2802,13 +3156,18 @@
       <c r="H17" s="2" t="s">
         <v>359</v>
       </c>
+      <c r="I17" t="s">
+        <v>596</v>
+      </c>
       <c r="J17" s="5" t="s">
         <v>393</v>
       </c>
       <c r="K17" t="s">
         <v>84</v>
       </c>
-      <c r="L17"/>
+      <c r="L17" t="s">
+        <v>683</v>
+      </c>
       <c r="M17" t="s">
         <v>20</v>
       </c>
@@ -2838,6 +3197,9 @@
       <c r="H18" s="2" t="s">
         <v>330</v>
       </c>
+      <c r="I18" t="s">
+        <v>597</v>
+      </c>
       <c r="J18" s="5" t="s">
         <v>394</v>
       </c>
@@ -2876,6 +3238,9 @@
       <c r="H19" s="2" t="s">
         <v>317</v>
       </c>
+      <c r="I19" t="s">
+        <v>598</v>
+      </c>
       <c r="J19" s="5" t="s">
         <v>395</v>
       </c>
@@ -2914,6 +3279,9 @@
       <c r="H20" s="2" t="s">
         <v>327</v>
       </c>
+      <c r="I20" t="s">
+        <v>599</v>
+      </c>
       <c r="J20" s="5" t="s">
         <v>396</v>
       </c>
@@ -2952,6 +3320,9 @@
       <c r="H21" s="2" t="s">
         <v>313</v>
       </c>
+      <c r="I21" t="s">
+        <v>600</v>
+      </c>
       <c r="J21" s="5" t="s">
         <v>397</v>
       </c>
@@ -2990,6 +3361,9 @@
       <c r="H22" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="I22" t="s">
+        <v>601</v>
+      </c>
       <c r="J22" s="5" t="s">
         <v>398</v>
       </c>
@@ -3025,6 +3399,9 @@
       <c r="H23" s="3" t="s">
         <v>399</v>
       </c>
+      <c r="I23" t="s">
+        <v>602</v>
+      </c>
       <c r="J23" s="5" t="s">
         <v>392</v>
       </c>
@@ -3063,6 +3440,9 @@
       <c r="H24" s="2" t="s">
         <v>399</v>
       </c>
+      <c r="I24" t="s">
+        <v>603</v>
+      </c>
       <c r="J24" s="5" t="s">
         <v>400</v>
       </c>
@@ -3098,6 +3478,9 @@
       <c r="H25" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="I25" t="s">
+        <v>604</v>
+      </c>
       <c r="J25" s="5" t="s">
         <v>80</v>
       </c>
@@ -3136,6 +3519,9 @@
       <c r="H26" s="3" t="s">
         <v>401</v>
       </c>
+      <c r="I26" t="s">
+        <v>605</v>
+      </c>
       <c r="J26" s="5" t="s">
         <v>402</v>
       </c>
@@ -3174,6 +3560,9 @@
       <c r="H27" s="2" t="s">
         <v>198</v>
       </c>
+      <c r="I27" t="s">
+        <v>606</v>
+      </c>
       <c r="J27" s="5" t="s">
         <v>403</v>
       </c>
@@ -3216,6 +3605,9 @@
       <c r="H29" s="2" t="s">
         <v>300</v>
       </c>
+      <c r="I29" t="s">
+        <v>607</v>
+      </c>
       <c r="J29" s="5" t="s">
         <v>404</v>
       </c>
@@ -3254,6 +3646,9 @@
       <c r="H30" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="I30" t="s">
+        <v>608</v>
+      </c>
       <c r="J30" s="5" t="s">
         <v>405</v>
       </c>
@@ -3292,6 +3687,9 @@
       <c r="H31" s="2" t="s">
         <v>321</v>
       </c>
+      <c r="I31" t="s">
+        <v>609</v>
+      </c>
       <c r="J31" s="5" t="s">
         <v>406</v>
       </c>
@@ -3330,6 +3728,9 @@
       <c r="H32" s="2" t="s">
         <v>325</v>
       </c>
+      <c r="I32" t="s">
+        <v>610</v>
+      </c>
       <c r="J32" s="5" t="s">
         <v>407</v>
       </c>
@@ -3368,6 +3769,9 @@
       <c r="H33" s="2" t="s">
         <v>334</v>
       </c>
+      <c r="I33" t="s">
+        <v>611</v>
+      </c>
       <c r="J33" s="5" t="s">
         <v>408</v>
       </c>
@@ -3406,6 +3810,9 @@
       <c r="H34" s="2" t="s">
         <v>270</v>
       </c>
+      <c r="I34" t="s">
+        <v>612</v>
+      </c>
       <c r="J34" s="5" t="s">
         <v>409</v>
       </c>
@@ -3444,6 +3851,9 @@
       <c r="H35" s="2" t="s">
         <v>217</v>
       </c>
+      <c r="I35" t="s">
+        <v>613</v>
+      </c>
       <c r="J35" s="5" t="s">
         <v>410</v>
       </c>
@@ -3482,6 +3892,9 @@
       <c r="H36" s="2" t="s">
         <v>235</v>
       </c>
+      <c r="I36" t="s">
+        <v>614</v>
+      </c>
       <c r="J36" s="5" t="s">
         <v>411</v>
       </c>
@@ -3520,6 +3933,9 @@
       <c r="H37" s="2" t="s">
         <v>210</v>
       </c>
+      <c r="I37" t="s">
+        <v>615</v>
+      </c>
       <c r="J37" s="5" t="s">
         <v>412</v>
       </c>
@@ -3558,6 +3974,9 @@
       <c r="H38" s="2" t="s">
         <v>350</v>
       </c>
+      <c r="I38" t="s">
+        <v>616</v>
+      </c>
       <c r="J38" s="5" t="s">
         <v>413</v>
       </c>
@@ -3596,6 +4015,9 @@
       <c r="H39" s="2" t="s">
         <v>414</v>
       </c>
+      <c r="I39" t="s">
+        <v>617</v>
+      </c>
       <c r="J39" s="5" t="s">
         <v>415</v>
       </c>
@@ -3634,6 +4056,9 @@
       <c r="H40" s="2" t="s">
         <v>337</v>
       </c>
+      <c r="I40" t="s">
+        <v>618</v>
+      </c>
       <c r="J40" s="5" t="s">
         <v>416</v>
       </c>
@@ -3672,6 +4097,9 @@
       <c r="H41" s="2" t="s">
         <v>341</v>
       </c>
+      <c r="I41" t="s">
+        <v>619</v>
+      </c>
       <c r="J41" s="5" t="s">
         <v>417</v>
       </c>
@@ -3710,6 +4138,9 @@
       <c r="H42" s="2" t="s">
         <v>125</v>
       </c>
+      <c r="I42" t="s">
+        <v>620</v>
+      </c>
       <c r="J42" s="5" t="s">
         <v>418</v>
       </c>
@@ -3748,6 +4179,9 @@
       <c r="H43" s="2" t="s">
         <v>344</v>
       </c>
+      <c r="I43" t="s">
+        <v>621</v>
+      </c>
       <c r="J43" s="5" t="s">
         <v>419</v>
       </c>
@@ -3786,6 +4220,9 @@
       <c r="H44" s="2" t="s">
         <v>348</v>
       </c>
+      <c r="I44" t="s">
+        <v>622</v>
+      </c>
       <c r="J44" s="5" t="s">
         <v>420</v>
       </c>
@@ -3824,6 +4261,9 @@
       <c r="H45" s="3" t="s">
         <v>421</v>
       </c>
+      <c r="I45" t="s">
+        <v>622</v>
+      </c>
       <c r="J45" s="5" t="s">
         <v>422</v>
       </c>
@@ -3862,6 +4302,9 @@
       <c r="H46" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="I46" t="s">
+        <v>623</v>
+      </c>
       <c r="J46" s="5" t="s">
         <v>423</v>
       </c>
@@ -3900,6 +4343,9 @@
       <c r="H47" s="2" t="s">
         <v>181</v>
       </c>
+      <c r="I47" t="s">
+        <v>624</v>
+      </c>
       <c r="J47" s="5" t="s">
         <v>424</v>
       </c>
@@ -3938,6 +4384,9 @@
       <c r="H48" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="I48" t="s">
+        <v>625</v>
+      </c>
       <c r="J48" s="5" t="s">
         <v>425</v>
       </c>
@@ -3976,6 +4425,9 @@
       <c r="H49" s="2" t="s">
         <v>246</v>
       </c>
+      <c r="I49" t="s">
+        <v>626</v>
+      </c>
       <c r="J49" s="5" t="s">
         <v>426</v>
       </c>
@@ -4011,6 +4463,9 @@
       <c r="H50" s="3" t="s">
         <v>427</v>
       </c>
+      <c r="I50" t="s">
+        <v>627</v>
+      </c>
       <c r="J50" s="5" t="s">
         <v>80</v>
       </c>
@@ -4046,6 +4501,9 @@
       <c r="H51" s="3" t="s">
         <v>428</v>
       </c>
+      <c r="I51" t="s">
+        <v>628</v>
+      </c>
       <c r="J51" s="5" t="s">
         <v>429</v>
       </c>
@@ -4084,6 +4542,9 @@
       <c r="H52" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="I52" t="s">
+        <v>629</v>
+      </c>
       <c r="J52" s="5" t="s">
         <v>430</v>
       </c>
@@ -4122,6 +4583,9 @@
       <c r="H53" s="3" t="s">
         <v>431</v>
       </c>
+      <c r="I53" t="s">
+        <v>630</v>
+      </c>
       <c r="J53" s="5" t="s">
         <v>432</v>
       </c>
@@ -4160,6 +4624,9 @@
       <c r="H54" s="2" t="s">
         <v>248</v>
       </c>
+      <c r="I54" t="s">
+        <v>631</v>
+      </c>
       <c r="J54" s="5" t="s">
         <v>433</v>
       </c>
@@ -4198,6 +4665,9 @@
       <c r="H55" s="2" t="s">
         <v>192</v>
       </c>
+      <c r="I55" t="s">
+        <v>632</v>
+      </c>
       <c r="J55" s="5" t="s">
         <v>434</v>
       </c>
@@ -4236,6 +4706,9 @@
       <c r="H56" s="2" t="s">
         <v>207</v>
       </c>
+      <c r="I56" t="s">
+        <v>633</v>
+      </c>
       <c r="J56" s="5" t="s">
         <v>435</v>
       </c>
@@ -4274,6 +4747,9 @@
       <c r="H57" s="2" t="s">
         <v>169</v>
       </c>
+      <c r="I57" t="s">
+        <v>634</v>
+      </c>
       <c r="J57" s="5" t="s">
         <v>436</v>
       </c>
@@ -4312,6 +4788,9 @@
       <c r="H58" s="2" t="s">
         <v>277</v>
       </c>
+      <c r="I58" t="s">
+        <v>635</v>
+      </c>
       <c r="J58" s="5" t="s">
         <v>437</v>
       </c>
@@ -4354,6 +4833,9 @@
       <c r="H60" s="3" t="s">
         <v>438</v>
       </c>
+      <c r="I60" t="s">
+        <v>636</v>
+      </c>
       <c r="J60" s="5" t="s">
         <v>78</v>
       </c>
@@ -4392,6 +4874,9 @@
       <c r="H61" s="2" t="s">
         <v>194</v>
       </c>
+      <c r="I61" t="s">
+        <v>637</v>
+      </c>
       <c r="J61" s="5" t="s">
         <v>439</v>
       </c>
@@ -4430,6 +4915,9 @@
       <c r="H62" s="3" t="s">
         <v>69</v>
       </c>
+      <c r="I62" t="s">
+        <v>638</v>
+      </c>
       <c r="J62" s="5" t="s">
         <v>440</v>
       </c>
@@ -4468,6 +4956,9 @@
       <c r="H63" s="2" t="s">
         <v>204</v>
       </c>
+      <c r="I63" t="s">
+        <v>639</v>
+      </c>
       <c r="J63" s="5" t="s">
         <v>441</v>
       </c>
@@ -4506,6 +4997,9 @@
       <c r="H64" s="2" t="s">
         <v>121</v>
       </c>
+      <c r="I64" t="s">
+        <v>640</v>
+      </c>
       <c r="J64" s="5" t="s">
         <v>442</v>
       </c>
@@ -4544,6 +5038,9 @@
       <c r="H65" s="2" t="s">
         <v>221</v>
       </c>
+      <c r="I65" t="s">
+        <v>641</v>
+      </c>
       <c r="J65" s="5" t="s">
         <v>443</v>
       </c>
@@ -4582,6 +5079,9 @@
       <c r="H66" s="2" t="s">
         <v>151</v>
       </c>
+      <c r="I66" t="s">
+        <v>642</v>
+      </c>
       <c r="J66" s="5" t="s">
         <v>444</v>
       </c>
@@ -4620,6 +5120,9 @@
       <c r="H67" s="2" t="s">
         <v>358</v>
       </c>
+      <c r="I67" t="s">
+        <v>643</v>
+      </c>
       <c r="J67" s="5" t="s">
         <v>445</v>
       </c>
@@ -4658,6 +5161,9 @@
       <c r="H68" s="3" t="s">
         <v>427</v>
       </c>
+      <c r="I68" t="s">
+        <v>638</v>
+      </c>
       <c r="J68" s="5" t="s">
         <v>77</v>
       </c>
@@ -4696,6 +5202,9 @@
       <c r="H69" s="2" t="s">
         <v>446</v>
       </c>
+      <c r="I69" t="s">
+        <v>644</v>
+      </c>
       <c r="J69" s="5" t="s">
         <v>447</v>
       </c>
@@ -4734,6 +5243,9 @@
       <c r="H70" s="2" t="s">
         <v>252</v>
       </c>
+      <c r="I70" t="s">
+        <v>645</v>
+      </c>
       <c r="J70" s="5" t="s">
         <v>448</v>
       </c>
@@ -4772,6 +5284,9 @@
       <c r="H71" s="2" t="s">
         <v>163</v>
       </c>
+      <c r="I71" t="s">
+        <v>646</v>
+      </c>
       <c r="J71" s="5" t="s">
         <v>449</v>
       </c>
@@ -4810,6 +5325,9 @@
       <c r="H72" s="2" t="s">
         <v>283</v>
       </c>
+      <c r="I72" t="s">
+        <v>647</v>
+      </c>
       <c r="J72" s="5" t="s">
         <v>450</v>
       </c>
@@ -4848,6 +5366,9 @@
       <c r="H73" s="3" t="s">
         <v>414</v>
       </c>
+      <c r="I73" t="s">
+        <v>648</v>
+      </c>
       <c r="J73" s="5" t="s">
         <v>440</v>
       </c>
@@ -4886,6 +5407,9 @@
       <c r="H74" s="2" t="s">
         <v>304</v>
       </c>
+      <c r="I74" t="s">
+        <v>649</v>
+      </c>
       <c r="J74" s="5" t="s">
         <v>451</v>
       </c>
@@ -4924,6 +5448,9 @@
       <c r="H75" s="2" t="s">
         <v>297</v>
       </c>
+      <c r="I75" t="s">
+        <v>650</v>
+      </c>
       <c r="J75" s="5" t="s">
         <v>452</v>
       </c>
@@ -4962,6 +5489,9 @@
       <c r="H76" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="I76" t="s">
+        <v>651</v>
+      </c>
       <c r="J76" s="5" t="s">
         <v>453</v>
       </c>
@@ -5000,6 +5530,9 @@
       <c r="H77" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="I77" t="s">
+        <v>652</v>
+      </c>
       <c r="J77" s="5" t="s">
         <v>454</v>
       </c>
@@ -5038,6 +5571,9 @@
       <c r="H78" s="2" t="s">
         <v>232</v>
       </c>
+      <c r="I78" t="s">
+        <v>653</v>
+      </c>
       <c r="J78" s="5" t="s">
         <v>455</v>
       </c>
@@ -5078,6 +5614,9 @@
         <v>37</v>
       </c>
       <c r="H80" s="3"/>
+      <c r="I80" t="s">
+        <v>654</v>
+      </c>
       <c r="J80" s="5" t="s">
         <v>481</v>
       </c>
@@ -5116,6 +5655,9 @@
       <c r="H81" s="2" t="s">
         <v>173</v>
       </c>
+      <c r="I81" t="s">
+        <v>655</v>
+      </c>
       <c r="J81" s="5" t="s">
         <v>456</v>
       </c>
@@ -5154,6 +5696,9 @@
       <c r="H82" s="2" t="s">
         <v>310</v>
       </c>
+      <c r="I82" t="s">
+        <v>656</v>
+      </c>
       <c r="J82" s="5" t="s">
         <v>480</v>
       </c>
@@ -5192,6 +5737,9 @@
       <c r="H83" s="2" t="s">
         <v>129</v>
       </c>
+      <c r="I83" t="s">
+        <v>657</v>
+      </c>
       <c r="J83" s="5" t="s">
         <v>457</v>
       </c>
@@ -5230,6 +5778,9 @@
       <c r="H84" s="2" t="s">
         <v>294</v>
       </c>
+      <c r="I84" t="s">
+        <v>658</v>
+      </c>
       <c r="J84" s="5" t="s">
         <v>458</v>
       </c>
@@ -5265,6 +5816,9 @@
       <c r="G85" t="s">
         <v>291</v>
       </c>
+      <c r="I85" t="s">
+        <v>659</v>
+      </c>
       <c r="J85" s="5" t="s">
         <v>478</v>
       </c>
@@ -5303,6 +5857,9 @@
       <c r="H86" s="2" t="s">
         <v>256</v>
       </c>
+      <c r="I86" t="s">
+        <v>660</v>
+      </c>
       <c r="J86" s="5" t="s">
         <v>459</v>
       </c>
@@ -5341,6 +5898,9 @@
       <c r="H87" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="I87" t="s">
+        <v>661</v>
+      </c>
       <c r="J87" s="5" t="s">
         <v>460</v>
       </c>
@@ -5379,6 +5939,9 @@
       <c r="H88" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="I88" t="s">
+        <v>662</v>
+      </c>
       <c r="J88" s="5" t="s">
         <v>461</v>
       </c>
@@ -5417,6 +5980,9 @@
       <c r="H89" s="2" t="s">
         <v>259</v>
       </c>
+      <c r="I89" t="s">
+        <v>663</v>
+      </c>
       <c r="J89" s="5" t="s">
         <v>462</v>
       </c>
@@ -5455,6 +6021,9 @@
       <c r="H90" s="2" t="s">
         <v>155</v>
       </c>
+      <c r="I90" t="s">
+        <v>664</v>
+      </c>
       <c r="J90" s="5" t="s">
         <v>463</v>
       </c>
@@ -5493,6 +6062,9 @@
       <c r="H91" s="2" t="s">
         <v>117</v>
       </c>
+      <c r="I91" t="s">
+        <v>665</v>
+      </c>
       <c r="J91" s="5" t="s">
         <v>464</v>
       </c>
@@ -5531,6 +6103,9 @@
       <c r="H92" s="2" t="s">
         <v>288</v>
       </c>
+      <c r="I92" t="s">
+        <v>666</v>
+      </c>
       <c r="J92" s="5" t="s">
         <v>465</v>
       </c>
@@ -5569,6 +6144,9 @@
       <c r="H93" s="2" t="s">
         <v>242</v>
       </c>
+      <c r="I93" t="s">
+        <v>667</v>
+      </c>
       <c r="J93" s="5" t="s">
         <v>466</v>
       </c>
@@ -5607,6 +6185,9 @@
       <c r="H94" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="I94" t="s">
+        <v>668</v>
+      </c>
       <c r="J94" s="5" t="s">
         <v>467</v>
       </c>
@@ -5645,6 +6226,9 @@
       <c r="H95" s="2" t="s">
         <v>468</v>
       </c>
+      <c r="I95" t="s">
+        <v>669</v>
+      </c>
       <c r="J95" s="5" t="s">
         <v>469</v>
       </c>
@@ -5683,6 +6267,9 @@
       <c r="H96" s="2" t="s">
         <v>470</v>
       </c>
+      <c r="I96" t="s">
+        <v>670</v>
+      </c>
       <c r="J96" s="5" t="s">
         <v>471</v>
       </c>
@@ -5721,6 +6308,9 @@
       <c r="H97" s="2" t="s">
         <v>177</v>
       </c>
+      <c r="I97" t="s">
+        <v>671</v>
+      </c>
       <c r="J97" s="5" t="s">
         <v>472</v>
       </c>
@@ -5759,6 +6349,9 @@
       <c r="H98" s="2" t="s">
         <v>159</v>
       </c>
+      <c r="I98" t="s">
+        <v>672</v>
+      </c>
       <c r="J98" s="5" t="s">
         <v>473</v>
       </c>
@@ -5797,6 +6390,9 @@
       <c r="H99" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="I99" t="s">
+        <v>673</v>
+      </c>
       <c r="J99" s="5" t="s">
         <v>474</v>
       </c>
@@ -5839,6 +6435,9 @@
       <c r="H101" s="2" t="s">
         <v>213</v>
       </c>
+      <c r="I101" t="s">
+        <v>674</v>
+      </c>
       <c r="J101" s="5" t="s">
         <v>477</v>
       </c>
@@ -5877,6 +6476,9 @@
       <c r="H102" s="2" t="s">
         <v>201</v>
       </c>
+      <c r="I102" t="s">
+        <v>675</v>
+      </c>
       <c r="J102" s="5" t="s">
         <v>475</v>
       </c>
@@ -5915,6 +6517,9 @@
       <c r="H103" s="2" t="s">
         <v>228</v>
       </c>
+      <c r="I103" t="s">
+        <v>676</v>
+      </c>
       <c r="J103" s="5" t="s">
         <v>482</v>
       </c>
@@ -5953,6 +6558,9 @@
       <c r="H104" s="2" t="s">
         <v>264</v>
       </c>
+      <c r="I104" t="s">
+        <v>677</v>
+      </c>
       <c r="J104" s="5" t="s">
         <v>483</v>
       </c>
@@ -5991,6 +6599,9 @@
       <c r="H105" s="2" t="s">
         <v>225</v>
       </c>
+      <c r="I105" t="s">
+        <v>678</v>
+      </c>
       <c r="J105" s="5" t="s">
         <v>479</v>
       </c>
@@ -6028,6 +6639,9 @@
       </c>
       <c r="H106" s="2" t="s">
         <v>273</v>
+      </c>
+      <c r="I106" t="s">
+        <v>679</v>
       </c>
       <c r="J106" s="5" t="s">
         <v>476</v>

</xml_diff>

<commit_message>
FIN DE LA PRACTICA 3 SHUHHHHHHHH
</commit_message>
<xml_diff>
--- a/SIS2-2020/resources/SistemasInformacionII.xlsx
+++ b/SIS2-2020/resources/SistemasInformacionII.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20357"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\NetBeansProjects\SIS2-2020\SIS2-2020\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\NetBeansProjects\Nominas2020\resources\original 2020\practica 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3551EBC0-E65F-461A-9382-184B17622728}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3860E0B4-8753-4E99-8361-EADC3FC2FC98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1380" windowWidth="15375" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2835" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="689">
   <si>
     <t>Nombre</t>
   </si>
@@ -265,6 +265,9 @@
     <t>20960031442124800000</t>
   </si>
   <si>
+    <t>20960056163231500000</t>
+  </si>
+  <si>
     <t>01826530120201560000</t>
   </si>
   <si>
@@ -493,9 +496,6 @@
     <t>Presa</t>
   </si>
   <si>
-    <t>Álvarez</t>
-  </si>
-  <si>
     <t>71425232C</t>
   </si>
   <si>
@@ -1114,6 +1114,24 @@
     <t>Latifa Epfouad Erre</t>
   </si>
   <si>
+    <t>51556584121251000254</t>
+  </si>
+  <si>
+    <t>26551681877651415636</t>
+  </si>
+  <si>
+    <t>62541122001110105611</t>
+  </si>
+  <si>
+    <t>65645150005168448896</t>
+  </si>
+  <si>
+    <t>20012541100023365233</t>
+  </si>
+  <si>
+    <t>23658965214585223202</t>
+  </si>
+  <si>
     <t>MC</t>
   </si>
   <si>
@@ -1177,6 +1195,12 @@
     <t>P2418823C</t>
   </si>
   <si>
+    <t>32145464138452163421</t>
+  </si>
+  <si>
+    <t>31645124473461205164</t>
+  </si>
+  <si>
     <t>65614874165615445616</t>
   </si>
   <si>
@@ -1462,321 +1486,324 @@
     <t>99558741836555551120</t>
   </si>
   <si>
+    <t>ES3520960043043554600000</t>
+  </si>
+  <si>
+    <t>ES7832145464138452163421</t>
+  </si>
+  <si>
+    <t>DK7331645124473461205164</t>
+  </si>
+  <si>
+    <t>ES8265614874165615445616</t>
+  </si>
+  <si>
+    <t>RO8832569523016220165156</t>
+  </si>
+  <si>
+    <t>DE7424561937521546497521</t>
+  </si>
+  <si>
+    <t>MC6436520125638451012515</t>
+  </si>
+  <si>
+    <t>GR9420125003305201112544</t>
+  </si>
+  <si>
+    <t>ES2821651484690980008984</t>
+  </si>
+  <si>
+    <t>FI5620960043043554600000</t>
+  </si>
+  <si>
+    <t>ES7921564975243245467995</t>
+  </si>
+  <si>
+    <t>LT8032566221522587754554</t>
+  </si>
+  <si>
+    <t>EE2023215465315456411515</t>
+  </si>
+  <si>
+    <t>BE9400750184310702510000</t>
+  </si>
+  <si>
+    <t>ES0721584976902154655487</t>
+  </si>
+  <si>
+    <t>SM2125894363475485700145</t>
+  </si>
+  <si>
+    <t>ES9596431245118150005156</t>
+  </si>
+  <si>
+    <t>AT6825030000114574745458</t>
+  </si>
+  <si>
+    <t>IT8915953684811254695203</t>
+  </si>
+  <si>
+    <t>ES9020960043023096200000</t>
+  </si>
+  <si>
+    <t>DK5800750184310702510000</t>
+  </si>
+  <si>
+    <t>ES5023455254943263234457</t>
+  </si>
+  <si>
+    <t>GR4920910936583000000000</t>
+  </si>
+  <si>
+    <t>ES3720960043032159000000</t>
+  </si>
+  <si>
+    <t>DE5512669681115112121210</t>
+  </si>
+  <si>
+    <t>ES2956187775315550000651</t>
+  </si>
+  <si>
+    <t>ES0425516848021156151054</t>
+  </si>
+  <si>
+    <t>PT5764578946740051516490</t>
+  </si>
+  <si>
+    <t>ES4534698752714600549403</t>
+  </si>
+  <si>
+    <t>ES2766649444162310000255</t>
+  </si>
+  <si>
+    <t>FR5623185484465641685100</t>
+  </si>
+  <si>
+    <t>ES4352198484752100515144</t>
+  </si>
+  <si>
+    <t>CZ9536250012804785523365</t>
+  </si>
+  <si>
+    <t>AT3122515651915640081000</t>
+  </si>
+  <si>
+    <t>DE5021508149175421346497</t>
+  </si>
+  <si>
+    <t>DE6721346154503164978451</t>
+  </si>
+  <si>
+    <t>ES7225187786311225455548</t>
+  </si>
+  <si>
+    <t>ES4723164897642213030615</t>
+  </si>
+  <si>
+    <t>ES2396536214865214585214</t>
+  </si>
+  <si>
+    <t>ES6885461325251978750005</t>
+  </si>
+  <si>
+    <t>FI5024587946032003165464</t>
+  </si>
+  <si>
+    <t>ES5020960043073071400000</t>
+  </si>
+  <si>
+    <t>ES8220960043042158800000</t>
+  </si>
+  <si>
+    <t>ES7521654587985156484454</t>
+  </si>
+  <si>
+    <t>ES3251651681961210656510</t>
+  </si>
+  <si>
+    <t>ES5566552211148855332200</t>
+  </si>
+  <si>
+    <t>GB9720910936583000000000</t>
+  </si>
+  <si>
+    <t>DE9301821135910205540000</t>
+  </si>
+  <si>
+    <t>DE7822631245526916432102</t>
+  </si>
+  <si>
+    <t>ES2120960043043075700000</t>
+  </si>
+  <si>
+    <t>SM7325635478321002541225</t>
+  </si>
+  <si>
+    <t>ES6832154697195423121000</t>
+  </si>
+  <si>
+    <t>GR3836521452736500658485</t>
+  </si>
+  <si>
+    <t>GB5520008521528775113366</t>
+  </si>
+  <si>
+    <t>ES6851651487910005118185</t>
+  </si>
+  <si>
+    <t>ES9001826530120201560000</t>
+  </si>
+  <si>
+    <t>ES9021651651812511133551</t>
+  </si>
+  <si>
+    <t>ES8020960043033000100000</t>
+  </si>
+  <si>
+    <t>GB0836585214290025478551</t>
+  </si>
+  <si>
+    <t>ES9012548523465214585214</t>
+  </si>
+  <si>
+    <t>ES6931624561042546920007</t>
+  </si>
+  <si>
+    <t>ES1436154231712500312566</t>
+  </si>
+  <si>
+    <t>ES8244875664127231645789</t>
+  </si>
+  <si>
+    <t>ES7920960031442124800000</t>
+  </si>
+  <si>
+    <t>ES1633620012937852100256</t>
+  </si>
+  <si>
+    <t>ES1933218885441445121022</t>
+  </si>
+  <si>
+    <t>ES8462581542713690044508</t>
+  </si>
+  <si>
+    <t>ES3925165151118666365100</t>
+  </si>
+  <si>
+    <t>PT3536952365020014425254</t>
+  </si>
+  <si>
+    <t>ES9565168874641561561500</t>
+  </si>
+  <si>
+    <t>ES3220960583831234500000</t>
+  </si>
+  <si>
+    <t>ES7221416325811510005514</t>
+  </si>
+  <si>
+    <t>LU0932628484504115151115</t>
+  </si>
+  <si>
+    <t>20960056133231500000</t>
+  </si>
+  <si>
+    <t>ES2220960056133231500000</t>
+  </si>
+  <si>
+    <t>ES8163516541828944000984</t>
+  </si>
+  <si>
+    <t>23658965274585223202</t>
+  </si>
+  <si>
+    <t>ES6223658965274585223202</t>
+  </si>
+  <si>
+    <t>FI6132658012367712548745</t>
+  </si>
+  <si>
+    <t>ES7223652365142254222000</t>
+  </si>
+  <si>
+    <t>20012541150023365233</t>
+  </si>
+  <si>
+    <t>FR3820012541150023365233</t>
+  </si>
+  <si>
+    <t>ES9232584216971684051000</t>
+  </si>
+  <si>
+    <t>ES6855065688761051056105</t>
+  </si>
+  <si>
+    <t>ES7395485212315484010000</t>
+  </si>
+  <si>
+    <t>LT9321856333126985542360</t>
+  </si>
+  <si>
+    <t>ES5736245978133245679001</t>
+  </si>
+  <si>
+    <t>ES7631245164156597845124</t>
+  </si>
+  <si>
+    <t>SM4423221158252545471411</t>
+  </si>
+  <si>
+    <t>SE6832574512085411002255</t>
+  </si>
+  <si>
+    <t>ES4420960043013468900000</t>
+  </si>
+  <si>
+    <t>ES5631215643855060225021</t>
+  </si>
+  <si>
+    <t>AT3285550564726165145610</t>
+  </si>
+  <si>
+    <t>ES1665165654918886005001</t>
+  </si>
+  <si>
+    <t>ES7426221011628048788896</t>
+  </si>
+  <si>
+    <t>ES9712548521518742146695</t>
+  </si>
+  <si>
     <t>51556584221251000254</t>
   </si>
   <si>
-    <t>20012541150023365233</t>
+    <t>IE6851556584221251000254</t>
+  </si>
+  <si>
+    <t>DK9032541112811220000588</t>
+  </si>
+  <si>
+    <t>62541122421110105611</t>
+  </si>
+  <si>
+    <t>LT9362541122421110105611</t>
+  </si>
+  <si>
+    <t>65645150865168448896</t>
+  </si>
+  <si>
+    <t>AT8365645150865168448896</t>
   </si>
   <si>
     <t>26551681807651415636</t>
   </si>
   <si>
-    <t>23658965274585223202</t>
-  </si>
-  <si>
-    <t>20960056133231500000</t>
-  </si>
-  <si>
-    <t>62541122421110105611</t>
-  </si>
-  <si>
-    <t>65645150865168448896</t>
-  </si>
-  <si>
-    <t>31645124473461205164</t>
-  </si>
-  <si>
-    <t>AT6825030000114574745458</t>
-  </si>
-  <si>
-    <t>DK5800750184310702510000</t>
-  </si>
-  <si>
-    <t>SM7325635478321002541225</t>
-  </si>
-  <si>
-    <t>DE9301821135910205540000</t>
-  </si>
-  <si>
-    <t>ES8462581542713690044508</t>
-  </si>
-  <si>
-    <t>ES9021651651812511133551</t>
-  </si>
-  <si>
-    <t>ES6832154697195423121000</t>
-  </si>
-  <si>
-    <t>ES9001826530120201560000</t>
-  </si>
-  <si>
-    <t>ES6931624561042546920007</t>
-  </si>
-  <si>
-    <t>ES4723164897642213030615</t>
-  </si>
-  <si>
-    <t>ES9232584216971684051000</t>
-  </si>
-  <si>
-    <t>IE6851556584221251000254</t>
-  </si>
-  <si>
-    <t>ES8220960043042158800000</t>
-  </si>
-  <si>
-    <t>ES4534698752714600549403</t>
-  </si>
-  <si>
-    <t>AT3122515651915640081000</t>
-  </si>
-  <si>
-    <t>ES5020960043073071400000</t>
-  </si>
-  <si>
-    <t>ES5023455254943263234457</t>
-  </si>
-  <si>
-    <t>ES9012548523465214585214</t>
-  </si>
-  <si>
-    <t>ES7631245164156597845124</t>
-  </si>
-  <si>
-    <t>DE5512669681115112121210</t>
-  </si>
-  <si>
-    <t>IT8915953684811254695203</t>
-  </si>
-  <si>
-    <t>DE5021508149175421346497</t>
-  </si>
-  <si>
-    <t>ES2766649444162310000255</t>
-  </si>
-  <si>
-    <t>CZ9536250012804785523365</t>
-  </si>
-  <si>
-    <t>ES3925165151118666365100</t>
-  </si>
-  <si>
-    <t>FR3820012541150023365233</t>
-  </si>
-  <si>
-    <t>ES2396536214865214585214</t>
-  </si>
-  <si>
-    <t>ES6885461325251978750005</t>
-  </si>
-  <si>
-    <t>ES7221416325811510005514</t>
-  </si>
-  <si>
-    <t>ES9712548521518742146695</t>
-  </si>
-  <si>
-    <t>ES7521654587985156484454</t>
-  </si>
-  <si>
-    <t>ES7426221011628048788896</t>
-  </si>
-  <si>
-    <t>PT3536952365020014425254</t>
-  </si>
-  <si>
-    <t>ES7223652365142254222000</t>
-  </si>
-  <si>
-    <t>ES1665165654918886005001</t>
-  </si>
-  <si>
-    <t>LU0932628484504115151115</t>
-  </si>
-  <si>
-    <t>GR3836521452736500658485</t>
-  </si>
-  <si>
-    <t>DE7822631245526916432102</t>
-  </si>
-  <si>
-    <t>ES3220960583831234500000</t>
-  </si>
-  <si>
-    <t>AT3285550564726165145610</t>
-  </si>
-  <si>
-    <t>GB9720910936583000000000</t>
-  </si>
-  <si>
-    <t>ES2956187775315550000651</t>
-  </si>
-  <si>
-    <t>ES8020960043033000100000</t>
-  </si>
-  <si>
-    <t>FI6132658012367712548745</t>
-  </si>
-  <si>
-    <t>PT5764578946740051516490</t>
-  </si>
-  <si>
-    <t>ES4352198484752100515144</t>
-  </si>
-  <si>
     <t>IT3526551681807651415636</t>
   </si>
   <si>
-    <t>ES5631215643855060225021</t>
-  </si>
-  <si>
-    <t>ES2120960043043075700000</t>
-  </si>
-  <si>
-    <t>GB5520008521528775113366</t>
-  </si>
-  <si>
-    <t>ES6855065688761051056105</t>
-  </si>
-  <si>
     <t>HU2399558741836555551120</t>
   </si>
   <si>
-    <t>LT9321856333126985542360</t>
-  </si>
-  <si>
-    <t>ES6223658965274585223202</t>
-  </si>
-  <si>
-    <t>ES0425516848021156151054</t>
-  </si>
-  <si>
-    <t>ES5736245978133245679001</t>
-  </si>
-  <si>
-    <t>ES7395485212315484010000</t>
-  </si>
-  <si>
-    <t>ES3720960043032159000000</t>
-  </si>
-  <si>
-    <t>ES1633620012937852100256</t>
-  </si>
-  <si>
-    <t>ES9020960043023096200000</t>
-  </si>
-  <si>
-    <t>GR4920910936583000000000</t>
-  </si>
-  <si>
-    <t>DK9032541112811220000588</t>
-  </si>
-  <si>
-    <t>GB0836585214290025478551</t>
-  </si>
-  <si>
-    <t>ES7920960031442124800000</t>
-  </si>
-  <si>
-    <t>ES1933218885441445121022</t>
-  </si>
-  <si>
-    <t>ES6851651487910005118185</t>
-  </si>
-  <si>
-    <t>ES5566552211148855332200</t>
-  </si>
-  <si>
-    <t>ES1436154231712500312566</t>
-  </si>
-  <si>
-    <t>DE6721346154503164978451</t>
-  </si>
-  <si>
-    <t>ES2220960056133231500000</t>
-  </si>
-  <si>
-    <t>ES8244875664127231645789</t>
-  </si>
-  <si>
-    <t>ES9565168874641561561500</t>
-  </si>
-  <si>
-    <t>SM4423221158252545471411</t>
-  </si>
-  <si>
-    <t>LT9362541122421110105611</t>
-  </si>
-  <si>
-    <t>SE6832574512085411002255</t>
-  </si>
-  <si>
-    <t>ES8163516541828944000984</t>
-  </si>
-  <si>
-    <t>FR5623185484465641685100</t>
-  </si>
-  <si>
-    <t>AT8365645150865168448896</t>
-  </si>
-  <si>
-    <t>ES3251651681961210656510</t>
-  </si>
-  <si>
-    <t>ES4420960043013468900000</t>
-  </si>
-  <si>
-    <t>ES7225187786311225455548</t>
-  </si>
-  <si>
-    <t>FI5024587946032003165464</t>
-  </si>
-  <si>
-    <t>MC6436520125638451012515</t>
-  </si>
-  <si>
-    <t>DK7331645124473461205164</t>
-  </si>
-  <si>
-    <t>SM2125894363475485700145</t>
-  </si>
-  <si>
-    <t>ES9596431245118150005156</t>
-  </si>
-  <si>
-    <t>BE9400750184310702510000</t>
-  </si>
-  <si>
-    <t>ES8265614874165615445616</t>
-  </si>
-  <si>
-    <t>RO8832569523016220165156</t>
-  </si>
-  <si>
-    <t>DE7424561937521546497521</t>
-  </si>
-  <si>
-    <t>GR9420125003305201112544</t>
-  </si>
-  <si>
-    <t>ES2821651484690980008984</t>
-  </si>
-  <si>
-    <t>FI5620960043043554600000</t>
-  </si>
-  <si>
-    <t>LT8032566221522587754554</t>
-  </si>
-  <si>
-    <t>EE2023215465315456411515</t>
-  </si>
-  <si>
-    <t>32145464138452163421</t>
-  </si>
-  <si>
-    <t>X9924125M</t>
-  </si>
-  <si>
     <t>am00@tecnoleonsl.es</t>
   </si>
   <si>
@@ -2069,18 +2096,6 @@
   </si>
   <si>
     <t>sss00@tecnoleonsl.es</t>
-  </si>
-  <si>
-    <t>ES3520960043043554600000</t>
-  </si>
-  <si>
-    <t>ES7832145464138452163421</t>
-  </si>
-  <si>
-    <t>ES7921564975243245467995</t>
-  </si>
-  <si>
-    <t>ES0721584976902154655487</t>
   </si>
 </sst>
 </file>
@@ -2117,7 +2132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2129,9 +2144,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2500,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="D73" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2550,7 +2562,7 @@
         <v>75</v>
       </c>
       <c r="K1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>13</v>
@@ -2561,10 +2573,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -2582,16 +2594,16 @@
         <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>582</v>
+        <v>591</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L2" t="s">
-        <v>680</v>
+        <v>485</v>
       </c>
       <c r="M2" t="s">
         <v>53</v>
@@ -2599,10 +2611,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -2623,16 +2635,16 @@
         <v>70</v>
       </c>
       <c r="I3" t="s">
-        <v>583</v>
+        <v>592</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>580</v>
+        <v>388</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L3" t="s">
-        <v>681</v>
+        <v>486</v>
       </c>
       <c r="M3" t="s">
         <v>53</v>
@@ -2640,10 +2652,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B4" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
@@ -2652,28 +2664,28 @@
         <v>39448</v>
       </c>
       <c r="E4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G4" t="s">
         <v>31</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I4" t="s">
-        <v>584</v>
+        <v>593</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>484</v>
+        <v>389</v>
       </c>
       <c r="K4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L4" t="s">
-        <v>568</v>
+        <v>487</v>
       </c>
       <c r="M4" t="s">
         <v>53</v>
@@ -2681,10 +2693,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B5" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C5" t="s">
         <v>50</v>
@@ -2705,16 +2717,16 @@
         <v>189</v>
       </c>
       <c r="I5" t="s">
-        <v>585</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>382</v>
+        <v>594</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>390</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L5" t="s">
-        <v>572</v>
+        <v>488</v>
       </c>
       <c r="M5" t="s">
         <v>53</v>
@@ -2725,7 +2737,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -2746,16 +2758,16 @@
         <v>238</v>
       </c>
       <c r="I6" t="s">
-        <v>586</v>
+        <v>595</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="K6" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="L6" t="s">
-        <v>573</v>
+        <v>489</v>
       </c>
       <c r="M6" t="s">
         <v>53</v>
@@ -2763,10 +2775,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -2787,16 +2799,16 @@
         <v>355</v>
       </c>
       <c r="I7" t="s">
-        <v>587</v>
+        <v>596</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="K7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L7" t="s">
-        <v>574</v>
+        <v>490</v>
       </c>
       <c r="M7" t="s">
         <v>20</v>
@@ -2807,7 +2819,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -2828,16 +2840,16 @@
         <v>250</v>
       </c>
       <c r="I8" t="s">
-        <v>588</v>
+        <v>597</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="K8" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="L8" t="s">
-        <v>567</v>
+        <v>491</v>
       </c>
       <c r="M8" t="s">
         <v>20</v>
@@ -2849,10 +2861,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B10" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C10" t="s">
         <v>45</v>
@@ -2873,16 +2885,16 @@
         <v>167</v>
       </c>
       <c r="I10" t="s">
-        <v>589</v>
+        <v>598</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="K10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L10" t="s">
-        <v>575</v>
+        <v>492</v>
       </c>
       <c r="M10" t="s">
         <v>53</v>
@@ -2890,10 +2902,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B11" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -2905,7 +2917,7 @@
         <v>278</v>
       </c>
       <c r="F11" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="G11" t="s">
         <v>241</v>
@@ -2914,16 +2926,16 @@
         <v>279</v>
       </c>
       <c r="I11" t="s">
-        <v>590</v>
+        <v>599</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="K11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L11" t="s">
-        <v>576</v>
+        <v>493</v>
       </c>
       <c r="M11" t="s">
         <v>53</v>
@@ -2931,10 +2943,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -2952,19 +2964,19 @@
         <v>58</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="I12" t="s">
-        <v>591</v>
+        <v>600</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L12" t="s">
-        <v>577</v>
+        <v>494</v>
       </c>
       <c r="M12" t="s">
         <v>53</v>
@@ -2972,10 +2984,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -2993,19 +3005,19 @@
         <v>58</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="I13" t="s">
-        <v>592</v>
+        <v>601</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="K13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L13" t="s">
-        <v>682</v>
+        <v>495</v>
       </c>
       <c r="M13" t="s">
         <v>53</v>
@@ -3013,10 +3025,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B14" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C14" t="s">
         <v>49</v>
@@ -3028,7 +3040,7 @@
         <v>284</v>
       </c>
       <c r="F14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G14" t="s">
         <v>285</v>
@@ -3037,16 +3049,16 @@
         <v>286</v>
       </c>
       <c r="I14" t="s">
-        <v>593</v>
+        <v>602</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>390</v>
+        <v>398</v>
       </c>
       <c r="K14" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="L14" t="s">
-        <v>578</v>
+        <v>496</v>
       </c>
       <c r="M14" t="s">
         <v>20</v>
@@ -3054,10 +3066,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B15" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -3072,22 +3084,22 @@
         <v>266</v>
       </c>
       <c r="G15" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>267</v>
       </c>
       <c r="I15" t="s">
-        <v>594</v>
+        <v>603</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
       <c r="K15" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="L15" t="s">
-        <v>579</v>
+        <v>497</v>
       </c>
       <c r="M15" t="s">
         <v>53</v>
@@ -3095,10 +3107,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
@@ -3116,16 +3128,16 @@
         <v>359</v>
       </c>
       <c r="I16" t="s">
-        <v>595</v>
+        <v>604</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="K16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L16" t="s">
-        <v>571</v>
+        <v>498</v>
       </c>
       <c r="M16" t="s">
         <v>20</v>
@@ -3133,10 +3145,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
@@ -3157,16 +3169,16 @@
         <v>359</v>
       </c>
       <c r="I17" t="s">
-        <v>596</v>
+        <v>605</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="K17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L17" t="s">
-        <v>683</v>
+        <v>499</v>
       </c>
       <c r="M17" t="s">
         <v>20</v>
@@ -3174,10 +3186,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B18" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -3192,22 +3204,22 @@
         <v>329</v>
       </c>
       <c r="G18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>330</v>
       </c>
       <c r="I18" t="s">
-        <v>597</v>
+        <v>606</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="K18" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="L18" t="s">
-        <v>569</v>
+        <v>500</v>
       </c>
       <c r="M18" t="s">
         <v>20</v>
@@ -3215,10 +3227,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B19" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C19" t="s">
         <v>47</v>
@@ -3239,16 +3251,16 @@
         <v>317</v>
       </c>
       <c r="I19" t="s">
-        <v>598</v>
+        <v>607</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
       <c r="K19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L19" t="s">
-        <v>570</v>
+        <v>501</v>
       </c>
       <c r="M19" t="s">
         <v>53</v>
@@ -3256,10 +3268,10 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B20" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C20" t="s">
         <v>48</v>
@@ -3280,16 +3292,16 @@
         <v>327</v>
       </c>
       <c r="I20" t="s">
-        <v>599</v>
+        <v>608</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>396</v>
+        <v>404</v>
       </c>
       <c r="K20" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="L20" t="s">
-        <v>485</v>
+        <v>502</v>
       </c>
       <c r="M20" t="s">
         <v>20</v>
@@ -3297,10 +3309,10 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B21" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
@@ -3321,16 +3333,16 @@
         <v>313</v>
       </c>
       <c r="I21" t="s">
-        <v>600</v>
+        <v>609</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="K21" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="L21" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="M21" t="s">
         <v>53</v>
@@ -3338,10 +3350,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -3350,10 +3362,10 @@
         <v>40909</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G22" t="s">
         <v>33</v>
@@ -3362,16 +3374,16 @@
         <v>43</v>
       </c>
       <c r="I22" t="s">
-        <v>601</v>
+        <v>610</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
       <c r="K22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L22" t="s">
-        <v>544</v>
+        <v>504</v>
       </c>
       <c r="M22" t="s">
         <v>53</v>
@@ -3379,10 +3391,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B23" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -3391,25 +3403,25 @@
         <v>41913</v>
       </c>
       <c r="E23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F23" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="I23" t="s">
-        <v>602</v>
+        <v>611</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="K23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L23" t="s">
-        <v>486</v>
+        <v>505</v>
       </c>
       <c r="M23" t="s">
         <v>20</v>
@@ -3420,7 +3432,7 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -3438,19 +3450,19 @@
         <v>61</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="I24" t="s">
-        <v>603</v>
+        <v>612</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
       <c r="K24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L24" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="M24" t="s">
         <v>20</v>
@@ -3458,10 +3470,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
@@ -3479,16 +3491,16 @@
         <v>64</v>
       </c>
       <c r="I25" t="s">
-        <v>604</v>
+        <v>613</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L25" t="s">
-        <v>545</v>
+        <v>507</v>
       </c>
       <c r="M25" t="s">
         <v>20</v>
@@ -3499,7 +3511,7 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
@@ -3517,19 +3529,19 @@
         <v>33</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
       <c r="I26" t="s">
-        <v>605</v>
+        <v>614</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
       <c r="K26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L26" t="s">
-        <v>542</v>
+        <v>508</v>
       </c>
       <c r="M26" t="s">
         <v>53</v>
@@ -3537,10 +3549,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B27" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C27" t="s">
         <v>48</v>
@@ -3555,22 +3567,22 @@
         <v>41</v>
       </c>
       <c r="G27" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>198</v>
       </c>
       <c r="I27" t="s">
-        <v>606</v>
+        <v>615</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>403</v>
+        <v>411</v>
       </c>
       <c r="K27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L27" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="M27" t="s">
         <v>53</v>
@@ -3582,10 +3594,10 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -3606,16 +3618,16 @@
         <v>300</v>
       </c>
       <c r="I29" t="s">
-        <v>607</v>
+        <v>616</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>404</v>
+        <v>412</v>
       </c>
       <c r="K29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L29" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="M29" t="s">
         <v>53</v>
@@ -3623,10 +3635,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B30" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
@@ -3647,16 +3659,16 @@
         <v>185</v>
       </c>
       <c r="I30" t="s">
-        <v>608</v>
+        <v>617</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>405</v>
+        <v>413</v>
       </c>
       <c r="K30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L30" t="s">
-        <v>539</v>
+        <v>511</v>
       </c>
       <c r="M30" t="s">
         <v>20</v>
@@ -3664,10 +3676,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B31" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
@@ -3688,16 +3700,16 @@
         <v>321</v>
       </c>
       <c r="I31" t="s">
-        <v>609</v>
+        <v>618</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="K31" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="L31" t="s">
-        <v>529</v>
+        <v>512</v>
       </c>
       <c r="M31" t="s">
         <v>53</v>
@@ -3705,10 +3717,10 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -3729,16 +3741,16 @@
         <v>325</v>
       </c>
       <c r="I32" t="s">
-        <v>610</v>
+        <v>619</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>407</v>
+        <v>415</v>
       </c>
       <c r="K32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L32" t="s">
-        <v>498</v>
+        <v>513</v>
       </c>
       <c r="M32" t="s">
         <v>20</v>
@@ -3746,10 +3758,10 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B33" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
@@ -3770,16 +3782,16 @@
         <v>334</v>
       </c>
       <c r="I33" t="s">
-        <v>611</v>
+        <v>620</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>408</v>
+        <v>416</v>
       </c>
       <c r="K33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L33" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="M33" t="s">
         <v>20</v>
@@ -3790,7 +3802,7 @@
         <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C34" t="s">
         <v>48</v>
@@ -3811,16 +3823,16 @@
         <v>270</v>
       </c>
       <c r="I34" t="s">
-        <v>612</v>
+        <v>621</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="K34" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="L34" t="s">
-        <v>561</v>
+        <v>515</v>
       </c>
       <c r="M34" t="s">
         <v>20</v>
@@ -3831,7 +3843,7 @@
         <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
         <v>50</v>
@@ -3852,16 +3864,16 @@
         <v>217</v>
       </c>
       <c r="I35" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="K35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L35" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="M35" t="s">
         <v>53</v>
@@ -3869,10 +3881,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B36" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
@@ -3893,16 +3905,16 @@
         <v>235</v>
       </c>
       <c r="I36" t="s">
-        <v>614</v>
+        <v>623</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="K36" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="L36" t="s">
-        <v>508</v>
+        <v>517</v>
       </c>
       <c r="M36" t="s">
         <v>53</v>
@@ -3910,10 +3922,10 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B37" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
@@ -3934,16 +3946,16 @@
         <v>210</v>
       </c>
       <c r="I37" t="s">
-        <v>615</v>
+        <v>624</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>412</v>
+        <v>420</v>
       </c>
       <c r="K37" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="L37" t="s">
-        <v>499</v>
+        <v>518</v>
       </c>
       <c r="M37" t="s">
         <v>53</v>
@@ -3951,10 +3963,10 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B38" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C38" t="s">
         <v>49</v>
@@ -3969,22 +3981,22 @@
         <v>39</v>
       </c>
       <c r="G38" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>350</v>
       </c>
       <c r="I38" t="s">
-        <v>616</v>
+        <v>625</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>413</v>
+        <v>421</v>
       </c>
       <c r="K38" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L38" t="s">
-        <v>506</v>
+        <v>519</v>
       </c>
       <c r="M38" t="s">
         <v>53</v>
@@ -3995,7 +4007,7 @@
         <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
         <v>45</v>
@@ -4013,19 +4025,19 @@
         <v>353</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="I39" t="s">
-        <v>617</v>
+        <v>626</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>415</v>
+        <v>423</v>
       </c>
       <c r="K39" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L39" t="s">
-        <v>553</v>
+        <v>520</v>
       </c>
       <c r="M39" t="s">
         <v>20</v>
@@ -4033,10 +4045,10 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B40" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C40" t="s">
         <v>71</v>
@@ -4057,16 +4069,16 @@
         <v>337</v>
       </c>
       <c r="I40" t="s">
-        <v>618</v>
+        <v>627</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="K40" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L40" t="s">
-        <v>565</v>
+        <v>521</v>
       </c>
       <c r="M40" t="s">
         <v>53</v>
@@ -4074,10 +4086,10 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
@@ -4098,16 +4110,16 @@
         <v>341</v>
       </c>
       <c r="I41" t="s">
-        <v>619</v>
+        <v>628</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="K41" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L41" t="s">
-        <v>494</v>
+        <v>522</v>
       </c>
       <c r="M41" t="s">
         <v>53</v>
@@ -4115,10 +4127,10 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
@@ -4127,28 +4139,28 @@
         <v>37865</v>
       </c>
       <c r="E42" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F42" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G42" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I42" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="K42" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L42" t="s">
-        <v>511</v>
+        <v>523</v>
       </c>
       <c r="M42" t="s">
         <v>53</v>
@@ -4156,10 +4168,10 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B43" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
@@ -4180,16 +4192,16 @@
         <v>344</v>
       </c>
       <c r="I43" t="s">
-        <v>621</v>
+        <v>630</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="K43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L43" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="M43" t="s">
         <v>53</v>
@@ -4197,10 +4209,10 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C44" t="s">
         <v>48</v>
@@ -4221,16 +4233,16 @@
         <v>348</v>
       </c>
       <c r="I44" t="s">
-        <v>622</v>
+        <v>631</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="K44" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L44" t="s">
-        <v>566</v>
+        <v>525</v>
       </c>
       <c r="M44" t="s">
         <v>53</v>
@@ -4238,10 +4250,10 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C45" t="s">
         <v>51</v>
@@ -4259,19 +4271,19 @@
         <v>39</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="I45" t="s">
-        <v>622</v>
+        <v>631</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="K45" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L45" t="s">
-        <v>500</v>
+        <v>526</v>
       </c>
       <c r="M45" t="s">
         <v>53</v>
@@ -4279,10 +4291,10 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C46" t="s">
         <v>46</v>
@@ -4303,16 +4315,16 @@
         <v>42</v>
       </c>
       <c r="I46" t="s">
-        <v>623</v>
+        <v>632</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>423</v>
+        <v>431</v>
       </c>
       <c r="K46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L46" t="s">
-        <v>497</v>
+        <v>527</v>
       </c>
       <c r="M46" t="s">
         <v>53</v>
@@ -4320,10 +4332,10 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B47" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
@@ -4344,16 +4356,16 @@
         <v>181</v>
       </c>
       <c r="I47" t="s">
-        <v>624</v>
+        <v>633</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>424</v>
+        <v>432</v>
       </c>
       <c r="K47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L47" t="s">
-        <v>515</v>
+        <v>528</v>
       </c>
       <c r="M47" t="s">
         <v>53</v>
@@ -4361,10 +4373,10 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B48" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
@@ -4373,28 +4385,28 @@
         <v>39692</v>
       </c>
       <c r="E48" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G48" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I48" t="s">
-        <v>625</v>
+        <v>634</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="K48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L48" t="s">
-        <v>563</v>
+        <v>529</v>
       </c>
       <c r="M48" t="s">
         <v>53</v>
@@ -4405,7 +4417,7 @@
         <v>19</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C49" t="s">
         <v>51</v>
@@ -4426,16 +4438,16 @@
         <v>246</v>
       </c>
       <c r="I49" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="K49" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L49" t="s">
-        <v>551</v>
+        <v>530</v>
       </c>
       <c r="M49" t="s">
         <v>20</v>
@@ -4443,10 +4455,10 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C50" t="s">
         <v>10</v>
@@ -4461,19 +4473,19 @@
         <v>66</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="I50" t="s">
-        <v>627</v>
+        <v>636</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L50" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="M50" t="s">
         <v>20</v>
@@ -4481,10 +4493,10 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B51" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C51" t="s">
         <v>46</v>
@@ -4499,19 +4511,19 @@
         <v>68</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="I51" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="K51" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L51" t="s">
-        <v>488</v>
+        <v>532</v>
       </c>
       <c r="M51" t="s">
         <v>20</v>
@@ -4519,10 +4531,10 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
         <v>45</v>
@@ -4531,28 +4543,28 @@
         <v>42887</v>
       </c>
       <c r="E52" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F52" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G52" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I52" t="s">
-        <v>629</v>
+        <v>638</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="K52" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L52" t="s">
-        <v>522</v>
+        <v>533</v>
       </c>
       <c r="M52" t="s">
         <v>53</v>
@@ -4560,10 +4572,10 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B53" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
         <v>10</v>
@@ -4581,19 +4593,19 @@
         <v>22</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="I53" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="K53" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L53" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="M53" t="s">
         <v>20</v>
@@ -4604,7 +4616,7 @@
         <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C54" t="s">
         <v>10</v>
@@ -4625,16 +4637,16 @@
         <v>248</v>
       </c>
       <c r="I54" t="s">
-        <v>631</v>
+        <v>640</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="K54" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="L54" t="s">
-        <v>487</v>
+        <v>535</v>
       </c>
       <c r="M54" t="s">
         <v>20</v>
@@ -4642,10 +4654,10 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B55" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C55" t="s">
         <v>11</v>
@@ -4666,16 +4678,16 @@
         <v>192</v>
       </c>
       <c r="I55" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="K55" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L55" t="s">
-        <v>491</v>
+        <v>536</v>
       </c>
       <c r="M55" t="s">
         <v>20</v>
@@ -4683,10 +4695,10 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B56" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C56" t="s">
         <v>51</v>
@@ -4707,16 +4719,16 @@
         <v>207</v>
       </c>
       <c r="I56" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="K56" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L56" t="s">
-        <v>521</v>
+        <v>537</v>
       </c>
       <c r="M56" t="s">
         <v>20</v>
@@ -4724,10 +4736,10 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B57" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C57" t="s">
         <v>51</v>
@@ -4742,22 +4754,22 @@
         <v>27</v>
       </c>
       <c r="G57" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>169</v>
       </c>
       <c r="I57" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="K57" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L57" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="M57" t="s">
         <v>53</v>
@@ -4768,7 +4780,7 @@
         <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C58" t="s">
         <v>51</v>
@@ -4789,16 +4801,16 @@
         <v>277</v>
       </c>
       <c r="I58" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="K58" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L58" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="M58" t="s">
         <v>20</v>
@@ -4810,10 +4822,10 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C60" t="s">
         <v>48</v>
@@ -4831,19 +4843,19 @@
         <v>32</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="I60" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K60" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L60" t="s">
-        <v>492</v>
+        <v>540</v>
       </c>
       <c r="M60" t="s">
         <v>20</v>
@@ -4851,10 +4863,10 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B61" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C61" t="s">
         <v>46</v>
@@ -4875,16 +4887,16 @@
         <v>194</v>
       </c>
       <c r="I61" t="s">
-        <v>637</v>
+        <v>646</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="K61" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L61" t="s">
-        <v>490</v>
+        <v>541</v>
       </c>
       <c r="M61" t="s">
         <v>53</v>
@@ -4892,10 +4904,10 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C62" t="s">
         <v>8</v>
@@ -4904,28 +4916,28 @@
         <v>42309</v>
       </c>
       <c r="E62" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F62" t="s">
         <v>33</v>
       </c>
       <c r="G62" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>69</v>
       </c>
       <c r="I62" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="K62" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L62" t="s">
-        <v>527</v>
+        <v>542</v>
       </c>
       <c r="M62" t="s">
         <v>20</v>
@@ -4933,10 +4945,10 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B63" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C63" t="s">
         <v>8</v>
@@ -4957,16 +4969,16 @@
         <v>204</v>
       </c>
       <c r="I63" t="s">
-        <v>639</v>
+        <v>648</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="K63" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L63" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="M63" t="s">
         <v>53</v>
@@ -4974,10 +4986,10 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B64" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C64" t="s">
         <v>48</v>
@@ -4986,28 +4998,28 @@
         <v>40544</v>
       </c>
       <c r="E64" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F64" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G64" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I64" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="K64" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L64" t="s">
-        <v>502</v>
+        <v>544</v>
       </c>
       <c r="M64" t="s">
         <v>20</v>
@@ -5018,7 +5030,7 @@
         <v>19</v>
       </c>
       <c r="B65" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
@@ -5039,16 +5051,16 @@
         <v>221</v>
       </c>
       <c r="I65" t="s">
-        <v>641</v>
+        <v>650</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="K65" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L65" t="s">
-        <v>493</v>
+        <v>545</v>
       </c>
       <c r="M65" t="s">
         <v>53</v>
@@ -5056,10 +5068,10 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B66" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C66" t="s">
         <v>46</v>
@@ -5068,28 +5080,28 @@
         <v>43282</v>
       </c>
       <c r="E66" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F66" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G66" t="s">
         <v>31</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I66" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="K66" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L66" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="M66" t="s">
         <v>20</v>
@@ -5097,10 +5109,10 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B67" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C67" t="s">
         <v>11</v>
@@ -5112,7 +5124,7 @@
         <v>356</v>
       </c>
       <c r="F67" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G67" t="s">
         <v>357</v>
@@ -5121,16 +5133,16 @@
         <v>358</v>
       </c>
       <c r="I67" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="K67" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L67" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="M67" t="s">
         <v>20</v>
@@ -5138,10 +5150,10 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B68" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C68" t="s">
         <v>45</v>
@@ -5150,25 +5162,25 @@
         <v>40057</v>
       </c>
       <c r="E68" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F68" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G68" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="I68" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="J68" s="5" t="s">
         <v>77</v>
       </c>
       <c r="K68" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L68" t="s">
         <v>548</v>
@@ -5179,10 +5191,10 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B69" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
@@ -5200,19 +5212,19 @@
         <v>306</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="I69" t="s">
-        <v>644</v>
+        <v>653</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="K69" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L69" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="M69" t="s">
         <v>53</v>
@@ -5220,10 +5232,10 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B70" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C70" t="s">
         <v>48</v>
@@ -5235,25 +5247,25 @@
         <v>251</v>
       </c>
       <c r="F70" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G70" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>252</v>
       </c>
       <c r="I70" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="K70" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L70" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="M70" t="s">
         <v>20</v>
@@ -5261,10 +5273,10 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B71" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C71" t="s">
         <v>9</v>
@@ -5285,16 +5297,16 @@
         <v>163</v>
       </c>
       <c r="I71" t="s">
-        <v>646</v>
+        <v>655</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="K71" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L71" t="s">
-        <v>489</v>
+        <v>551</v>
       </c>
       <c r="M71" t="s">
         <v>20</v>
@@ -5302,10 +5314,10 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B72" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C72" t="s">
         <v>10</v>
@@ -5326,16 +5338,16 @@
         <v>283</v>
       </c>
       <c r="I72" t="s">
-        <v>647</v>
+        <v>656</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="K72" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L72" t="s">
-        <v>509</v>
+        <v>552</v>
       </c>
       <c r="M72" t="s">
         <v>20</v>
@@ -5343,10 +5355,10 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B73" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C73" t="s">
         <v>52</v>
@@ -5364,19 +5376,19 @@
         <v>35</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="I73" t="s">
-        <v>648</v>
+        <v>657</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="K73" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L73" t="s">
-        <v>527</v>
+        <v>542</v>
       </c>
       <c r="M73" t="s">
         <v>20</v>
@@ -5384,10 +5396,10 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C74" t="s">
         <v>10</v>
@@ -5408,16 +5420,16 @@
         <v>304</v>
       </c>
       <c r="I74" t="s">
-        <v>649</v>
+        <v>658</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="K74" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="L74" t="s">
-        <v>517</v>
+        <v>553</v>
       </c>
       <c r="M74" t="s">
         <v>53</v>
@@ -5425,10 +5437,10 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B75" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C75" t="s">
         <v>11</v>
@@ -5443,22 +5455,22 @@
         <v>296</v>
       </c>
       <c r="G75" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>297</v>
       </c>
       <c r="I75" t="s">
-        <v>650</v>
+        <v>659</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="K75" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L75" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="M75" t="s">
         <v>53</v>
@@ -5466,10 +5478,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B76" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C76" t="s">
         <v>8</v>
@@ -5490,16 +5502,16 @@
         <v>69</v>
       </c>
       <c r="I76" t="s">
-        <v>651</v>
+        <v>660</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
       <c r="K76" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L76" t="s">
-        <v>523</v>
+        <v>555</v>
       </c>
       <c r="M76" t="s">
         <v>20</v>
@@ -5507,10 +5519,10 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B77" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
@@ -5531,16 +5543,16 @@
         <v>254</v>
       </c>
       <c r="I77" t="s">
-        <v>652</v>
+        <v>661</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="K77" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L77" t="s">
-        <v>513</v>
+        <v>556</v>
       </c>
       <c r="M77" t="s">
         <v>20</v>
@@ -5551,7 +5563,7 @@
         <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C78" t="s">
         <v>45</v>
@@ -5572,16 +5584,16 @@
         <v>232</v>
       </c>
       <c r="I78" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="K78" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="L78" t="s">
-        <v>520</v>
+        <v>557</v>
       </c>
       <c r="M78" t="s">
         <v>53</v>
@@ -5593,10 +5605,10 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B80" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C80" t="s">
         <v>12</v>
@@ -5605,7 +5617,7 @@
         <v>42705</v>
       </c>
       <c r="E80" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F80" t="s">
         <v>36</v>
@@ -5615,16 +5627,16 @@
       </c>
       <c r="H80" s="3"/>
       <c r="I80" t="s">
-        <v>654</v>
+        <v>663</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>481</v>
+        <v>558</v>
       </c>
       <c r="K80" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L80" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="M80" t="s">
         <v>20</v>
@@ -5632,10 +5644,10 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B81" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C81" t="s">
         <v>52</v>
@@ -5656,13 +5668,13 @@
         <v>173</v>
       </c>
       <c r="I81" t="s">
-        <v>655</v>
+        <v>664</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="K81" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L81" t="s">
         <v>560</v>
@@ -5673,10 +5685,10 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C82" t="s">
         <v>46</v>
@@ -5697,16 +5709,16 @@
         <v>310</v>
       </c>
       <c r="I82" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>480</v>
+        <v>561</v>
       </c>
       <c r="K82" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L82" t="s">
-        <v>538</v>
+        <v>562</v>
       </c>
       <c r="M82" t="s">
         <v>53</v>
@@ -5714,10 +5726,10 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B83" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C83" t="s">
         <v>50</v>
@@ -5726,28 +5738,28 @@
         <v>38139</v>
       </c>
       <c r="E83" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F83" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G83" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I83" t="s">
-        <v>657</v>
+        <v>666</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="K83" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L83" t="s">
-        <v>528</v>
+        <v>563</v>
       </c>
       <c r="M83" t="s">
         <v>20</v>
@@ -5755,10 +5767,10 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B84" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C84" t="s">
         <v>48</v>
@@ -5779,16 +5791,16 @@
         <v>294</v>
       </c>
       <c r="I84" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="K84" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L84" t="s">
-        <v>518</v>
+        <v>564</v>
       </c>
       <c r="M84" t="s">
         <v>53</v>
@@ -5796,10 +5808,10 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B85" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C85" t="s">
         <v>9</v>
@@ -5817,16 +5829,16 @@
         <v>291</v>
       </c>
       <c r="I85" t="s">
-        <v>659</v>
+        <v>668</v>
       </c>
       <c r="J85" s="5" t="s">
-        <v>478</v>
+        <v>565</v>
       </c>
       <c r="K85" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="L85" t="s">
-        <v>510</v>
+        <v>566</v>
       </c>
       <c r="M85" t="s">
         <v>20</v>
@@ -5834,10 +5846,10 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B86" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C86" t="s">
         <v>8</v>
@@ -5858,16 +5870,16 @@
         <v>256</v>
       </c>
       <c r="I86" t="s">
-        <v>660</v>
+        <v>669</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="K86" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L86" t="s">
-        <v>495</v>
+        <v>567</v>
       </c>
       <c r="M86" t="s">
         <v>20</v>
@@ -5875,10 +5887,10 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B87" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C87" t="s">
         <v>9</v>
@@ -5887,28 +5899,28 @@
         <v>38687</v>
       </c>
       <c r="E87" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F87" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G87" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I87" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="K87" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L87" t="s">
-        <v>535</v>
+        <v>568</v>
       </c>
       <c r="M87" t="s">
         <v>53</v>
@@ -5916,10 +5928,10 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B88" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C88" t="s">
         <v>8</v>
@@ -5928,28 +5940,28 @@
         <v>43282</v>
       </c>
       <c r="E88" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F88" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G88" t="s">
         <v>33</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I88" t="s">
-        <v>662</v>
+        <v>671</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="K88" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L88" t="s">
-        <v>541</v>
+        <v>569</v>
       </c>
       <c r="M88" t="s">
         <v>53</v>
@@ -5960,7 +5972,7 @@
         <v>19</v>
       </c>
       <c r="B89" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C89" t="s">
         <v>10</v>
@@ -5981,16 +5993,16 @@
         <v>259</v>
       </c>
       <c r="I89" t="s">
-        <v>663</v>
+        <v>672</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="K89" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="L89" t="s">
-        <v>537</v>
+        <v>570</v>
       </c>
       <c r="M89" t="s">
         <v>20</v>
@@ -5998,10 +6010,10 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B90" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C90" t="s">
         <v>48</v>
@@ -6010,28 +6022,28 @@
         <v>41426</v>
       </c>
       <c r="E90" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F90" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G90" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>155</v>
       </c>
       <c r="I90" t="s">
-        <v>664</v>
+        <v>673</v>
       </c>
       <c r="J90" s="5" t="s">
-        <v>463</v>
+        <v>471</v>
       </c>
       <c r="K90" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L90" t="s">
-        <v>540</v>
+        <v>571</v>
       </c>
       <c r="M90" t="s">
         <v>20</v>
@@ -6039,10 +6051,10 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B91" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C91" t="s">
         <v>8</v>
@@ -6051,28 +6063,28 @@
         <v>38838</v>
       </c>
       <c r="E91" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F91" t="s">
         <v>32</v>
       </c>
       <c r="G91" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I91" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K91" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L91" t="s">
-        <v>503</v>
+        <v>572</v>
       </c>
       <c r="M91" t="s">
         <v>20</v>
@@ -6080,10 +6092,10 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B92" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C92" t="s">
         <v>8</v>
@@ -6104,16 +6116,16 @@
         <v>288</v>
       </c>
       <c r="I92" t="s">
-        <v>666</v>
+        <v>675</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="K92" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="L92" t="s">
-        <v>557</v>
+        <v>573</v>
       </c>
       <c r="M92" t="s">
         <v>20</v>
@@ -6124,7 +6136,7 @@
         <v>19</v>
       </c>
       <c r="B93" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C93" t="s">
         <v>71</v>
@@ -6145,16 +6157,16 @@
         <v>242</v>
       </c>
       <c r="I93" t="s">
-        <v>667</v>
+        <v>676</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="K93" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="L93" t="s">
-        <v>559</v>
+        <v>574</v>
       </c>
       <c r="M93" t="s">
         <v>53</v>
@@ -6162,10 +6174,10 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B94" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C94" t="s">
         <v>8</v>
@@ -6186,16 +6198,16 @@
         <v>44</v>
       </c>
       <c r="I94" t="s">
-        <v>668</v>
+        <v>677</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="K94" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L94" t="s">
-        <v>564</v>
+        <v>575</v>
       </c>
       <c r="M94" t="s">
         <v>20</v>
@@ -6206,7 +6218,7 @@
         <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C95" t="s">
         <v>9</v>
@@ -6224,19 +6236,19 @@
         <v>222</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="I95" t="s">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="J95" s="5" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="K95" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L95" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="M95" t="s">
         <v>20</v>
@@ -6247,7 +6259,7 @@
         <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C96" t="s">
         <v>11</v>
@@ -6265,19 +6277,19 @@
         <v>33</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="I96" t="s">
-        <v>670</v>
+        <v>679</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="K96" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="L96" t="s">
-        <v>524</v>
+        <v>577</v>
       </c>
       <c r="M96" t="s">
         <v>20</v>
@@ -6285,10 +6297,10 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B97" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C97" t="s">
         <v>12</v>
@@ -6309,16 +6321,16 @@
         <v>177</v>
       </c>
       <c r="I97" t="s">
-        <v>671</v>
+        <v>680</v>
       </c>
       <c r="J97" s="5" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="K97" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L97" t="s">
-        <v>519</v>
+        <v>578</v>
       </c>
       <c r="M97" t="s">
         <v>20</v>
@@ -6326,10 +6338,10 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B98" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C98" t="s">
         <v>11</v>
@@ -6350,16 +6362,16 @@
         <v>159</v>
       </c>
       <c r="I98" t="s">
-        <v>672</v>
+        <v>681</v>
       </c>
       <c r="J98" s="5" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="K98" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L98" t="s">
-        <v>516</v>
+        <v>579</v>
       </c>
       <c r="M98" t="s">
         <v>20</v>
@@ -6367,10 +6379,10 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B99" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C99" t="s">
         <v>52</v>
@@ -6379,28 +6391,28 @@
         <v>39203</v>
       </c>
       <c r="E99" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F99" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G99" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I99" t="s">
-        <v>673</v>
+        <v>682</v>
       </c>
       <c r="J99" s="5" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="K99" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L99" t="s">
-        <v>514</v>
+        <v>580</v>
       </c>
       <c r="M99" t="s">
         <v>20</v>
@@ -6412,10 +6424,10 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B101" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C101" t="s">
         <v>10</v>
@@ -6427,7 +6439,7 @@
         <v>211</v>
       </c>
       <c r="F101" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G101" t="s">
         <v>212</v>
@@ -6436,16 +6448,16 @@
         <v>213</v>
       </c>
       <c r="I101" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="J101" s="5" t="s">
-        <v>477</v>
+        <v>581</v>
       </c>
       <c r="K101" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="L101" t="s">
-        <v>496</v>
+        <v>582</v>
       </c>
       <c r="M101" t="s">
         <v>20</v>
@@ -6453,10 +6465,10 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B102" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C102" t="s">
         <v>45</v>
@@ -6471,22 +6483,22 @@
         <v>200</v>
       </c>
       <c r="G102" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H102" s="2" t="s">
         <v>201</v>
       </c>
       <c r="I102" t="s">
-        <v>675</v>
+        <v>684</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="K102" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L102" t="s">
-        <v>546</v>
+        <v>583</v>
       </c>
       <c r="M102" t="s">
         <v>20</v>
@@ -6497,7 +6509,7 @@
         <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C103" t="s">
         <v>48</v>
@@ -6518,16 +6530,16 @@
         <v>228</v>
       </c>
       <c r="I103" t="s">
-        <v>676</v>
+        <v>685</v>
       </c>
       <c r="J103" s="5" t="s">
-        <v>482</v>
+        <v>584</v>
       </c>
       <c r="K103" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="L103" t="s">
-        <v>558</v>
+        <v>585</v>
       </c>
       <c r="M103" t="s">
         <v>20</v>
@@ -6535,10 +6547,10 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B104" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C104" t="s">
         <v>50</v>
@@ -6559,16 +6571,16 @@
         <v>264</v>
       </c>
       <c r="I104" t="s">
-        <v>677</v>
+        <v>686</v>
       </c>
       <c r="J104" s="5" t="s">
-        <v>483</v>
+        <v>586</v>
       </c>
       <c r="K104" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="L104" t="s">
-        <v>562</v>
+        <v>587</v>
       </c>
       <c r="M104" t="s">
         <v>20</v>
@@ -6579,7 +6591,7 @@
         <v>19</v>
       </c>
       <c r="B105" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C105" t="s">
         <v>52</v>
@@ -6594,22 +6606,22 @@
         <v>224</v>
       </c>
       <c r="G105" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H105" s="2" t="s">
         <v>225</v>
       </c>
       <c r="I105" t="s">
-        <v>678</v>
+        <v>687</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>479</v>
+        <v>588</v>
       </c>
       <c r="K105" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="L105" t="s">
-        <v>531</v>
+        <v>589</v>
       </c>
       <c r="M105" t="s">
         <v>20</v>
@@ -6620,7 +6632,7 @@
         <v>19</v>
       </c>
       <c r="B106" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C106" t="s">
         <v>45</v>
@@ -6635,33 +6647,33 @@
         <v>272</v>
       </c>
       <c r="G106" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H106" s="2" t="s">
         <v>273</v>
       </c>
       <c r="I106" t="s">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="J106" s="5" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="K106" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="L106" t="s">
-        <v>536</v>
+        <v>590</v>
       </c>
       <c r="M106" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:L106">
+  <sortState ref="F2:L106">
     <sortCondition ref="F1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7291,7 +7303,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1">
         <v>4.7</v>
@@ -7299,7 +7311,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B2">
         <v>1.6</v>
@@ -7307,7 +7319,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B3">
         <v>0.1</v>
@@ -7315,7 +7327,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B4">
         <v>23.6</v>
@@ -7323,7 +7335,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B5">
         <v>0.2</v>
@@ -7331,7 +7343,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B6">
         <v>6.7</v>
@@ -7339,7 +7351,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B7">
         <v>0.6</v>
@@ -7347,7 +7359,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -7374,10 +7386,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>